<commit_message>
v0.0.2 enabled api excel file download, song position rearranged 2022/11/20 semi-confirmed
</commit_message>
<xml_diff>
--- a/歌单.xlsx
+++ b/歌单.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$D$127</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$D$128</definedName>
   </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
@@ -685,6 +685,12 @@
     <t>心理测量者 ED</t>
   </si>
   <si>
+    <t>Departures~あなたにおくるアイの歌~</t>
+  </si>
+  <si>
+    <t>罪恶王冠 ED1</t>
+  </si>
+  <si>
     <t>星の在り処</t>
   </si>
   <si>
@@ -697,7 +703,7 @@
     <t>KING</t>
   </si>
   <si>
-    <t>Kanaria</t>
+    <t>Kanaria&amp;VOCALOID</t>
   </si>
   <si>
     <t>朧月</t>
@@ -1184,12 +1190,6 @@
   </si>
   <si>
     <t>月光的指引/黑之契约者第二季 OP</t>
-  </si>
-  <si>
-    <t>Departures~あなたにおくるアイの歌~</t>
-  </si>
-  <si>
-    <t>罪恶王冠 ED1</t>
   </si>
   <si>
     <t>同担☆拒否</t>
@@ -5869,12 +5869,12 @@
   <sheetPr/>
   <dimension ref="A1:D945"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="F112" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="30" zoomScaleNormal="30" workbookViewId="0">
+      <pane xSplit="4" ySplit="3" topLeftCell="E93" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B112" sqref="$A1:$XFD1048576"/>
+      <selection pane="bottomRight" activeCell="E93" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.625" defaultRowHeight="23.5" customHeight="1" outlineLevelCol="3"/>
@@ -7239,73 +7239,75 @@
         <v>221</v>
       </c>
     </row>
-    <row r="102" s="2" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A102" s="15" t="s">
+    <row r="102" customHeight="1" spans="1:4">
+      <c r="A102" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="B102" s="15" t="s">
+      <c r="B102" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D102" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="C102" s="2" t="s">
+    </row>
+    <row r="103" s="2" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A103" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="B103" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="C103" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D102" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="103" s="2" customFormat="1" customHeight="1" spans="1:3">
-      <c r="A103" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="B103" s="15" t="s">
+      <c r="D103" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="C103" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="104" customHeight="1" spans="1:4">
-      <c r="A104" s="2" t="s">
+    </row>
+    <row r="104" s="2" customFormat="1" customHeight="1" spans="1:3">
+      <c r="A104" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="B104" s="15" t="s">
         <v>228</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D104" s="8"/>
     </row>
     <row r="105" customHeight="1" spans="1:4">
-      <c r="A105" s="3" t="s">
+      <c r="A105" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B105" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="C105" s="3" t="s">
+      <c r="B105" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D105" s="8"/>
+    </row>
+    <row r="106" customHeight="1" spans="1:4">
+      <c r="A106" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C106" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D105" s="3"/>
-    </row>
-    <row r="106" customHeight="1" spans="1:4">
-      <c r="A106" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D106" s="8"/>
+      <c r="D106" s="3"/>
     </row>
     <row r="107" customHeight="1" spans="1:4">
       <c r="A107" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>7</v>
@@ -7314,10 +7316,10 @@
     </row>
     <row r="108" customHeight="1" spans="1:4">
       <c r="A108" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>7</v>
@@ -7326,153 +7328,151 @@
     </row>
     <row r="109" customHeight="1" spans="1:4">
       <c r="A109" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C109" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D109" s="8"/>
     </row>
-    <row r="110" customHeight="1" spans="1:3">
+    <row r="110" customHeight="1" spans="1:4">
       <c r="A110" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="D110" s="8"/>
     </row>
     <row r="111" customHeight="1" spans="1:3">
       <c r="A111" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="112" customHeight="1" spans="1:4">
-      <c r="A112" s="8" t="s">
-        <v>236</v>
+    <row r="112" customHeight="1" spans="1:3">
+      <c r="A112" s="2" t="s">
+        <v>237</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D112" s="2" t="s">
-        <v>237</v>
-      </c>
     </row>
     <row r="113" customHeight="1" spans="1:4">
-      <c r="A113" s="14" t="s">
+      <c r="A113" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="B113" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="C113" s="3" t="s">
+      <c r="B113" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="114" customHeight="1" spans="1:4">
+      <c r="A114" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C114" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D113" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="114" customHeight="1" spans="1:4">
-      <c r="A114" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="C114" s="1" t="s">
+      <c r="D114" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="115" customHeight="1" spans="1:4">
+      <c r="A115" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C115" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D114" s="2" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="115" customHeight="1" spans="1:4">
-      <c r="A115" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="B115" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="C115" s="3" t="s">
+      <c r="D115" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="116" customHeight="1" spans="1:4">
+      <c r="A116" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C116" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D115" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="116" customHeight="1" spans="1:3">
-      <c r="A116" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="117" customHeight="1" spans="1:4">
+      <c r="D116" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="117" customHeight="1" spans="1:3">
       <c r="A117" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D117" s="2" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="118" customHeight="1" spans="1:3">
+    </row>
+    <row r="118" customHeight="1" spans="1:4">
       <c r="A118" s="2" t="s">
         <v>247</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="D118" s="2" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="119" customHeight="1" spans="1:3">
       <c r="A119" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="120" customHeight="1" spans="1:4">
+    <row r="120" customHeight="1" spans="1:3">
       <c r="A120" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="D120" s="2" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="121" customHeight="1" spans="1:4">
@@ -7480,38 +7480,38 @@
         <v>251</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D121" s="1" t="s">
+      <c r="D121" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="122" customHeight="1" spans="1:3">
+    <row r="122" customHeight="1" spans="1:4">
       <c r="A122" s="2" t="s">
         <v>253</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="123" customHeight="1" spans="1:4">
+      <c r="D122" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="123" customHeight="1" spans="1:3">
       <c r="A123" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="124" customHeight="1" spans="1:4">
@@ -7519,12 +7519,12 @@
         <v>256</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D124" s="2" t="s">
+      <c r="D124" s="1" t="s">
         <v>257</v>
       </c>
     </row>
@@ -7533,7 +7533,7 @@
         <v>258</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>7</v>
@@ -7543,11 +7543,11 @@
       </c>
     </row>
     <row r="126" customHeight="1" spans="1:4">
-      <c r="A126" s="8" t="s">
+      <c r="A126" s="2" t="s">
         <v>260</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>7</v>
@@ -7561,7 +7561,7 @@
         <v>262</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>7</v>
@@ -7575,21 +7575,21 @@
         <v>264</v>
       </c>
       <c r="B128" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D128" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="C128" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D128" s="2" t="s">
+    </row>
+    <row r="129" customHeight="1" spans="1:4">
+      <c r="A129" s="8" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="129" customHeight="1" spans="1:4">
-      <c r="A129" s="2" t="s">
+      <c r="B129" s="2" t="s">
         <v>267</v>
-      </c>
-      <c r="B129" s="2" t="s">
-        <v>265</v>
       </c>
       <c r="C129" s="2" t="s">
         <v>14</v>
@@ -7602,8 +7602,8 @@
       <c r="A130" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="B130" s="1" t="s">
-        <v>265</v>
+      <c r="B130" s="2" t="s">
+        <v>267</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>14</v>
@@ -7613,11 +7613,11 @@
       </c>
     </row>
     <row r="131" customHeight="1" spans="1:4">
-      <c r="A131" s="8" t="s">
+      <c r="A131" s="2" t="s">
         <v>271</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>14</v>
@@ -7631,7 +7631,7 @@
         <v>273</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>14</v>
@@ -7641,39 +7641,39 @@
       </c>
     </row>
     <row r="133" customHeight="1" spans="1:4">
-      <c r="A133" s="2" t="s">
+      <c r="A133" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B133" s="2" t="s">
-        <v>276</v>
+      <c r="B133" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="C133" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="134" customHeight="1" spans="1:4">
       <c r="A134" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B134" s="2" t="s">
         <v>278</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>279</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="135" customHeight="1" spans="1:4">
       <c r="A135" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B135" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>279</v>
       </c>
       <c r="C135" s="2" t="s">
         <v>14</v>
@@ -7687,181 +7687,181 @@
         <v>283</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C136" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D136" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="137" customHeight="1" spans="1:4">
+      <c r="A137" s="2" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="137" customHeight="1" spans="1:4">
-      <c r="A137" s="3" t="s">
+      <c r="B137" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="B137" s="4" t="s">
+      <c r="C137" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D137" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="C137" s="3" t="s">
+    </row>
+    <row r="138" customHeight="1" spans="1:4">
+      <c r="A138" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C138" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D137" s="16" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="138" customHeight="1" spans="1:4">
-      <c r="A138" s="11" t="s">
-        <v>289</v>
-      </c>
-      <c r="B138" s="11" t="s">
+      <c r="D138" s="16" t="s">
         <v>290</v>
-      </c>
-      <c r="C138" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D138" s="17" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="139" customHeight="1" spans="1:4">
       <c r="A139" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="B139" s="11" t="s">
         <v>292</v>
       </c>
-      <c r="B139" s="11" t="s">
+      <c r="C139" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D139" s="17" t="s">
         <v>293</v>
-      </c>
-      <c r="C139" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D139" s="11" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="140" customHeight="1" spans="1:4">
       <c r="A140" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="B140" s="11" t="s">
         <v>295</v>
-      </c>
-      <c r="B140" s="11" t="s">
-        <v>296</v>
       </c>
       <c r="C140" s="11" t="s">
         <v>14</v>
       </c>
       <c r="D140" s="11" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="141" customHeight="1" spans="1:4">
+      <c r="A141" s="11" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="141" customHeight="1" spans="1:4">
-      <c r="A141" s="2" t="s">
+      <c r="B141" s="11" t="s">
         <v>298</v>
       </c>
-      <c r="B141" s="11" t="s">
+      <c r="C141" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D141" s="11" t="s">
         <v>299</v>
-      </c>
-      <c r="C141" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D141" s="11" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="142" customHeight="1" spans="1:4">
       <c r="A142" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B142" s="11" t="s">
         <v>301</v>
-      </c>
-      <c r="B142" s="11" t="s">
-        <v>302</v>
       </c>
       <c r="C142" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D142" s="11" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="143" customHeight="1" spans="1:4">
-      <c r="A143" s="11" t="s">
+      <c r="A143" s="2" t="s">
         <v>303</v>
       </c>
       <c r="B143" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D143" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="C143" s="11" t="s">
+    </row>
+    <row r="144" customHeight="1" spans="1:4">
+      <c r="A144" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="B144" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="C144" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D143" s="11" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="144" customHeight="1" spans="1:4">
-      <c r="A144" s="2" t="s">
+      <c r="D144" s="11" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="145" customHeight="1" spans="1:4">
+      <c r="A145" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B145" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="B144" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="C144" s="2" t="s">
+      <c r="C145" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D144" s="2" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="145" customHeight="1" spans="1:4">
-      <c r="A145" s="11" t="s">
-        <v>306</v>
-      </c>
-      <c r="B145" s="11" t="s">
+      <c r="D145" s="2" t="s">
         <v>307</v>
-      </c>
-      <c r="C145" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D145" s="11" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="146" customHeight="1" spans="1:4">
       <c r="A146" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="B146" s="11" t="s">
         <v>309</v>
-      </c>
-      <c r="B146" s="11" t="s">
-        <v>307</v>
       </c>
       <c r="C146" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D146" s="2" t="s">
-        <v>308</v>
+      <c r="D146" s="11" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="147" customHeight="1" spans="1:4">
-      <c r="A147" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="B147" s="2" t="s">
+      <c r="A147" s="11" t="s">
         <v>311</v>
+      </c>
+      <c r="B147" s="11" t="s">
+        <v>309</v>
       </c>
       <c r="C147" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D147" s="12" t="s">
-        <v>312</v>
+      <c r="D147" s="2" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="148" customHeight="1" spans="1:4">
       <c r="A148" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B148" s="2" t="s">
         <v>313</v>
-      </c>
-      <c r="B148" s="2" t="s">
-        <v>314</v>
       </c>
       <c r="C148" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D148" s="2" t="s">
-        <v>312</v>
+      <c r="D148" s="12" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="149" customHeight="1" spans="1:4">
@@ -7869,13 +7869,13 @@
         <v>315</v>
       </c>
       <c r="B149" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C149" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D149" s="2" t="s">
         <v>314</v>
-      </c>
-      <c r="C149" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D149" s="12" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="150" customHeight="1" spans="1:4">
@@ -7883,35 +7883,35 @@
         <v>317</v>
       </c>
       <c r="B150" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D150" s="12" t="s">
         <v>318</v>
-      </c>
-      <c r="C150" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D150" s="2" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="151" customHeight="1" spans="1:4">
       <c r="A151" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B151" s="2" t="s">
         <v>320</v>
-      </c>
-      <c r="B151" s="2" t="s">
-        <v>321</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="152" customHeight="1" spans="1:4">
       <c r="A152" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B152" s="2" t="s">
         <v>323</v>
-      </c>
-      <c r="B152" s="2" t="s">
-        <v>321</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>14</v>
@@ -7925,130 +7925,130 @@
         <v>325</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D153" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="154" customHeight="1" spans="1:4">
+      <c r="A154" s="2" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="154" customHeight="1" spans="1:4">
-      <c r="A154" s="1" t="s">
+      <c r="B154" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="B154" s="1" t="s">
+      <c r="C154" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D154" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="C154" s="2" t="s">
+    </row>
+    <row r="155" customHeight="1" spans="1:4">
+      <c r="A155" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C155" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D154" s="2" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="155" customHeight="1" spans="1:4">
-      <c r="A155" s="3" t="s">
+      <c r="D155" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="156" customHeight="1" spans="1:4">
+      <c r="A156" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="B156" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="B155" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="C155" s="3" t="s">
+      <c r="C156" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D155" s="3" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="156" customHeight="1" spans="1:4">
-      <c r="A156" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="B156" s="9" t="s">
+      <c r="D156" s="3" t="s">
         <v>334</v>
-      </c>
-      <c r="C156" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D156" s="2" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="157" customHeight="1" spans="1:4">
       <c r="A157" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B157" s="9" t="s">
         <v>336</v>
-      </c>
-      <c r="B157" s="2" t="s">
-        <v>337</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="158" customHeight="1" spans="1:4">
       <c r="A158" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B158" s="2" t="s">
         <v>339</v>
-      </c>
-      <c r="B158" s="2" t="s">
-        <v>340</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="159" customHeight="1" spans="1:4">
       <c r="A159" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B159" s="2" t="s">
         <v>342</v>
-      </c>
-      <c r="B159" s="2" t="s">
-        <v>343</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D159" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="160" customHeight="1" spans="1:4">
+      <c r="A160" s="2" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="160" customHeight="1" spans="1:3">
-      <c r="A160" s="2" t="s">
+      <c r="B160" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="B160" s="2" t="s">
+      <c r="C160" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D160" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="C160" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="161" customHeight="1" spans="1:4">
+    </row>
+    <row r="161" customHeight="1" spans="1:3">
       <c r="A161" s="2" t="s">
         <v>347</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="C161" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D161" s="2" t="s">
         <v>348</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="162" customHeight="1" spans="1:4">
       <c r="A162" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="B162" s="1" t="b">
-        <v>1</v>
+      <c r="B162" s="2" t="s">
+        <v>348</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>14</v>
@@ -8061,22 +8061,22 @@
       <c r="A163" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="B163" s="2" t="s">
-        <v>352</v>
+      <c r="B163" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="164" customHeight="1" spans="1:4">
       <c r="A164" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B164" s="2" t="s">
         <v>354</v>
-      </c>
-      <c r="B164" s="2" t="s">
-        <v>352</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>14</v>
@@ -8090,35 +8090,35 @@
         <v>356</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="166" customHeight="1" spans="1:4">
       <c r="A166" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B166" s="2" t="s">
         <v>359</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>360</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="167" customHeight="1" spans="1:4">
       <c r="A167" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="B167" s="2" t="s">
         <v>362</v>
-      </c>
-      <c r="B167" s="2" t="s">
-        <v>360</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>14</v>
@@ -8132,131 +8132,131 @@
         <v>364</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C168" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="169" customHeight="1" spans="1:4">
       <c r="A169" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B169" s="2" t="s">
         <v>367</v>
-      </c>
-      <c r="B169" s="2" t="s">
-        <v>368</v>
       </c>
       <c r="C169" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="170" customHeight="1" spans="1:4">
       <c r="A170" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B170" s="2" t="s">
         <v>370</v>
-      </c>
-      <c r="B170" s="2" t="s">
-        <v>371</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="171" customHeight="1" spans="1:4">
       <c r="A171" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B171" s="2" t="s">
         <v>373</v>
-      </c>
-      <c r="B171" s="2" t="s">
-        <v>374</v>
       </c>
       <c r="C171" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="172" customHeight="1" spans="1:4">
       <c r="A172" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="B172" s="2" t="s">
         <v>376</v>
-      </c>
-      <c r="B172" s="2" t="s">
-        <v>377</v>
       </c>
       <c r="C172" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="173" customHeight="1" spans="1:4">
       <c r="A173" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="B173" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="B173" s="2" t="s">
+      <c r="C173" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D173" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="C173" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D173" s="2"/>
     </row>
     <row r="174" customHeight="1" spans="1:4">
       <c r="A174" s="2" t="s">
         <v>381</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="C174" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D174" s="2" t="s">
         <v>382</v>
       </c>
+      <c r="C174" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D174" s="2"/>
     </row>
     <row r="175" customHeight="1" spans="1:4">
       <c r="A175" s="2" t="s">
         <v>383</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="176" customHeight="1" spans="1:4">
       <c r="A176" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="B176" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="B176" s="2" t="s">
-        <v>387</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="177" customHeight="1" spans="1:4">
       <c r="A177" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="B177" s="2" t="s">
         <v>389</v>
-      </c>
-      <c r="B177" s="2" t="s">
-        <v>220</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>14</v>
@@ -16906,8 +16906,8 @@
     <mergeCell ref="A1:D2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B154" r:id="rId1" display="fripSide" tooltip="fripSide"/>
     <hyperlink ref="B155" r:id="rId1" display="fripSide" tooltip="fripSide"/>
+    <hyperlink ref="B156" r:id="rId1" display="fripSide" tooltip="fripSide"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>

<commit_message>
v0.1.3 update, updated song list 230102
</commit_message>
<xml_diff>
--- a/歌单.xlsx
+++ b/歌单.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3052" uniqueCount="1578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3055" uniqueCount="1579">
   <si>
     <t>2022年3月22日18:18:30更新</t>
   </si>
@@ -4547,6 +4547,9 @@
   </si>
   <si>
     <t>如水</t>
+  </si>
+  <si>
+    <t>一格格</t>
   </si>
   <si>
     <t>如风</t>
@@ -4793,45 +4796,45 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="39">
+    <numFmt numFmtId="6" formatCode="&quot;￥&quot;#,##0;[Red]&quot;￥&quot;\-#,##0"/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="6" formatCode="&quot;￥&quot;#,##0;[Red]&quot;￥&quot;\-#,##0"/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="23" formatCode="\$#,##0_);\(\$#,##0\)"/>
+    <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
+    <numFmt numFmtId="25" formatCode="\$#,##0.00_);\(\$#,##0.00\)"/>
     <numFmt numFmtId="176" formatCode="#\ ??/??"/>
     <numFmt numFmtId="177" formatCode="mmmm\-yy"/>
+    <numFmt numFmtId="178" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
+    <numFmt numFmtId="179" formatCode="[DBNum1][$-804]m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="180" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
+    <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
+    <numFmt numFmtId="181" formatCode="#\ ?/?"/>
+    <numFmt numFmtId="182" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="183" formatCode="mmmmm\-yy"/>
+    <numFmt numFmtId="184" formatCode="h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="185" formatCode="\¥#,##0.00;[Red]\¥\-#,##0.00"/>
+    <numFmt numFmtId="186" formatCode="yy/m/d"/>
+    <numFmt numFmtId="187" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="188" formatCode="m/d"/>
+    <numFmt numFmtId="189" formatCode="\¥#,##0;\¥\-#,##0"/>
+    <numFmt numFmtId="190" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;"/>
+    <numFmt numFmtId="191" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
+    <numFmt numFmtId="192" formatCode="h:mm\ AM/PM"/>
+    <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="193" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="194" formatCode="dd\-mmm\-yy"/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="195" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
+    <numFmt numFmtId="196" formatCode="mmmmm"/>
+    <numFmt numFmtId="197" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="198" formatCode="[$-804]aaa"/>
+    <numFmt numFmtId="199" formatCode="[$-804]aaaa"/>
+    <numFmt numFmtId="200" formatCode="#\ ??"/>
+    <numFmt numFmtId="201" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
     <numFmt numFmtId="5" formatCode="&quot;￥&quot;#,##0;&quot;￥&quot;\-#,##0"/>
-    <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="178" formatCode="#\ ?/?"/>
-    <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
-    <numFmt numFmtId="179" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
-    <numFmt numFmtId="180" formatCode="[$-804]aaa"/>
-    <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
-    <numFmt numFmtId="181" formatCode="h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="182" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
-    <numFmt numFmtId="183" formatCode="[DBNum1][$-804]m&quot;月&quot;d&quot;日&quot;"/>
     <numFmt numFmtId="8" formatCode="&quot;￥&quot;#,##0.00;[Red]&quot;￥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="184" formatCode="mm/dd/yy"/>
-    <numFmt numFmtId="185" formatCode="yy/m/d"/>
-    <numFmt numFmtId="186" formatCode="[=1]&quot;☑&quot;;[=0]&quot;☐&quot;;0;@"/>
-    <numFmt numFmtId="187" formatCode="dd\-mmm\-yy"/>
-    <numFmt numFmtId="188" formatCode="mmmmm"/>
-    <numFmt numFmtId="189" formatCode="mmmmm\-yy"/>
-    <numFmt numFmtId="190" formatCode="m/d"/>
-    <numFmt numFmtId="25" formatCode="\$#,##0.00_);\(\$#,##0.00\)"/>
-    <numFmt numFmtId="191" formatCode="h:mm\ AM/PM"/>
-    <numFmt numFmtId="192" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
-    <numFmt numFmtId="193" formatCode="\¥#,##0.00;[Red]\¥\-#,##0.00"/>
-    <numFmt numFmtId="194" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;"/>
-    <numFmt numFmtId="195" formatCode="[$-804]aaaa"/>
-    <numFmt numFmtId="196" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
-    <numFmt numFmtId="197" formatCode="\¥#,##0;\¥\-#,##0"/>
-    <numFmt numFmtId="198" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="199" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
-    <numFmt numFmtId="200" formatCode="#\ ??"/>
-    <numFmt numFmtId="201" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
-    <numFmt numFmtId="23" formatCode="\$#,##0_);\(\$#,##0\)"/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="202" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="202" formatCode="[=1]&quot;☑&quot;;[=0]&quot;☐&quot;;0;@"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -4892,14 +4895,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -4907,9 +4918,33 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4921,9 +4956,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4945,54 +4987,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -5007,24 +5011,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -5049,7 +5052,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5061,31 +5136,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5097,25 +5178,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5127,25 +5202,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5157,79 +5232,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5289,6 +5292,45 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -5330,45 +5372,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -5382,145 +5385,145 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="34" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="202" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="197" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="193" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="198" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -5540,7 +5543,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="202" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5564,7 +5567,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="186" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="202" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5585,10 +5588,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="202" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="202" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5919,14 +5922,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E954"/>
+  <dimension ref="A1:E955"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="3" topLeftCell="E104" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E104" sqref="$A1:$XFD1048576"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.625" defaultRowHeight="23.5" customHeight="1" outlineLevelCol="4"/>
@@ -19316,18 +19319,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="913" customHeight="1" spans="1:5">
+    <row r="913" customHeight="1" spans="1:3">
       <c r="A913" s="2" t="s">
         <v>1510</v>
       </c>
       <c r="B913" s="2" t="s">
-        <v>674</v>
+        <v>1508</v>
       </c>
       <c r="C913" s="2" t="s">
         <v>837</v>
-      </c>
-      <c r="E913" s="4">
-        <v>0</v>
       </c>
     </row>
     <row r="914" customHeight="1" spans="1:5">
@@ -19335,7 +19335,7 @@
         <v>1511</v>
       </c>
       <c r="B914" s="2" t="s">
-        <v>1512</v>
+        <v>674</v>
       </c>
       <c r="C914" s="2" t="s">
         <v>837</v>
@@ -19346,13 +19346,13 @@
     </row>
     <row r="915" customHeight="1" spans="1:5">
       <c r="A915" s="2" t="s">
+        <v>1512</v>
+      </c>
+      <c r="B915" s="2" t="s">
         <v>1513</v>
       </c>
-      <c r="B915" s="2" t="s">
-        <v>1514</v>
-      </c>
       <c r="C915" s="2" t="s">
-        <v>1515</v>
+        <v>837</v>
       </c>
       <c r="E915" s="4">
         <v>0</v>
@@ -19360,13 +19360,13 @@
     </row>
     <row r="916" customHeight="1" spans="1:5">
       <c r="A916" s="2" t="s">
+        <v>1514</v>
+      </c>
+      <c r="B916" s="2" t="s">
+        <v>1515</v>
+      </c>
+      <c r="C916" s="2" t="s">
         <v>1516</v>
-      </c>
-      <c r="B916" s="2" t="s">
-        <v>1517</v>
-      </c>
-      <c r="C916" s="2" t="s">
-        <v>1515</v>
       </c>
       <c r="E916" s="4">
         <v>0</v>
@@ -19374,13 +19374,13 @@
     </row>
     <row r="917" customHeight="1" spans="1:5">
       <c r="A917" s="2" t="s">
+        <v>1517</v>
+      </c>
+      <c r="B917" s="2" t="s">
         <v>1518</v>
       </c>
-      <c r="B917" s="2" t="s">
-        <v>1517</v>
-      </c>
       <c r="C917" s="2" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="E917" s="4">
         <v>0</v>
@@ -19391,10 +19391,10 @@
         <v>1519</v>
       </c>
       <c r="B918" s="2" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="C918" s="2" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="E918" s="4">
         <v>0</v>
@@ -19405,10 +19405,10 @@
         <v>1520</v>
       </c>
       <c r="B919" s="2" t="s">
-        <v>1501</v>
+        <v>1518</v>
       </c>
       <c r="C919" s="2" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="E919" s="4">
         <v>0</v>
@@ -19419,10 +19419,10 @@
         <v>1521</v>
       </c>
       <c r="B920" s="2" t="s">
-        <v>1295</v>
+        <v>1501</v>
       </c>
       <c r="C920" s="2" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="E920" s="4">
         <v>0</v>
@@ -19433,10 +19433,10 @@
         <v>1522</v>
       </c>
       <c r="B921" s="2" t="s">
-        <v>1523</v>
+        <v>1295</v>
       </c>
       <c r="C921" s="2" t="s">
-        <v>1092</v>
+        <v>1516</v>
       </c>
       <c r="E921" s="4">
         <v>0</v>
@@ -19444,10 +19444,10 @@
     </row>
     <row r="922" customHeight="1" spans="1:5">
       <c r="A922" s="2" t="s">
+        <v>1523</v>
+      </c>
+      <c r="B922" s="2" t="s">
         <v>1524</v>
-      </c>
-      <c r="B922" s="2" t="s">
-        <v>1525</v>
       </c>
       <c r="C922" s="2" t="s">
         <v>1092</v>
@@ -19458,10 +19458,10 @@
     </row>
     <row r="923" customHeight="1" spans="1:5">
       <c r="A923" s="2" t="s">
+        <v>1525</v>
+      </c>
+      <c r="B923" s="2" t="s">
         <v>1526</v>
-      </c>
-      <c r="B923" s="2" t="s">
-        <v>1527</v>
       </c>
       <c r="C923" s="2" t="s">
         <v>1092</v>
@@ -19472,10 +19472,10 @@
     </row>
     <row r="924" customHeight="1" spans="1:5">
       <c r="A924" s="2" t="s">
+        <v>1527</v>
+      </c>
+      <c r="B924" s="2" t="s">
         <v>1528</v>
-      </c>
-      <c r="B924" s="2" t="s">
-        <v>1529</v>
       </c>
       <c r="C924" s="2" t="s">
         <v>1092</v>
@@ -19486,10 +19486,10 @@
     </row>
     <row r="925" customHeight="1" spans="1:5">
       <c r="A925" s="2" t="s">
+        <v>1529</v>
+      </c>
+      <c r="B925" s="2" t="s">
         <v>1530</v>
-      </c>
-      <c r="B925" s="2" t="s">
-        <v>1531</v>
       </c>
       <c r="C925" s="2" t="s">
         <v>1092</v>
@@ -19500,10 +19500,10 @@
     </row>
     <row r="926" customHeight="1" spans="1:5">
       <c r="A926" s="2" t="s">
+        <v>1531</v>
+      </c>
+      <c r="B926" s="2" t="s">
         <v>1532</v>
-      </c>
-      <c r="B926" s="2" t="s">
-        <v>1533</v>
       </c>
       <c r="C926" s="2" t="s">
         <v>1092</v>
@@ -19514,10 +19514,10 @@
     </row>
     <row r="927" customHeight="1" spans="1:5">
       <c r="A927" s="2" t="s">
+        <v>1533</v>
+      </c>
+      <c r="B927" s="2" t="s">
         <v>1534</v>
-      </c>
-      <c r="B927" s="2" t="s">
-        <v>1535</v>
       </c>
       <c r="C927" s="2" t="s">
         <v>1092</v>
@@ -19528,10 +19528,10 @@
     </row>
     <row r="928" customHeight="1" spans="1:5">
       <c r="A928" s="2" t="s">
+        <v>1535</v>
+      </c>
+      <c r="B928" s="2" t="s">
         <v>1536</v>
-      </c>
-      <c r="B928" s="2" t="s">
-        <v>814</v>
       </c>
       <c r="C928" s="2" t="s">
         <v>1092</v>
@@ -19545,7 +19545,7 @@
         <v>1537</v>
       </c>
       <c r="B929" s="2" t="s">
-        <v>1529</v>
+        <v>814</v>
       </c>
       <c r="C929" s="2" t="s">
         <v>1092</v>
@@ -19559,7 +19559,7 @@
         <v>1538</v>
       </c>
       <c r="B930" s="2" t="s">
-        <v>1539</v>
+        <v>1530</v>
       </c>
       <c r="C930" s="2" t="s">
         <v>1092</v>
@@ -19570,10 +19570,10 @@
     </row>
     <row r="931" customHeight="1" spans="1:5">
       <c r="A931" s="2" t="s">
+        <v>1539</v>
+      </c>
+      <c r="B931" s="2" t="s">
         <v>1540</v>
-      </c>
-      <c r="B931" s="2" t="s">
-        <v>1525</v>
       </c>
       <c r="C931" s="2" t="s">
         <v>1092</v>
@@ -19587,7 +19587,7 @@
         <v>1541</v>
       </c>
       <c r="B932" s="2" t="s">
-        <v>1529</v>
+        <v>1526</v>
       </c>
       <c r="C932" s="2" t="s">
         <v>1092</v>
@@ -19601,7 +19601,7 @@
         <v>1542</v>
       </c>
       <c r="B933" s="2" t="s">
-        <v>1535</v>
+        <v>1530</v>
       </c>
       <c r="C933" s="2" t="s">
         <v>1092</v>
@@ -19615,7 +19615,7 @@
         <v>1543</v>
       </c>
       <c r="B934" s="2" t="s">
-        <v>1533</v>
+        <v>1536</v>
       </c>
       <c r="C934" s="2" t="s">
         <v>1092</v>
@@ -19629,7 +19629,7 @@
         <v>1544</v>
       </c>
       <c r="B935" s="2" t="s">
-        <v>1529</v>
+        <v>1534</v>
       </c>
       <c r="C935" s="2" t="s">
         <v>1092</v>
@@ -19643,7 +19643,7 @@
         <v>1545</v>
       </c>
       <c r="B936" s="2" t="s">
-        <v>1546</v>
+        <v>1530</v>
       </c>
       <c r="C936" s="2" t="s">
         <v>1092</v>
@@ -19654,10 +19654,10 @@
     </row>
     <row r="937" customHeight="1" spans="1:5">
       <c r="A937" s="2" t="s">
+        <v>1546</v>
+      </c>
+      <c r="B937" s="2" t="s">
         <v>1547</v>
-      </c>
-      <c r="B937" s="2" t="s">
-        <v>1529</v>
       </c>
       <c r="C937" s="2" t="s">
         <v>1092</v>
@@ -19671,7 +19671,7 @@
         <v>1548</v>
       </c>
       <c r="B938" s="2" t="s">
-        <v>1549</v>
+        <v>1530</v>
       </c>
       <c r="C938" s="2" t="s">
         <v>1092</v>
@@ -19682,10 +19682,10 @@
     </row>
     <row r="939" customHeight="1" spans="1:5">
       <c r="A939" s="2" t="s">
+        <v>1549</v>
+      </c>
+      <c r="B939" s="2" t="s">
         <v>1550</v>
-      </c>
-      <c r="B939" s="2" t="s">
-        <v>1551</v>
       </c>
       <c r="C939" s="2" t="s">
         <v>1092</v>
@@ -19696,10 +19696,10 @@
     </row>
     <row r="940" customHeight="1" spans="1:5">
       <c r="A940" s="2" t="s">
+        <v>1551</v>
+      </c>
+      <c r="B940" s="2" t="s">
         <v>1552</v>
-      </c>
-      <c r="B940" s="2" t="s">
-        <v>1553</v>
       </c>
       <c r="C940" s="2" t="s">
         <v>1092</v>
@@ -19710,10 +19710,10 @@
     </row>
     <row r="941" customHeight="1" spans="1:5">
       <c r="A941" s="2" t="s">
+        <v>1553</v>
+      </c>
+      <c r="B941" s="2" t="s">
         <v>1554</v>
-      </c>
-      <c r="B941" s="2" t="s">
-        <v>1555</v>
       </c>
       <c r="C941" s="2" t="s">
         <v>1092</v>
@@ -19724,56 +19724,56 @@
     </row>
     <row r="942" customHeight="1" spans="1:5">
       <c r="A942" s="2" t="s">
+        <v>1555</v>
+      </c>
+      <c r="B942" s="2" t="s">
         <v>1556</v>
-      </c>
-      <c r="B942" s="10" t="s">
-        <v>1557</v>
       </c>
       <c r="C942" s="2" t="s">
         <v>1092</v>
       </c>
-      <c r="D942" s="2" t="s">
-        <v>1558</v>
-      </c>
       <c r="E942" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="943" customHeight="1" spans="1:5">
       <c r="A943" s="2" t="s">
-        <v>1559</v>
+        <v>1557</v>
       </c>
       <c r="B943" s="10" t="s">
-        <v>1560</v>
+        <v>1558</v>
       </c>
       <c r="C943" s="2" t="s">
         <v>1092</v>
       </c>
-      <c r="D943" s="2"/>
+      <c r="D943" s="2" t="s">
+        <v>1559</v>
+      </c>
       <c r="E943" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="944" customHeight="1" spans="1:5">
       <c r="A944" s="2" t="s">
+        <v>1560</v>
+      </c>
+      <c r="B944" s="10" t="s">
         <v>1561</v>
-      </c>
-      <c r="B944" s="2" t="s">
-        <v>1562</v>
       </c>
       <c r="C944" s="2" t="s">
         <v>1092</v>
       </c>
+      <c r="D944" s="2"/>
       <c r="E944" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="945" customHeight="1" spans="1:5">
       <c r="A945" s="2" t="s">
+        <v>1562</v>
+      </c>
+      <c r="B945" s="2" t="s">
         <v>1563</v>
-      </c>
-      <c r="B945" s="2" t="s">
-        <v>1529</v>
       </c>
       <c r="C945" s="2" t="s">
         <v>1092</v>
@@ -19787,7 +19787,7 @@
         <v>1564</v>
       </c>
       <c r="B946" s="2" t="s">
-        <v>1546</v>
+        <v>1530</v>
       </c>
       <c r="C946" s="2" t="s">
         <v>1092</v>
@@ -19801,7 +19801,7 @@
         <v>1565</v>
       </c>
       <c r="B947" s="2" t="s">
-        <v>1566</v>
+        <v>1547</v>
       </c>
       <c r="C947" s="2" t="s">
         <v>1092</v>
@@ -19812,10 +19812,10 @@
     </row>
     <row r="948" customHeight="1" spans="1:5">
       <c r="A948" s="2" t="s">
+        <v>1566</v>
+      </c>
+      <c r="B948" s="2" t="s">
         <v>1567</v>
-      </c>
-      <c r="B948" s="2" t="s">
-        <v>1535</v>
       </c>
       <c r="C948" s="2" t="s">
         <v>1092</v>
@@ -19829,7 +19829,7 @@
         <v>1568</v>
       </c>
       <c r="B949" s="2" t="s">
-        <v>1529</v>
+        <v>1536</v>
       </c>
       <c r="C949" s="2" t="s">
         <v>1092</v>
@@ -19842,8 +19842,8 @@
       <c r="A950" s="2" t="s">
         <v>1569</v>
       </c>
-      <c r="B950" s="10" t="s">
-        <v>1570</v>
+      <c r="B950" s="2" t="s">
+        <v>1530</v>
       </c>
       <c r="C950" s="2" t="s">
         <v>1092</v>
@@ -19854,10 +19854,10 @@
     </row>
     <row r="951" customHeight="1" spans="1:5">
       <c r="A951" s="2" t="s">
+        <v>1570</v>
+      </c>
+      <c r="B951" s="10" t="s">
         <v>1571</v>
-      </c>
-      <c r="B951" s="2" t="s">
-        <v>1533</v>
       </c>
       <c r="C951" s="2" t="s">
         <v>1092</v>
@@ -19871,7 +19871,7 @@
         <v>1572</v>
       </c>
       <c r="B952" s="2" t="s">
-        <v>1529</v>
+        <v>1534</v>
       </c>
       <c r="C952" s="2" t="s">
         <v>1092</v>
@@ -19885,7 +19885,7 @@
         <v>1573</v>
       </c>
       <c r="B953" s="2" t="s">
-        <v>1535</v>
+        <v>1530</v>
       </c>
       <c r="C953" s="2" t="s">
         <v>1092</v>
@@ -19895,19 +19895,33 @@
       </c>
     </row>
     <row r="954" customHeight="1" spans="1:5">
-      <c r="A954" s="23" t="s">
+      <c r="A954" s="2" t="s">
         <v>1574</v>
       </c>
       <c r="B954" s="2" t="s">
+        <v>1536</v>
+      </c>
+      <c r="C954" s="2" t="s">
+        <v>1092</v>
+      </c>
+      <c r="E954" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="955" customHeight="1" spans="1:5">
+      <c r="A955" s="23" t="s">
         <v>1575</v>
       </c>
-      <c r="C954" s="2" t="s">
+      <c r="B955" s="2" t="s">
         <v>1576</v>
       </c>
-      <c r="D954" s="2" t="s">
+      <c r="C955" s="2" t="s">
         <v>1577</v>
       </c>
-      <c r="E954" s="4">
+      <c r="D955" s="2" t="s">
+        <v>1578</v>
+      </c>
+      <c r="E955" s="4">
         <v>0</v>
       </c>
     </row>
@@ -19917,7 +19931,7 @@
     <mergeCell ref="A1:D2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="输入内容有误" error="请选择勾选或取消勾选" sqref="E104 E2:E103 E105:E1048576">
+    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="输入内容有误" error="请选择勾选或取消勾选" sqref="E913 E2:E912 E914:E1048576">
       <formula1>IF(TRUE,OR(E2=0,E2=1),"Checkbox")</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
v0.1.5 update, updated song list 2023/3/4
</commit_message>
<xml_diff>
--- a/歌单.xlsx
+++ b/歌单.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3062" uniqueCount="1585">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3059" uniqueCount="1584">
   <si>
     <t>2022年3月22日18:18:30更新</t>
   </si>
@@ -3503,9 +3503,6 @@
   </si>
   <si>
     <t>山外小楼夜听雨</t>
-  </si>
-  <si>
-    <t>Super star</t>
   </si>
   <si>
     <t>讨厌</t>
@@ -4814,45 +4811,45 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="39">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;"/>
     <numFmt numFmtId="6" formatCode="&quot;￥&quot;#,##0;[Red]&quot;￥&quot;\-#,##0"/>
+    <numFmt numFmtId="177" formatCode="\¥#,##0.00;[Red]\¥\-#,##0.00"/>
+    <numFmt numFmtId="23" formatCode="\$#,##0_);\(\$#,##0\)"/>
+    <numFmt numFmtId="178" formatCode="#\ ??/??"/>
+    <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
+    <numFmt numFmtId="179" formatCode="#\ ?/?"/>
+    <numFmt numFmtId="180" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
+    <numFmt numFmtId="181" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
+    <numFmt numFmtId="182" formatCode="[$-804]aaa"/>
+    <numFmt numFmtId="25" formatCode="\$#,##0.00_);\(\$#,##0.00\)"/>
+    <numFmt numFmtId="183" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="184" formatCode="m/d"/>
+    <numFmt numFmtId="185" formatCode="mmmmm\-yy"/>
+    <numFmt numFmtId="186" formatCode="h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="8" formatCode="&quot;￥&quot;#,##0.00;[Red]&quot;￥&quot;\-#,##0.00"/>
+    <numFmt numFmtId="187" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="188" formatCode="mmmmm"/>
+    <numFmt numFmtId="189" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
+    <numFmt numFmtId="190" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="\¥#,##0.00;[Red]\¥\-#,##0.00"/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="#\ ??/??"/>
-    <numFmt numFmtId="178" formatCode="mmmm\-yy"/>
-    <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
-    <numFmt numFmtId="23" formatCode="\$#,##0_);\(\$#,##0\)"/>
-    <numFmt numFmtId="179" formatCode="#\ ?/?"/>
-    <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="180" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
-    <numFmt numFmtId="181" formatCode="[$-804]aaa"/>
-    <numFmt numFmtId="182" formatCode="h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="183" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
-    <numFmt numFmtId="184" formatCode="h:mm\ AM/PM"/>
-    <numFmt numFmtId="185" formatCode="[$-804]aaaa"/>
-    <numFmt numFmtId="186" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
-    <numFmt numFmtId="187" formatCode="mm/dd/yy"/>
-    <numFmt numFmtId="188" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
-    <numFmt numFmtId="25" formatCode="\$#,##0.00_);\(\$#,##0.00\)"/>
-    <numFmt numFmtId="189" formatCode="yy/m/d"/>
-    <numFmt numFmtId="190" formatCode="mmmmm"/>
-    <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
-    <numFmt numFmtId="191" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;"/>
-    <numFmt numFmtId="192" formatCode="mmmmm\-yy"/>
-    <numFmt numFmtId="193" formatCode="m/d"/>
-    <numFmt numFmtId="194" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="195" formatCode="#\ ??"/>
-    <numFmt numFmtId="196" formatCode="dd\-mmm\-yy"/>
-    <numFmt numFmtId="197" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
-    <numFmt numFmtId="198" formatCode="[DBNum1][$-804]m&quot;月&quot;d&quot;日&quot;"/>
-    <numFmt numFmtId="199" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
-    <numFmt numFmtId="8" formatCode="&quot;￥&quot;#,##0.00;[Red]&quot;￥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="200" formatCode="[=1]&quot;☑&quot;;[=0]&quot;☐&quot;;0;@"/>
-    <numFmt numFmtId="201" formatCode="\¥#,##0;\¥\-#,##0"/>
+    <numFmt numFmtId="191" formatCode="yy/m/d"/>
+    <numFmt numFmtId="192" formatCode="h:mm\ AM/PM"/>
+    <numFmt numFmtId="193" formatCode="[$-804]aaaa"/>
+    <numFmt numFmtId="194" formatCode="[=1]&quot;☑&quot;;[=0]&quot;☐&quot;;0;@"/>
     <numFmt numFmtId="5" formatCode="&quot;￥&quot;#,##0;&quot;￥&quot;\-#,##0"/>
-    <numFmt numFmtId="202" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="195" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
+    <numFmt numFmtId="196" formatCode="\¥#,##0;\¥\-#,##0"/>
+    <numFmt numFmtId="197" formatCode="#\ ??"/>
+    <numFmt numFmtId="198" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="199" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
+    <numFmt numFmtId="200" formatCode="dd\-mmm\-yy"/>
+    <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
+    <numFmt numFmtId="201" formatCode="mmmm\-yy"/>
+    <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
+    <numFmt numFmtId="202" formatCode="[DBNum1][$-804]m&quot;月&quot;d&quot;日&quot;"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -4906,16 +4903,39 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4927,23 +4947,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4957,22 +4963,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4988,14 +4981,37 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -5009,41 +5025,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -5070,7 +5067,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5082,25 +5145,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5112,19 +5175,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5136,121 +5241,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5304,15 +5301,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -5343,28 +5331,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5384,17 +5361,37 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5403,148 +5400,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="194" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="198" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="190" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="202" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -5561,7 +5558,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="200" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="194" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5588,7 +5585,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="200" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="194" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5609,10 +5606,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="200" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="194" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="200" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="194" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5943,14 +5940,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E957"/>
+  <dimension ref="A1:E956"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E104" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A1" sqref="$A1:$XFD1048576"/>
+      <selection pane="bottomRight" activeCell="A646" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.625" defaultRowHeight="23.5" customHeight="1" outlineLevelCol="4"/>
@@ -15591,7 +15588,7 @@
         <v>1162</v>
       </c>
       <c r="B646" s="2" t="s">
-        <v>647</v>
+        <v>852</v>
       </c>
       <c r="C646" s="2" t="s">
         <v>553</v>
@@ -15605,7 +15602,7 @@
         <v>1163</v>
       </c>
       <c r="B647" s="2" t="s">
-        <v>852</v>
+        <v>1164</v>
       </c>
       <c r="C647" s="2" t="s">
         <v>553</v>
@@ -15616,10 +15613,10 @@
     </row>
     <row r="648" customHeight="1" spans="1:5">
       <c r="A648" s="2" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="B648" s="2" t="s">
-        <v>1165</v>
+        <v>604</v>
       </c>
       <c r="C648" s="2" t="s">
         <v>553</v>
@@ -15629,30 +15626,30 @@
       </c>
     </row>
     <row r="649" customHeight="1" spans="1:5">
-      <c r="A649" s="2" t="s">
+      <c r="A649" s="5" t="s">
         <v>1166</v>
       </c>
-      <c r="B649" s="2" t="s">
-        <v>604</v>
-      </c>
-      <c r="C649" s="2" t="s">
-        <v>553</v>
-      </c>
+      <c r="B649" s="5" t="s">
+        <v>590</v>
+      </c>
+      <c r="C649" s="5" t="s">
+        <v>591</v>
+      </c>
+      <c r="D649" s="6"/>
       <c r="E649" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="650" customHeight="1" spans="1:5">
-      <c r="A650" s="5" t="s">
+      <c r="A650" s="2" t="s">
         <v>1167</v>
       </c>
-      <c r="B650" s="5" t="s">
-        <v>590</v>
-      </c>
-      <c r="C650" s="5" t="s">
-        <v>591</v>
-      </c>
-      <c r="D650" s="6"/>
+      <c r="B650" s="2" t="s">
+        <v>835</v>
+      </c>
+      <c r="C650" s="2" t="s">
+        <v>553</v>
+      </c>
       <c r="E650" s="4">
         <v>0</v>
       </c>
@@ -15662,7 +15659,7 @@
         <v>1168</v>
       </c>
       <c r="B651" s="2" t="s">
-        <v>835</v>
+        <v>557</v>
       </c>
       <c r="C651" s="2" t="s">
         <v>553</v>
@@ -15676,7 +15673,7 @@
         <v>1169</v>
       </c>
       <c r="B652" s="2" t="s">
-        <v>557</v>
+        <v>912</v>
       </c>
       <c r="C652" s="2" t="s">
         <v>553</v>
@@ -15690,7 +15687,7 @@
         <v>1170</v>
       </c>
       <c r="B653" s="2" t="s">
-        <v>912</v>
+        <v>622</v>
       </c>
       <c r="C653" s="2" t="s">
         <v>553</v>
@@ -15704,7 +15701,7 @@
         <v>1171</v>
       </c>
       <c r="B654" s="2" t="s">
-        <v>622</v>
+        <v>657</v>
       </c>
       <c r="C654" s="2" t="s">
         <v>553</v>
@@ -15718,7 +15715,7 @@
         <v>1172</v>
       </c>
       <c r="B655" s="2" t="s">
-        <v>657</v>
+        <v>645</v>
       </c>
       <c r="C655" s="2" t="s">
         <v>553</v>
@@ -15732,7 +15729,7 @@
         <v>1173</v>
       </c>
       <c r="B656" s="2" t="s">
-        <v>645</v>
+        <v>1174</v>
       </c>
       <c r="C656" s="2" t="s">
         <v>553</v>
@@ -15743,10 +15740,10 @@
     </row>
     <row r="657" customHeight="1" spans="1:5">
       <c r="A657" s="2" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="B657" s="2" t="s">
-        <v>1175</v>
+        <v>647</v>
       </c>
       <c r="C657" s="2" t="s">
         <v>553</v>
@@ -15760,7 +15757,7 @@
         <v>1176</v>
       </c>
       <c r="B658" s="2" t="s">
-        <v>647</v>
+        <v>677</v>
       </c>
       <c r="C658" s="2" t="s">
         <v>553</v>
@@ -15774,7 +15771,7 @@
         <v>1177</v>
       </c>
       <c r="B659" s="2" t="s">
-        <v>677</v>
+        <v>1178</v>
       </c>
       <c r="C659" s="2" t="s">
         <v>553</v>
@@ -15785,10 +15782,10 @@
     </row>
     <row r="660" customHeight="1" spans="1:5">
       <c r="A660" s="2" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="B660" s="2" t="s">
-        <v>1179</v>
+        <v>645</v>
       </c>
       <c r="C660" s="2" t="s">
         <v>553</v>
@@ -15802,7 +15799,7 @@
         <v>1180</v>
       </c>
       <c r="B661" s="2" t="s">
-        <v>645</v>
+        <v>1181</v>
       </c>
       <c r="C661" s="2" t="s">
         <v>553</v>
@@ -15813,10 +15810,10 @@
     </row>
     <row r="662" customHeight="1" spans="1:5">
       <c r="A662" s="2" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="B662" s="2" t="s">
-        <v>1182</v>
+        <v>557</v>
       </c>
       <c r="C662" s="2" t="s">
         <v>553</v>
@@ -15830,7 +15827,7 @@
         <v>1183</v>
       </c>
       <c r="B663" s="2" t="s">
-        <v>557</v>
+        <v>597</v>
       </c>
       <c r="C663" s="2" t="s">
         <v>553</v>
@@ -15844,38 +15841,39 @@
         <v>1184</v>
       </c>
       <c r="B664" s="2" t="s">
-        <v>597</v>
+        <v>602</v>
       </c>
       <c r="C664" s="2" t="s">
-        <v>553</v>
+        <v>616</v>
       </c>
       <c r="E664" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="665" customHeight="1" spans="1:5">
-      <c r="A665" s="2" t="s">
+      <c r="A665" s="5" t="s">
         <v>1185</v>
       </c>
-      <c r="B665" s="2" t="s">
-        <v>602</v>
-      </c>
-      <c r="C665" s="2" t="s">
-        <v>616</v>
-      </c>
+      <c r="B665" s="5" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C665" s="5" t="s">
+        <v>564</v>
+      </c>
+      <c r="D665" s="6"/>
       <c r="E665" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="666" customHeight="1" spans="1:5">
       <c r="A666" s="5" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="B666" s="5" t="s">
-        <v>1187</v>
+        <v>817</v>
       </c>
       <c r="C666" s="5" t="s">
-        <v>564</v>
+        <v>591</v>
       </c>
       <c r="D666" s="6"/>
       <c r="E666" s="4">
@@ -15883,29 +15881,28 @@
       </c>
     </row>
     <row r="667" customHeight="1" spans="1:5">
-      <c r="A667" s="5" t="s">
+      <c r="A667" s="2" t="s">
         <v>1188</v>
       </c>
-      <c r="B667" s="5" t="s">
-        <v>817</v>
-      </c>
-      <c r="C667" s="5" t="s">
-        <v>591</v>
-      </c>
-      <c r="D667" s="6"/>
+      <c r="B667" s="2" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C667" s="2" t="s">
+        <v>616</v>
+      </c>
       <c r="E667" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="668" customHeight="1" spans="1:5">
       <c r="A668" s="2" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="B668" s="2" t="s">
-        <v>1190</v>
+        <v>552</v>
       </c>
       <c r="C668" s="2" t="s">
-        <v>616</v>
+        <v>553</v>
       </c>
       <c r="E668" s="4">
         <v>0</v>
@@ -15916,7 +15913,7 @@
         <v>1191</v>
       </c>
       <c r="B669" s="2" t="s">
-        <v>552</v>
+        <v>1192</v>
       </c>
       <c r="C669" s="2" t="s">
         <v>553</v>
@@ -15927,10 +15924,10 @@
     </row>
     <row r="670" customHeight="1" spans="1:5">
       <c r="A670" s="2" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="B670" s="2" t="s">
-        <v>1193</v>
+        <v>730</v>
       </c>
       <c r="C670" s="2" t="s">
         <v>553</v>
@@ -15944,7 +15941,7 @@
         <v>1194</v>
       </c>
       <c r="B671" s="2" t="s">
-        <v>730</v>
+        <v>682</v>
       </c>
       <c r="C671" s="2" t="s">
         <v>553</v>
@@ -15958,7 +15955,7 @@
         <v>1195</v>
       </c>
       <c r="B672" s="2" t="s">
-        <v>682</v>
+        <v>880</v>
       </c>
       <c r="C672" s="2" t="s">
         <v>553</v>
@@ -15972,7 +15969,7 @@
         <v>1196</v>
       </c>
       <c r="B673" s="2" t="s">
-        <v>880</v>
+        <v>647</v>
       </c>
       <c r="C673" s="2" t="s">
         <v>553</v>
@@ -15986,7 +15983,7 @@
         <v>1197</v>
       </c>
       <c r="B674" s="2" t="s">
-        <v>647</v>
+        <v>1111</v>
       </c>
       <c r="C674" s="2" t="s">
         <v>553</v>
@@ -16000,7 +15997,7 @@
         <v>1198</v>
       </c>
       <c r="B675" s="2" t="s">
-        <v>1111</v>
+        <v>557</v>
       </c>
       <c r="C675" s="2" t="s">
         <v>553</v>
@@ -16014,7 +16011,7 @@
         <v>1199</v>
       </c>
       <c r="B676" s="2" t="s">
-        <v>557</v>
+        <v>1124</v>
       </c>
       <c r="C676" s="2" t="s">
         <v>553</v>
@@ -16028,7 +16025,7 @@
         <v>1200</v>
       </c>
       <c r="B677" s="2" t="s">
-        <v>1124</v>
+        <v>1201</v>
       </c>
       <c r="C677" s="2" t="s">
         <v>553</v>
@@ -16039,10 +16036,10 @@
     </row>
     <row r="678" customHeight="1" spans="1:5">
       <c r="A678" s="2" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="B678" s="2" t="s">
-        <v>1202</v>
+        <v>597</v>
       </c>
       <c r="C678" s="2" t="s">
         <v>553</v>
@@ -16056,7 +16053,7 @@
         <v>1203</v>
       </c>
       <c r="B679" s="2" t="s">
-        <v>597</v>
+        <v>880</v>
       </c>
       <c r="C679" s="2" t="s">
         <v>553</v>
@@ -16070,7 +16067,7 @@
         <v>1204</v>
       </c>
       <c r="B680" s="2" t="s">
-        <v>880</v>
+        <v>776</v>
       </c>
       <c r="C680" s="2" t="s">
         <v>553</v>
@@ -16084,7 +16081,7 @@
         <v>1205</v>
       </c>
       <c r="B681" s="2" t="s">
-        <v>776</v>
+        <v>649</v>
       </c>
       <c r="C681" s="2" t="s">
         <v>553</v>
@@ -16098,7 +16095,7 @@
         <v>1206</v>
       </c>
       <c r="B682" s="2" t="s">
-        <v>649</v>
+        <v>1006</v>
       </c>
       <c r="C682" s="2" t="s">
         <v>553</v>
@@ -16112,7 +16109,7 @@
         <v>1207</v>
       </c>
       <c r="B683" s="2" t="s">
-        <v>1006</v>
+        <v>677</v>
       </c>
       <c r="C683" s="2" t="s">
         <v>553</v>
@@ -16126,7 +16123,7 @@
         <v>1208</v>
       </c>
       <c r="B684" s="2" t="s">
-        <v>677</v>
+        <v>689</v>
       </c>
       <c r="C684" s="2" t="s">
         <v>553</v>
@@ -16140,10 +16137,10 @@
         <v>1209</v>
       </c>
       <c r="B685" s="2" t="s">
-        <v>689</v>
+        <v>830</v>
       </c>
       <c r="C685" s="2" t="s">
-        <v>553</v>
+        <v>810</v>
       </c>
       <c r="E685" s="4">
         <v>0</v>
@@ -16154,10 +16151,10 @@
         <v>1210</v>
       </c>
       <c r="B686" s="2" t="s">
-        <v>830</v>
+        <v>572</v>
       </c>
       <c r="C686" s="2" t="s">
-        <v>810</v>
+        <v>553</v>
       </c>
       <c r="E686" s="4">
         <v>0</v>
@@ -16168,10 +16165,10 @@
         <v>1211</v>
       </c>
       <c r="B687" s="2" t="s">
-        <v>572</v>
+        <v>693</v>
       </c>
       <c r="C687" s="2" t="s">
-        <v>553</v>
+        <v>616</v>
       </c>
       <c r="E687" s="4">
         <v>0</v>
@@ -16182,10 +16179,10 @@
         <v>1212</v>
       </c>
       <c r="B688" s="2" t="s">
-        <v>693</v>
+        <v>817</v>
       </c>
       <c r="C688" s="2" t="s">
-        <v>616</v>
+        <v>553</v>
       </c>
       <c r="E688" s="4">
         <v>0</v>
@@ -16196,7 +16193,7 @@
         <v>1213</v>
       </c>
       <c r="B689" s="2" t="s">
-        <v>817</v>
+        <v>1214</v>
       </c>
       <c r="C689" s="2" t="s">
         <v>553</v>
@@ -16207,10 +16204,10 @@
     </row>
     <row r="690" customHeight="1" spans="1:5">
       <c r="A690" s="2" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="B690" s="2" t="s">
-        <v>1215</v>
+        <v>557</v>
       </c>
       <c r="C690" s="2" t="s">
         <v>553</v>
@@ -16224,7 +16221,7 @@
         <v>1216</v>
       </c>
       <c r="B691" s="2" t="s">
-        <v>557</v>
+        <v>776</v>
       </c>
       <c r="C691" s="2" t="s">
         <v>553</v>
@@ -16238,7 +16235,7 @@
         <v>1217</v>
       </c>
       <c r="B692" s="2" t="s">
-        <v>776</v>
+        <v>782</v>
       </c>
       <c r="C692" s="2" t="s">
         <v>553</v>
@@ -16252,7 +16249,7 @@
         <v>1218</v>
       </c>
       <c r="B693" s="2" t="s">
-        <v>782</v>
+        <v>649</v>
       </c>
       <c r="C693" s="2" t="s">
         <v>553</v>
@@ -16266,10 +16263,10 @@
         <v>1219</v>
       </c>
       <c r="B694" s="2" t="s">
-        <v>649</v>
+        <v>1220</v>
       </c>
       <c r="C694" s="2" t="s">
-        <v>553</v>
+        <v>1221</v>
       </c>
       <c r="E694" s="4">
         <v>0</v>
@@ -16277,13 +16274,13 @@
     </row>
     <row r="695" customHeight="1" spans="1:5">
       <c r="A695" s="2" t="s">
-        <v>1220</v>
+        <v>1222</v>
       </c>
       <c r="B695" s="2" t="s">
-        <v>1221</v>
+        <v>1223</v>
       </c>
       <c r="C695" s="2" t="s">
-        <v>1222</v>
+        <v>553</v>
       </c>
       <c r="E695" s="4">
         <v>0</v>
@@ -16291,13 +16288,13 @@
     </row>
     <row r="696" customHeight="1" spans="1:5">
       <c r="A696" s="2" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B696" s="2" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="C696" s="2" t="s">
-        <v>553</v>
+        <v>810</v>
       </c>
       <c r="E696" s="4">
         <v>0</v>
@@ -16305,13 +16302,13 @@
     </row>
     <row r="697" customHeight="1" spans="1:5">
       <c r="A697" s="2" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="B697" s="2" t="s">
-        <v>1226</v>
+        <v>593</v>
       </c>
       <c r="C697" s="2" t="s">
-        <v>810</v>
+        <v>553</v>
       </c>
       <c r="E697" s="4">
         <v>0</v>
@@ -16322,7 +16319,7 @@
         <v>1227</v>
       </c>
       <c r="B698" s="2" t="s">
-        <v>593</v>
+        <v>1228</v>
       </c>
       <c r="C698" s="2" t="s">
         <v>553</v>
@@ -16333,10 +16330,10 @@
     </row>
     <row r="699" customHeight="1" spans="1:5">
       <c r="A699" s="2" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="B699" s="2" t="s">
-        <v>1229</v>
+        <v>602</v>
       </c>
       <c r="C699" s="2" t="s">
         <v>553</v>
@@ -16350,7 +16347,7 @@
         <v>1230</v>
       </c>
       <c r="B700" s="2" t="s">
-        <v>602</v>
+        <v>620</v>
       </c>
       <c r="C700" s="2" t="s">
         <v>553</v>
@@ -16364,7 +16361,7 @@
         <v>1231</v>
       </c>
       <c r="B701" s="2" t="s">
-        <v>620</v>
+        <v>645</v>
       </c>
       <c r="C701" s="2" t="s">
         <v>553</v>
@@ -16378,7 +16375,7 @@
         <v>1232</v>
       </c>
       <c r="B702" s="2" t="s">
-        <v>645</v>
+        <v>590</v>
       </c>
       <c r="C702" s="2" t="s">
         <v>553</v>
@@ -16392,7 +16389,7 @@
         <v>1233</v>
       </c>
       <c r="B703" s="2" t="s">
-        <v>590</v>
+        <v>1234</v>
       </c>
       <c r="C703" s="2" t="s">
         <v>553</v>
@@ -16403,10 +16400,10 @@
     </row>
     <row r="704" customHeight="1" spans="1:5">
       <c r="A704" s="2" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="B704" s="2" t="s">
-        <v>1235</v>
+        <v>645</v>
       </c>
       <c r="C704" s="2" t="s">
         <v>553</v>
@@ -16420,7 +16417,7 @@
         <v>1236</v>
       </c>
       <c r="B705" s="2" t="s">
-        <v>645</v>
+        <v>1237</v>
       </c>
       <c r="C705" s="2" t="s">
         <v>553</v>
@@ -16431,10 +16428,10 @@
     </row>
     <row r="706" customHeight="1" spans="1:5">
       <c r="A706" s="2" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="B706" s="2" t="s">
-        <v>1238</v>
+        <v>604</v>
       </c>
       <c r="C706" s="2" t="s">
         <v>553</v>
@@ -16448,7 +16445,7 @@
         <v>1239</v>
       </c>
       <c r="B707" s="2" t="s">
-        <v>604</v>
+        <v>785</v>
       </c>
       <c r="C707" s="2" t="s">
         <v>553</v>
@@ -16462,7 +16459,7 @@
         <v>1240</v>
       </c>
       <c r="B708" s="2" t="s">
-        <v>785</v>
+        <v>1241</v>
       </c>
       <c r="C708" s="2" t="s">
         <v>553</v>
@@ -16473,10 +16470,10 @@
     </row>
     <row r="709" customHeight="1" spans="1:5">
       <c r="A709" s="2" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="B709" s="2" t="s">
-        <v>1242</v>
+        <v>649</v>
       </c>
       <c r="C709" s="2" t="s">
         <v>553</v>
@@ -16490,7 +16487,7 @@
         <v>1243</v>
       </c>
       <c r="B710" s="2" t="s">
-        <v>649</v>
+        <v>1244</v>
       </c>
       <c r="C710" s="2" t="s">
         <v>553</v>
@@ -16501,10 +16498,10 @@
     </row>
     <row r="711" customHeight="1" spans="1:5">
       <c r="A711" s="2" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="B711" s="2" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="C711" s="2" t="s">
         <v>553</v>
@@ -16515,10 +16512,10 @@
     </row>
     <row r="712" customHeight="1" spans="1:5">
       <c r="A712" s="2" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="B712" s="2" t="s">
-        <v>1247</v>
+        <v>817</v>
       </c>
       <c r="C712" s="2" t="s">
         <v>553</v>
@@ -16532,7 +16529,7 @@
         <v>1248</v>
       </c>
       <c r="B713" s="2" t="s">
-        <v>817</v>
+        <v>1249</v>
       </c>
       <c r="C713" s="2" t="s">
         <v>553</v>
@@ -16543,10 +16540,10 @@
     </row>
     <row r="714" customHeight="1" spans="1:5">
       <c r="A714" s="2" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="B714" s="2" t="s">
-        <v>1250</v>
+        <v>997</v>
       </c>
       <c r="C714" s="2" t="s">
         <v>553</v>
@@ -16560,7 +16557,7 @@
         <v>1251</v>
       </c>
       <c r="B715" s="2" t="s">
-        <v>997</v>
+        <v>590</v>
       </c>
       <c r="C715" s="2" t="s">
         <v>553</v>
@@ -16574,7 +16571,7 @@
         <v>1252</v>
       </c>
       <c r="B716" s="2" t="s">
-        <v>590</v>
+        <v>1124</v>
       </c>
       <c r="C716" s="2" t="s">
         <v>553</v>
@@ -16588,7 +16585,7 @@
         <v>1253</v>
       </c>
       <c r="B717" s="2" t="s">
-        <v>1124</v>
+        <v>677</v>
       </c>
       <c r="C717" s="2" t="s">
         <v>553</v>
@@ -16602,7 +16599,7 @@
         <v>1254</v>
       </c>
       <c r="B718" s="2" t="s">
-        <v>677</v>
+        <v>1255</v>
       </c>
       <c r="C718" s="2" t="s">
         <v>553</v>
@@ -16613,10 +16610,10 @@
     </row>
     <row r="719" customHeight="1" spans="1:5">
       <c r="A719" s="2" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="B719" s="2" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="C719" s="2" t="s">
         <v>553</v>
@@ -16627,10 +16624,10 @@
     </row>
     <row r="720" customHeight="1" spans="1:5">
       <c r="A720" s="2" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="B720" s="2" t="s">
-        <v>1258</v>
+        <v>1111</v>
       </c>
       <c r="C720" s="2" t="s">
         <v>553</v>
@@ -16644,7 +16641,7 @@
         <v>1259</v>
       </c>
       <c r="B721" s="2" t="s">
-        <v>1111</v>
+        <v>1228</v>
       </c>
       <c r="C721" s="2" t="s">
         <v>553</v>
@@ -16658,7 +16655,7 @@
         <v>1260</v>
       </c>
       <c r="B722" s="2" t="s">
-        <v>1229</v>
+        <v>1261</v>
       </c>
       <c r="C722" s="2" t="s">
         <v>553</v>
@@ -16669,10 +16666,10 @@
     </row>
     <row r="723" customHeight="1" spans="1:5">
       <c r="A723" s="2" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="B723" s="2" t="s">
-        <v>1262</v>
+        <v>785</v>
       </c>
       <c r="C723" s="2" t="s">
         <v>553</v>
@@ -16686,7 +16683,7 @@
         <v>1263</v>
       </c>
       <c r="B724" s="2" t="s">
-        <v>785</v>
+        <v>955</v>
       </c>
       <c r="C724" s="2" t="s">
         <v>553</v>
@@ -16700,7 +16697,7 @@
         <v>1264</v>
       </c>
       <c r="B725" s="2" t="s">
-        <v>955</v>
+        <v>597</v>
       </c>
       <c r="C725" s="2" t="s">
         <v>553</v>
@@ -16714,7 +16711,7 @@
         <v>1265</v>
       </c>
       <c r="B726" s="2" t="s">
-        <v>597</v>
+        <v>1266</v>
       </c>
       <c r="C726" s="2" t="s">
         <v>553</v>
@@ -16725,10 +16722,10 @@
     </row>
     <row r="727" customHeight="1" spans="1:5">
       <c r="A727" s="2" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="B727" s="2" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="C727" s="2" t="s">
         <v>553</v>
@@ -16739,10 +16736,10 @@
     </row>
     <row r="728" customHeight="1" spans="1:5">
       <c r="A728" s="2" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="B728" s="2" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="C728" s="2" t="s">
         <v>553</v>
@@ -16753,10 +16750,10 @@
     </row>
     <row r="729" customHeight="1" spans="1:5">
       <c r="A729" s="2" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="B729" s="2" t="s">
-        <v>1271</v>
+        <v>677</v>
       </c>
       <c r="C729" s="2" t="s">
         <v>553</v>
@@ -16770,7 +16767,7 @@
         <v>1272</v>
       </c>
       <c r="B730" s="2" t="s">
-        <v>677</v>
+        <v>693</v>
       </c>
       <c r="C730" s="2" t="s">
         <v>553</v>
@@ -16784,7 +16781,7 @@
         <v>1273</v>
       </c>
       <c r="B731" s="2" t="s">
-        <v>693</v>
+        <v>1274</v>
       </c>
       <c r="C731" s="2" t="s">
         <v>553</v>
@@ -16795,10 +16792,10 @@
     </row>
     <row r="732" customHeight="1" spans="1:5">
       <c r="A732" s="2" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="B732" s="2" t="s">
-        <v>1275</v>
+        <v>719</v>
       </c>
       <c r="C732" s="2" t="s">
         <v>553</v>
@@ -16812,7 +16809,7 @@
         <v>1276</v>
       </c>
       <c r="B733" s="2" t="s">
-        <v>719</v>
+        <v>1277</v>
       </c>
       <c r="C733" s="2" t="s">
         <v>553</v>
@@ -16823,10 +16820,10 @@
     </row>
     <row r="734" customHeight="1" spans="1:5">
       <c r="A734" s="2" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="B734" s="2" t="s">
-        <v>1278</v>
+        <v>645</v>
       </c>
       <c r="C734" s="2" t="s">
         <v>553</v>
@@ -16840,7 +16837,7 @@
         <v>1279</v>
       </c>
       <c r="B735" s="2" t="s">
-        <v>645</v>
+        <v>1280</v>
       </c>
       <c r="C735" s="2" t="s">
         <v>553</v>
@@ -16851,13 +16848,13 @@
     </row>
     <row r="736" customHeight="1" spans="1:5">
       <c r="A736" s="2" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="B736" s="2" t="s">
-        <v>1281</v>
+        <v>809</v>
       </c>
       <c r="C736" s="2" t="s">
-        <v>553</v>
+        <v>810</v>
       </c>
       <c r="E736" s="4">
         <v>0</v>
@@ -16868,10 +16865,10 @@
         <v>1282</v>
       </c>
       <c r="B737" s="2" t="s">
-        <v>809</v>
+        <v>1283</v>
       </c>
       <c r="C737" s="2" t="s">
-        <v>810</v>
+        <v>553</v>
       </c>
       <c r="E737" s="4">
         <v>0</v>
@@ -16879,10 +16876,10 @@
     </row>
     <row r="738" customHeight="1" spans="1:5">
       <c r="A738" s="2" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="B738" s="2" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="C738" s="2" t="s">
         <v>553</v>
@@ -16893,10 +16890,10 @@
     </row>
     <row r="739" customHeight="1" spans="1:5">
       <c r="A739" s="2" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="B739" s="2" t="s">
-        <v>1286</v>
+        <v>613</v>
       </c>
       <c r="C739" s="2" t="s">
         <v>553</v>
@@ -16910,7 +16907,7 @@
         <v>1287</v>
       </c>
       <c r="B740" s="2" t="s">
-        <v>613</v>
+        <v>1266</v>
       </c>
       <c r="C740" s="2" t="s">
         <v>553</v>
@@ -16920,30 +16917,30 @@
       </c>
     </row>
     <row r="741" customHeight="1" spans="1:5">
-      <c r="A741" s="2" t="s">
+      <c r="A741" s="5" t="s">
         <v>1288</v>
       </c>
-      <c r="B741" s="2" t="s">
-        <v>1267</v>
-      </c>
-      <c r="C741" s="2" t="s">
-        <v>553</v>
-      </c>
+      <c r="B741" s="5" t="s">
+        <v>1289</v>
+      </c>
+      <c r="C741" s="5" t="s">
+        <v>564</v>
+      </c>
+      <c r="D741" s="6"/>
       <c r="E741" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="742" customHeight="1" spans="1:5">
-      <c r="A742" s="5" t="s">
-        <v>1289</v>
-      </c>
-      <c r="B742" s="5" t="s">
+      <c r="A742" s="2" t="s">
         <v>1290</v>
       </c>
-      <c r="C742" s="5" t="s">
-        <v>564</v>
-      </c>
-      <c r="D742" s="6"/>
+      <c r="B742" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="C742" s="2" t="s">
+        <v>553</v>
+      </c>
       <c r="E742" s="4">
         <v>0</v>
       </c>
@@ -16953,7 +16950,7 @@
         <v>1291</v>
       </c>
       <c r="B743" s="2" t="s">
-        <v>649</v>
+        <v>1016</v>
       </c>
       <c r="C743" s="2" t="s">
         <v>553</v>
@@ -16967,7 +16964,7 @@
         <v>1292</v>
       </c>
       <c r="B744" s="2" t="s">
-        <v>1016</v>
+        <v>1228</v>
       </c>
       <c r="C744" s="2" t="s">
         <v>553</v>
@@ -16981,7 +16978,7 @@
         <v>1293</v>
       </c>
       <c r="B745" s="2" t="s">
-        <v>1229</v>
+        <v>604</v>
       </c>
       <c r="C745" s="2" t="s">
         <v>553</v>
@@ -16995,7 +16992,7 @@
         <v>1294</v>
       </c>
       <c r="B746" s="2" t="s">
-        <v>604</v>
+        <v>613</v>
       </c>
       <c r="C746" s="2" t="s">
         <v>553</v>
@@ -17009,7 +17006,7 @@
         <v>1295</v>
       </c>
       <c r="B747" s="2" t="s">
-        <v>613</v>
+        <v>677</v>
       </c>
       <c r="C747" s="2" t="s">
         <v>553</v>
@@ -17023,10 +17020,10 @@
         <v>1296</v>
       </c>
       <c r="B748" s="2" t="s">
-        <v>677</v>
+        <v>1109</v>
       </c>
       <c r="C748" s="2" t="s">
-        <v>553</v>
+        <v>616</v>
       </c>
       <c r="E748" s="4">
         <v>0</v>
@@ -17037,10 +17034,10 @@
         <v>1297</v>
       </c>
       <c r="B749" s="2" t="s">
-        <v>1109</v>
+        <v>1298</v>
       </c>
       <c r="C749" s="2" t="s">
-        <v>616</v>
+        <v>553</v>
       </c>
       <c r="E749" s="4">
         <v>0</v>
@@ -17048,13 +17045,13 @@
     </row>
     <row r="750" customHeight="1" spans="1:5">
       <c r="A750" s="2" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="B750" s="2" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="C750" s="2" t="s">
-        <v>553</v>
+        <v>840</v>
       </c>
       <c r="E750" s="4">
         <v>0</v>
@@ -17062,13 +17059,13 @@
     </row>
     <row r="751" customHeight="1" spans="1:5">
       <c r="A751" s="2" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="B751" s="2" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="C751" s="2" t="s">
-        <v>840</v>
+        <v>553</v>
       </c>
       <c r="E751" s="4">
         <v>0</v>
@@ -17076,10 +17073,10 @@
     </row>
     <row r="752" customHeight="1" spans="1:5">
       <c r="A752" s="2" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="B752" s="2" t="s">
-        <v>1303</v>
+        <v>625</v>
       </c>
       <c r="C752" s="2" t="s">
         <v>553</v>
@@ -17093,7 +17090,7 @@
         <v>1304</v>
       </c>
       <c r="B753" s="2" t="s">
-        <v>625</v>
+        <v>1305</v>
       </c>
       <c r="C753" s="2" t="s">
         <v>553</v>
@@ -17104,10 +17101,10 @@
     </row>
     <row r="754" customHeight="1" spans="1:5">
       <c r="A754" s="2" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="B754" s="2" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="C754" s="2" t="s">
         <v>553</v>
@@ -17118,10 +17115,10 @@
     </row>
     <row r="755" customHeight="1" spans="1:5">
       <c r="A755" s="2" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="B755" s="2" t="s">
-        <v>1308</v>
+        <v>552</v>
       </c>
       <c r="C755" s="2" t="s">
         <v>553</v>
@@ -17135,7 +17132,7 @@
         <v>1309</v>
       </c>
       <c r="B756" s="2" t="s">
-        <v>552</v>
+        <v>578</v>
       </c>
       <c r="C756" s="2" t="s">
         <v>553</v>
@@ -17149,7 +17146,7 @@
         <v>1310</v>
       </c>
       <c r="B757" s="2" t="s">
-        <v>578</v>
+        <v>1311</v>
       </c>
       <c r="C757" s="2" t="s">
         <v>553</v>
@@ -17160,10 +17157,10 @@
     </row>
     <row r="758" customHeight="1" spans="1:5">
       <c r="A758" s="2" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="B758" s="2" t="s">
-        <v>1312</v>
+        <v>727</v>
       </c>
       <c r="C758" s="2" t="s">
         <v>553</v>
@@ -17177,7 +17174,7 @@
         <v>1313</v>
       </c>
       <c r="B759" s="2" t="s">
-        <v>727</v>
+        <v>734</v>
       </c>
       <c r="C759" s="2" t="s">
         <v>553</v>
@@ -17191,7 +17188,7 @@
         <v>1314</v>
       </c>
       <c r="B760" s="2" t="s">
-        <v>734</v>
+        <v>1315</v>
       </c>
       <c r="C760" s="2" t="s">
         <v>553</v>
@@ -17202,10 +17199,10 @@
     </row>
     <row r="761" customHeight="1" spans="1:5">
       <c r="A761" s="2" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="B761" s="2" t="s">
-        <v>1316</v>
+        <v>737</v>
       </c>
       <c r="C761" s="2" t="s">
         <v>553</v>
@@ -17219,7 +17216,7 @@
         <v>1317</v>
       </c>
       <c r="B762" s="2" t="s">
-        <v>737</v>
+        <v>620</v>
       </c>
       <c r="C762" s="2" t="s">
         <v>553</v>
@@ -17233,7 +17230,7 @@
         <v>1318</v>
       </c>
       <c r="B763" s="2" t="s">
-        <v>620</v>
+        <v>1319</v>
       </c>
       <c r="C763" s="2" t="s">
         <v>553</v>
@@ -17244,10 +17241,10 @@
     </row>
     <row r="764" customHeight="1" spans="1:5">
       <c r="A764" s="2" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="B764" s="2" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="C764" s="2" t="s">
         <v>553</v>
@@ -17258,10 +17255,10 @@
     </row>
     <row r="765" customHeight="1" spans="1:5">
       <c r="A765" s="2" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="B765" s="2" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="C765" s="2" t="s">
         <v>553</v>
@@ -17272,10 +17269,10 @@
     </row>
     <row r="766" customHeight="1" spans="1:5">
       <c r="A766" s="2" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="B766" s="2" t="s">
-        <v>1324</v>
+        <v>812</v>
       </c>
       <c r="C766" s="2" t="s">
         <v>553</v>
@@ -17289,7 +17286,7 @@
         <v>1325</v>
       </c>
       <c r="B767" s="2" t="s">
-        <v>812</v>
+        <v>595</v>
       </c>
       <c r="C767" s="2" t="s">
         <v>553</v>
@@ -17303,10 +17300,10 @@
         <v>1326</v>
       </c>
       <c r="B768" s="2" t="s">
-        <v>595</v>
+        <v>1327</v>
       </c>
       <c r="C768" s="2" t="s">
-        <v>553</v>
+        <v>616</v>
       </c>
       <c r="E768" s="4">
         <v>0</v>
@@ -17314,13 +17311,13 @@
     </row>
     <row r="769" customHeight="1" spans="1:5">
       <c r="A769" s="2" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="B769" s="2" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="C769" s="2" t="s">
-        <v>616</v>
+        <v>553</v>
       </c>
       <c r="E769" s="4">
         <v>0</v>
@@ -17328,10 +17325,10 @@
     </row>
     <row r="770" customHeight="1" spans="1:5">
       <c r="A770" s="2" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="B770" s="2" t="s">
-        <v>1330</v>
+        <v>912</v>
       </c>
       <c r="C770" s="2" t="s">
         <v>553</v>
@@ -17345,7 +17342,7 @@
         <v>1331</v>
       </c>
       <c r="B771" s="2" t="s">
-        <v>912</v>
+        <v>1274</v>
       </c>
       <c r="C771" s="2" t="s">
         <v>553</v>
@@ -17359,7 +17356,7 @@
         <v>1332</v>
       </c>
       <c r="B772" s="2" t="s">
-        <v>1275</v>
+        <v>1333</v>
       </c>
       <c r="C772" s="2" t="s">
         <v>553</v>
@@ -17370,10 +17367,10 @@
     </row>
     <row r="773" customHeight="1" spans="1:5">
       <c r="A773" s="2" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="B773" s="2" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="C773" s="2" t="s">
         <v>553</v>
@@ -17384,10 +17381,10 @@
     </row>
     <row r="774" customHeight="1" spans="1:5">
       <c r="A774" s="2" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="B774" s="2" t="s">
-        <v>1336</v>
+        <v>812</v>
       </c>
       <c r="C774" s="2" t="s">
         <v>553</v>
@@ -17401,7 +17398,7 @@
         <v>1337</v>
       </c>
       <c r="B775" s="2" t="s">
-        <v>812</v>
+        <v>755</v>
       </c>
       <c r="C775" s="2" t="s">
         <v>553</v>
@@ -17415,7 +17412,7 @@
         <v>1338</v>
       </c>
       <c r="B776" s="2" t="s">
-        <v>755</v>
+        <v>620</v>
       </c>
       <c r="C776" s="2" t="s">
         <v>553</v>
@@ -17429,7 +17426,7 @@
         <v>1339</v>
       </c>
       <c r="B777" s="2" t="s">
-        <v>620</v>
+        <v>708</v>
       </c>
       <c r="C777" s="2" t="s">
         <v>553</v>
@@ -17443,7 +17440,7 @@
         <v>1340</v>
       </c>
       <c r="B778" s="2" t="s">
-        <v>708</v>
+        <v>812</v>
       </c>
       <c r="C778" s="2" t="s">
         <v>553</v>
@@ -17453,30 +17450,30 @@
       </c>
     </row>
     <row r="779" customHeight="1" spans="1:5">
-      <c r="A779" s="2" t="s">
+      <c r="A779" s="5" t="s">
         <v>1341</v>
       </c>
-      <c r="B779" s="2" t="s">
-        <v>812</v>
-      </c>
-      <c r="C779" s="2" t="s">
-        <v>553</v>
-      </c>
+      <c r="B779" s="5" t="s">
+        <v>590</v>
+      </c>
+      <c r="C779" s="5" t="s">
+        <v>591</v>
+      </c>
+      <c r="D779" s="6"/>
       <c r="E779" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="780" customHeight="1" spans="1:5">
-      <c r="A780" s="5" t="s">
+      <c r="A780" s="2" t="s">
         <v>1342</v>
       </c>
-      <c r="B780" s="5" t="s">
+      <c r="B780" s="2" t="s">
         <v>590</v>
       </c>
-      <c r="C780" s="5" t="s">
-        <v>591</v>
-      </c>
-      <c r="D780" s="6"/>
+      <c r="C780" s="2" t="s">
+        <v>553</v>
+      </c>
       <c r="E780" s="4">
         <v>0</v>
       </c>
@@ -17486,41 +17483,41 @@
         <v>1343</v>
       </c>
       <c r="B781" s="2" t="s">
-        <v>590</v>
+        <v>1344</v>
       </c>
       <c r="C781" s="2" t="s">
         <v>553</v>
       </c>
+      <c r="D781" s="2" t="s">
+        <v>1345</v>
+      </c>
       <c r="E781" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="782" customHeight="1" spans="1:5">
-      <c r="A782" s="2" t="s">
-        <v>1344</v>
+      <c r="A782" s="1">
+        <v>1219</v>
       </c>
       <c r="B782" s="2" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="C782" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="D782" s="2" t="s">
-        <v>1346</v>
-      </c>
       <c r="E782" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="783" customHeight="1" spans="1:5">
-      <c r="A783" s="1">
-        <v>1219</v>
+      <c r="A783" s="2" t="s">
+        <v>1347</v>
       </c>
       <c r="B783" s="2" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="C783" s="2" t="s">
-        <v>553</v>
+        <v>840</v>
       </c>
       <c r="E783" s="4">
         <v>0</v>
@@ -17528,13 +17525,13 @@
     </row>
     <row r="784" customHeight="1" spans="1:5">
       <c r="A784" s="2" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="B784" s="2" t="s">
-        <v>1349</v>
+        <v>622</v>
       </c>
       <c r="C784" s="2" t="s">
-        <v>840</v>
+        <v>553</v>
       </c>
       <c r="E784" s="4">
         <v>0</v>
@@ -17545,7 +17542,7 @@
         <v>1350</v>
       </c>
       <c r="B785" s="2" t="s">
-        <v>622</v>
+        <v>955</v>
       </c>
       <c r="C785" s="2" t="s">
         <v>553</v>
@@ -17559,10 +17556,10 @@
         <v>1351</v>
       </c>
       <c r="B786" s="2" t="s">
-        <v>955</v>
+        <v>697</v>
       </c>
       <c r="C786" s="2" t="s">
-        <v>553</v>
+        <v>616</v>
       </c>
       <c r="E786" s="4">
         <v>0</v>
@@ -17573,7 +17570,7 @@
         <v>1352</v>
       </c>
       <c r="B787" s="2" t="s">
-        <v>697</v>
+        <v>706</v>
       </c>
       <c r="C787" s="2" t="s">
         <v>616</v>
@@ -17587,10 +17584,10 @@
         <v>1353</v>
       </c>
       <c r="B788" s="2" t="s">
-        <v>706</v>
+        <v>926</v>
       </c>
       <c r="C788" s="2" t="s">
-        <v>616</v>
+        <v>553</v>
       </c>
       <c r="E788" s="4">
         <v>0</v>
@@ -17601,7 +17598,7 @@
         <v>1354</v>
       </c>
       <c r="B789" s="2" t="s">
-        <v>926</v>
+        <v>1355</v>
       </c>
       <c r="C789" s="2" t="s">
         <v>553</v>
@@ -17612,10 +17609,10 @@
     </row>
     <row r="790" customHeight="1" spans="1:5">
       <c r="A790" s="2" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="B790" s="2" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="C790" s="2" t="s">
         <v>553</v>
@@ -17626,10 +17623,10 @@
     </row>
     <row r="791" customHeight="1" spans="1:5">
       <c r="A791" s="2" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="B791" s="2" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="C791" s="2" t="s">
         <v>553</v>
@@ -17640,10 +17637,10 @@
     </row>
     <row r="792" customHeight="1" spans="1:5">
       <c r="A792" s="2" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="B792" s="2" t="s">
-        <v>1360</v>
+        <v>689</v>
       </c>
       <c r="C792" s="2" t="s">
         <v>553</v>
@@ -17657,7 +17654,7 @@
         <v>1361</v>
       </c>
       <c r="B793" s="2" t="s">
-        <v>689</v>
+        <v>622</v>
       </c>
       <c r="C793" s="2" t="s">
         <v>553</v>
@@ -17668,10 +17665,10 @@
     </row>
     <row r="794" customHeight="1" spans="1:5">
       <c r="A794" s="2" t="s">
+        <v>1361</v>
+      </c>
+      <c r="B794" s="2" t="s">
         <v>1362</v>
-      </c>
-      <c r="B794" s="2" t="s">
-        <v>622</v>
       </c>
       <c r="C794" s="2" t="s">
         <v>553</v>
@@ -17682,10 +17679,10 @@
     </row>
     <row r="795" customHeight="1" spans="1:5">
       <c r="A795" s="2" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="B795" s="2" t="s">
-        <v>1363</v>
+        <v>604</v>
       </c>
       <c r="C795" s="2" t="s">
         <v>553</v>
@@ -17699,7 +17696,7 @@
         <v>1364</v>
       </c>
       <c r="B796" s="2" t="s">
-        <v>604</v>
+        <v>1365</v>
       </c>
       <c r="C796" s="2" t="s">
         <v>553</v>
@@ -17710,10 +17707,10 @@
     </row>
     <row r="797" customHeight="1" spans="1:5">
       <c r="A797" s="2" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="B797" s="2" t="s">
-        <v>1366</v>
+        <v>568</v>
       </c>
       <c r="C797" s="2" t="s">
         <v>553</v>
@@ -17727,7 +17724,7 @@
         <v>1367</v>
       </c>
       <c r="B798" s="2" t="s">
-        <v>568</v>
+        <v>1368</v>
       </c>
       <c r="C798" s="2" t="s">
         <v>553</v>
@@ -17738,10 +17735,10 @@
     </row>
     <row r="799" customHeight="1" spans="1:5">
       <c r="A799" s="2" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="B799" s="2" t="s">
-        <v>1369</v>
+        <v>595</v>
       </c>
       <c r="C799" s="2" t="s">
         <v>553</v>
@@ -17752,10 +17749,10 @@
     </row>
     <row r="800" customHeight="1" spans="1:5">
       <c r="A800" s="2" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="B800" s="2" t="s">
-        <v>595</v>
+        <v>572</v>
       </c>
       <c r="C800" s="2" t="s">
         <v>553</v>
@@ -17766,10 +17763,10 @@
     </row>
     <row r="801" customHeight="1" spans="1:5">
       <c r="A801" s="2" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="B801" s="2" t="s">
-        <v>572</v>
+        <v>590</v>
       </c>
       <c r="C801" s="2" t="s">
         <v>553</v>
@@ -17783,7 +17780,7 @@
         <v>1370</v>
       </c>
       <c r="B802" s="2" t="s">
-        <v>590</v>
+        <v>645</v>
       </c>
       <c r="C802" s="2" t="s">
         <v>553</v>
@@ -17797,7 +17794,7 @@
         <v>1371</v>
       </c>
       <c r="B803" s="2" t="s">
-        <v>645</v>
+        <v>1372</v>
       </c>
       <c r="C803" s="2" t="s">
         <v>553</v>
@@ -17808,10 +17805,10 @@
     </row>
     <row r="804" customHeight="1" spans="1:5">
       <c r="A804" s="2" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="B804" s="2" t="s">
-        <v>1373</v>
+        <v>620</v>
       </c>
       <c r="C804" s="2" t="s">
         <v>553</v>
@@ -17825,7 +17822,7 @@
         <v>1374</v>
       </c>
       <c r="B805" s="2" t="s">
-        <v>620</v>
+        <v>734</v>
       </c>
       <c r="C805" s="2" t="s">
         <v>553</v>
@@ -17839,7 +17836,7 @@
         <v>1375</v>
       </c>
       <c r="B806" s="2" t="s">
-        <v>734</v>
+        <v>1376</v>
       </c>
       <c r="C806" s="2" t="s">
         <v>553</v>
@@ -17850,10 +17847,10 @@
     </row>
     <row r="807" customHeight="1" spans="1:5">
       <c r="A807" s="2" t="s">
+        <v>1377</v>
+      </c>
+      <c r="B807" s="2" t="s">
         <v>1376</v>
-      </c>
-      <c r="B807" s="2" t="s">
-        <v>1377</v>
       </c>
       <c r="C807" s="2" t="s">
         <v>553</v>
@@ -17867,7 +17864,7 @@
         <v>1378</v>
       </c>
       <c r="B808" s="2" t="s">
-        <v>1377</v>
+        <v>1105</v>
       </c>
       <c r="C808" s="2" t="s">
         <v>553</v>
@@ -17881,7 +17878,7 @@
         <v>1379</v>
       </c>
       <c r="B809" s="2" t="s">
-        <v>1105</v>
+        <v>880</v>
       </c>
       <c r="C809" s="2" t="s">
         <v>553</v>
@@ -17895,10 +17892,10 @@
         <v>1380</v>
       </c>
       <c r="B810" s="2" t="s">
-        <v>880</v>
+        <v>719</v>
       </c>
       <c r="C810" s="2" t="s">
-        <v>553</v>
+        <v>840</v>
       </c>
       <c r="E810" s="4">
         <v>0</v>
@@ -17909,10 +17906,10 @@
         <v>1381</v>
       </c>
       <c r="B811" s="2" t="s">
-        <v>719</v>
+        <v>1382</v>
       </c>
       <c r="C811" s="2" t="s">
-        <v>840</v>
+        <v>553</v>
       </c>
       <c r="E811" s="4">
         <v>0</v>
@@ -17920,10 +17917,10 @@
     </row>
     <row r="812" customHeight="1" spans="1:5">
       <c r="A812" s="2" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="B812" s="2" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="C812" s="2" t="s">
         <v>553</v>
@@ -17934,10 +17931,10 @@
     </row>
     <row r="813" customHeight="1" spans="1:5">
       <c r="A813" s="2" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="B813" s="2" t="s">
-        <v>1385</v>
+        <v>593</v>
       </c>
       <c r="C813" s="2" t="s">
         <v>553</v>
@@ -17965,7 +17962,7 @@
         <v>1387</v>
       </c>
       <c r="B815" s="2" t="s">
-        <v>593</v>
+        <v>655</v>
       </c>
       <c r="C815" s="2" t="s">
         <v>553</v>
@@ -17979,7 +17976,7 @@
         <v>1388</v>
       </c>
       <c r="B816" s="2" t="s">
-        <v>655</v>
+        <v>1389</v>
       </c>
       <c r="C816" s="2" t="s">
         <v>553</v>
@@ -17990,10 +17987,10 @@
     </row>
     <row r="817" customHeight="1" spans="1:5">
       <c r="A817" s="2" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="B817" s="2" t="s">
-        <v>1390</v>
+        <v>645</v>
       </c>
       <c r="C817" s="2" t="s">
         <v>553</v>
@@ -18007,10 +18004,10 @@
         <v>1391</v>
       </c>
       <c r="B818" s="2" t="s">
-        <v>645</v>
+        <v>655</v>
       </c>
       <c r="C818" s="2" t="s">
-        <v>553</v>
+        <v>616</v>
       </c>
       <c r="E818" s="4">
         <v>0</v>
@@ -18021,10 +18018,10 @@
         <v>1392</v>
       </c>
       <c r="B819" s="2" t="s">
-        <v>655</v>
+        <v>557</v>
       </c>
       <c r="C819" s="2" t="s">
-        <v>616</v>
+        <v>553</v>
       </c>
       <c r="E819" s="4">
         <v>0</v>
@@ -18035,7 +18032,7 @@
         <v>1393</v>
       </c>
       <c r="B820" s="2" t="s">
-        <v>557</v>
+        <v>835</v>
       </c>
       <c r="C820" s="2" t="s">
         <v>553</v>
@@ -18049,7 +18046,7 @@
         <v>1394</v>
       </c>
       <c r="B821" s="2" t="s">
-        <v>835</v>
+        <v>1016</v>
       </c>
       <c r="C821" s="2" t="s">
         <v>553</v>
@@ -18063,7 +18060,7 @@
         <v>1395</v>
       </c>
       <c r="B822" s="2" t="s">
-        <v>1016</v>
+        <v>645</v>
       </c>
       <c r="C822" s="2" t="s">
         <v>553</v>
@@ -18077,10 +18074,10 @@
         <v>1396</v>
       </c>
       <c r="B823" s="2" t="s">
-        <v>645</v>
+        <v>1397</v>
       </c>
       <c r="C823" s="2" t="s">
-        <v>553</v>
+        <v>810</v>
       </c>
       <c r="E823" s="4">
         <v>0</v>
@@ -18088,13 +18085,13 @@
     </row>
     <row r="824" customHeight="1" spans="1:5">
       <c r="A824" s="2" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="B824" s="2" t="s">
-        <v>1398</v>
+        <v>826</v>
       </c>
       <c r="C824" s="2" t="s">
-        <v>810</v>
+        <v>553</v>
       </c>
       <c r="E824" s="4">
         <v>0</v>
@@ -18105,7 +18102,7 @@
         <v>1399</v>
       </c>
       <c r="B825" s="2" t="s">
-        <v>826</v>
+        <v>557</v>
       </c>
       <c r="C825" s="2" t="s">
         <v>553</v>
@@ -18119,7 +18116,7 @@
         <v>1400</v>
       </c>
       <c r="B826" s="2" t="s">
-        <v>557</v>
+        <v>647</v>
       </c>
       <c r="C826" s="2" t="s">
         <v>553</v>
@@ -18133,10 +18130,10 @@
         <v>1401</v>
       </c>
       <c r="B827" s="2" t="s">
-        <v>647</v>
+        <v>797</v>
       </c>
       <c r="C827" s="2" t="s">
-        <v>553</v>
+        <v>616</v>
       </c>
       <c r="E827" s="4">
         <v>0</v>
@@ -18147,10 +18144,10 @@
         <v>1402</v>
       </c>
       <c r="B828" s="2" t="s">
-        <v>797</v>
+        <v>645</v>
       </c>
       <c r="C828" s="2" t="s">
-        <v>616</v>
+        <v>553</v>
       </c>
       <c r="E828" s="4">
         <v>0</v>
@@ -18161,10 +18158,10 @@
         <v>1403</v>
       </c>
       <c r="B829" s="2" t="s">
-        <v>645</v>
+        <v>950</v>
       </c>
       <c r="C829" s="2" t="s">
-        <v>553</v>
+        <v>810</v>
       </c>
       <c r="E829" s="4">
         <v>0</v>
@@ -18175,10 +18172,10 @@
         <v>1404</v>
       </c>
       <c r="B830" s="2" t="s">
-        <v>950</v>
+        <v>1405</v>
       </c>
       <c r="C830" s="2" t="s">
-        <v>810</v>
+        <v>553</v>
       </c>
       <c r="E830" s="4">
         <v>0</v>
@@ -18186,10 +18183,10 @@
     </row>
     <row r="831" customHeight="1" spans="1:5">
       <c r="A831" s="2" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="B831" s="2" t="s">
-        <v>1406</v>
+        <v>1255</v>
       </c>
       <c r="C831" s="2" t="s">
         <v>553</v>
@@ -18203,7 +18200,7 @@
         <v>1407</v>
       </c>
       <c r="B832" s="2" t="s">
-        <v>1256</v>
+        <v>604</v>
       </c>
       <c r="C832" s="2" t="s">
         <v>553</v>
@@ -18217,7 +18214,7 @@
         <v>1408</v>
       </c>
       <c r="B833" s="2" t="s">
-        <v>604</v>
+        <v>620</v>
       </c>
       <c r="C833" s="2" t="s">
         <v>553</v>
@@ -18231,7 +18228,7 @@
         <v>1409</v>
       </c>
       <c r="B834" s="2" t="s">
-        <v>620</v>
+        <v>812</v>
       </c>
       <c r="C834" s="2" t="s">
         <v>553</v>
@@ -18245,7 +18242,7 @@
         <v>1410</v>
       </c>
       <c r="B835" s="2" t="s">
-        <v>812</v>
+        <v>967</v>
       </c>
       <c r="C835" s="2" t="s">
         <v>553</v>
@@ -18259,7 +18256,7 @@
         <v>1411</v>
       </c>
       <c r="B836" s="2" t="s">
-        <v>967</v>
+        <v>620</v>
       </c>
       <c r="C836" s="2" t="s">
         <v>553</v>
@@ -18273,7 +18270,7 @@
         <v>1412</v>
       </c>
       <c r="B837" s="2" t="s">
-        <v>620</v>
+        <v>804</v>
       </c>
       <c r="C837" s="2" t="s">
         <v>553</v>
@@ -18287,7 +18284,7 @@
         <v>1413</v>
       </c>
       <c r="B838" s="2" t="s">
-        <v>804</v>
+        <v>1010</v>
       </c>
       <c r="C838" s="2" t="s">
         <v>553</v>
@@ -18301,10 +18298,10 @@
         <v>1414</v>
       </c>
       <c r="B839" s="2" t="s">
-        <v>1010</v>
+        <v>787</v>
       </c>
       <c r="C839" s="2" t="s">
-        <v>553</v>
+        <v>788</v>
       </c>
       <c r="E839" s="4">
         <v>0</v>
@@ -18315,10 +18312,10 @@
         <v>1415</v>
       </c>
       <c r="B840" s="2" t="s">
-        <v>787</v>
+        <v>755</v>
       </c>
       <c r="C840" s="2" t="s">
-        <v>788</v>
+        <v>553</v>
       </c>
       <c r="E840" s="4">
         <v>0</v>
@@ -18329,7 +18326,7 @@
         <v>1416</v>
       </c>
       <c r="B841" s="2" t="s">
-        <v>755</v>
+        <v>713</v>
       </c>
       <c r="C841" s="2" t="s">
         <v>553</v>
@@ -18343,7 +18340,7 @@
         <v>1417</v>
       </c>
       <c r="B842" s="2" t="s">
-        <v>713</v>
+        <v>590</v>
       </c>
       <c r="C842" s="2" t="s">
         <v>553</v>
@@ -18357,7 +18354,7 @@
         <v>1418</v>
       </c>
       <c r="B843" s="2" t="s">
-        <v>590</v>
+        <v>568</v>
       </c>
       <c r="C843" s="2" t="s">
         <v>553</v>
@@ -18371,7 +18368,7 @@
         <v>1419</v>
       </c>
       <c r="B844" s="2" t="s">
-        <v>568</v>
+        <v>732</v>
       </c>
       <c r="C844" s="2" t="s">
         <v>553</v>
@@ -18385,7 +18382,7 @@
         <v>1420</v>
       </c>
       <c r="B845" s="2" t="s">
-        <v>732</v>
+        <v>657</v>
       </c>
       <c r="C845" s="2" t="s">
         <v>553</v>
@@ -18399,7 +18396,7 @@
         <v>1421</v>
       </c>
       <c r="B846" s="2" t="s">
-        <v>657</v>
+        <v>734</v>
       </c>
       <c r="C846" s="2" t="s">
         <v>553</v>
@@ -18413,10 +18410,10 @@
         <v>1422</v>
       </c>
       <c r="B847" s="2" t="s">
-        <v>734</v>
+        <v>1423</v>
       </c>
       <c r="C847" s="2" t="s">
-        <v>553</v>
+        <v>840</v>
       </c>
       <c r="E847" s="4">
         <v>0</v>
@@ -18424,13 +18421,13 @@
     </row>
     <row r="848" customHeight="1" spans="1:5">
       <c r="A848" s="2" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="B848" s="2" t="s">
-        <v>1424</v>
+        <v>950</v>
       </c>
       <c r="C848" s="2" t="s">
-        <v>840</v>
+        <v>810</v>
       </c>
       <c r="E848" s="4">
         <v>0</v>
@@ -18441,10 +18438,10 @@
         <v>1425</v>
       </c>
       <c r="B849" s="2" t="s">
-        <v>950</v>
+        <v>938</v>
       </c>
       <c r="C849" s="2" t="s">
-        <v>810</v>
+        <v>553</v>
       </c>
       <c r="E849" s="4">
         <v>0</v>
@@ -18455,7 +18452,7 @@
         <v>1426</v>
       </c>
       <c r="B850" s="2" t="s">
-        <v>938</v>
+        <v>722</v>
       </c>
       <c r="C850" s="2" t="s">
         <v>553</v>
@@ -18469,7 +18466,7 @@
         <v>1427</v>
       </c>
       <c r="B851" s="2" t="s">
-        <v>722</v>
+        <v>880</v>
       </c>
       <c r="C851" s="2" t="s">
         <v>553</v>
@@ -18483,7 +18480,7 @@
         <v>1428</v>
       </c>
       <c r="B852" s="2" t="s">
-        <v>880</v>
+        <v>1274</v>
       </c>
       <c r="C852" s="2" t="s">
         <v>553</v>
@@ -18497,7 +18494,7 @@
         <v>1429</v>
       </c>
       <c r="B853" s="2" t="s">
-        <v>1275</v>
+        <v>590</v>
       </c>
       <c r="C853" s="2" t="s">
         <v>553</v>
@@ -18511,7 +18508,7 @@
         <v>1430</v>
       </c>
       <c r="B854" s="2" t="s">
-        <v>590</v>
+        <v>677</v>
       </c>
       <c r="C854" s="2" t="s">
         <v>553</v>
@@ -18525,7 +18522,7 @@
         <v>1431</v>
       </c>
       <c r="B855" s="2" t="s">
-        <v>677</v>
+        <v>647</v>
       </c>
       <c r="C855" s="2" t="s">
         <v>553</v>
@@ -18539,7 +18536,7 @@
         <v>1432</v>
       </c>
       <c r="B856" s="2" t="s">
-        <v>647</v>
+        <v>782</v>
       </c>
       <c r="C856" s="2" t="s">
         <v>553</v>
@@ -18553,7 +18550,7 @@
         <v>1433</v>
       </c>
       <c r="B857" s="2" t="s">
-        <v>782</v>
+        <v>604</v>
       </c>
       <c r="C857" s="2" t="s">
         <v>553</v>
@@ -18567,7 +18564,7 @@
         <v>1434</v>
       </c>
       <c r="B858" s="2" t="s">
-        <v>604</v>
+        <v>1435</v>
       </c>
       <c r="C858" s="2" t="s">
         <v>553</v>
@@ -18578,10 +18575,10 @@
     </row>
     <row r="859" customHeight="1" spans="1:5">
       <c r="A859" s="2" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="B859" s="2" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="C859" s="2" t="s">
         <v>553</v>
@@ -18592,10 +18589,10 @@
     </row>
     <row r="860" customHeight="1" spans="1:5">
       <c r="A860" s="2" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="B860" s="2" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="C860" s="2" t="s">
         <v>553</v>
@@ -18606,10 +18603,10 @@
     </row>
     <row r="861" customHeight="1" spans="1:5">
       <c r="A861" s="2" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="B861" s="2" t="s">
-        <v>1440</v>
+        <v>677</v>
       </c>
       <c r="C861" s="2" t="s">
         <v>553</v>
@@ -18623,10 +18620,10 @@
         <v>1441</v>
       </c>
       <c r="B862" s="2" t="s">
-        <v>677</v>
+        <v>1442</v>
       </c>
       <c r="C862" s="2" t="s">
-        <v>553</v>
+        <v>616</v>
       </c>
       <c r="E862" s="4">
         <v>0</v>
@@ -18634,41 +18631,42 @@
     </row>
     <row r="863" customHeight="1" spans="1:5">
       <c r="A863" s="2" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="B863" s="2" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="C863" s="2" t="s">
-        <v>616</v>
+        <v>810</v>
       </c>
       <c r="E863" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="864" customHeight="1" spans="1:5">
-      <c r="A864" s="2" t="s">
-        <v>1444</v>
-      </c>
-      <c r="B864" s="2" t="s">
+      <c r="A864" s="5" t="s">
         <v>1445</v>
       </c>
-      <c r="C864" s="2" t="s">
-        <v>810</v>
-      </c>
+      <c r="B864" s="5" t="s">
+        <v>1446</v>
+      </c>
+      <c r="C864" s="5" t="s">
+        <v>560</v>
+      </c>
+      <c r="D864" s="6"/>
       <c r="E864" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="865" customHeight="1" spans="1:5">
       <c r="A865" s="5" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="B865" s="5" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="C865" s="5" t="s">
-        <v>560</v>
+        <v>564</v>
       </c>
       <c r="D865" s="6"/>
       <c r="E865" s="4">
@@ -18676,26 +18674,25 @@
       </c>
     </row>
     <row r="866" customHeight="1" spans="1:5">
-      <c r="A866" s="5" t="s">
-        <v>1448</v>
-      </c>
-      <c r="B866" s="5" t="s">
+      <c r="A866" s="1" t="s">
         <v>1449</v>
       </c>
-      <c r="C866" s="5" t="s">
-        <v>564</v>
-      </c>
-      <c r="D866" s="6"/>
+      <c r="B866" s="2" t="s">
+        <v>1450</v>
+      </c>
+      <c r="C866" s="2" t="s">
+        <v>553</v>
+      </c>
       <c r="E866" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="867" customHeight="1" spans="1:5">
-      <c r="A867" s="1" t="s">
-        <v>1450</v>
+      <c r="A867" s="2" t="s">
+        <v>1451</v>
       </c>
       <c r="B867" s="2" t="s">
-        <v>1451</v>
+        <v>732</v>
       </c>
       <c r="C867" s="2" t="s">
         <v>553</v>
@@ -18709,7 +18706,7 @@
         <v>1452</v>
       </c>
       <c r="B868" s="2" t="s">
-        <v>732</v>
+        <v>557</v>
       </c>
       <c r="C868" s="2" t="s">
         <v>553</v>
@@ -18723,7 +18720,7 @@
         <v>1453</v>
       </c>
       <c r="B869" s="2" t="s">
-        <v>557</v>
+        <v>732</v>
       </c>
       <c r="C869" s="2" t="s">
         <v>553</v>
@@ -18737,13 +18734,13 @@
         <v>1454</v>
       </c>
       <c r="B870" s="2" t="s">
-        <v>732</v>
+        <v>677</v>
       </c>
       <c r="C870" s="2" t="s">
         <v>553</v>
       </c>
       <c r="E870" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="871" customHeight="1" spans="1:5">
@@ -18751,13 +18748,13 @@
         <v>1455</v>
       </c>
       <c r="B871" s="2" t="s">
-        <v>677</v>
+        <v>1111</v>
       </c>
       <c r="C871" s="2" t="s">
         <v>553</v>
       </c>
       <c r="E871" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="872" customHeight="1" spans="1:5">
@@ -18765,7 +18762,7 @@
         <v>1456</v>
       </c>
       <c r="B872" s="2" t="s">
-        <v>1111</v>
+        <v>1457</v>
       </c>
       <c r="C872" s="2" t="s">
         <v>553</v>
@@ -18776,10 +18773,10 @@
     </row>
     <row r="873" customHeight="1" spans="1:5">
       <c r="A873" s="2" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="B873" s="2" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="C873" s="2" t="s">
         <v>553</v>
@@ -18790,10 +18787,10 @@
     </row>
     <row r="874" customHeight="1" spans="1:5">
       <c r="A874" s="2" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="B874" s="2" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="C874" s="2" t="s">
         <v>553</v>
@@ -18804,10 +18801,10 @@
     </row>
     <row r="875" customHeight="1" spans="1:5">
       <c r="A875" s="2" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="B875" s="2" t="s">
-        <v>1462</v>
+        <v>1255</v>
       </c>
       <c r="C875" s="2" t="s">
         <v>553</v>
@@ -18821,7 +18818,7 @@
         <v>1463</v>
       </c>
       <c r="B876" s="2" t="s">
-        <v>1256</v>
+        <v>1302</v>
       </c>
       <c r="C876" s="2" t="s">
         <v>553</v>
@@ -18835,7 +18832,7 @@
         <v>1464</v>
       </c>
       <c r="B877" s="2" t="s">
-        <v>1303</v>
+        <v>1465</v>
       </c>
       <c r="C877" s="2" t="s">
         <v>553</v>
@@ -18846,10 +18843,10 @@
     </row>
     <row r="878" customHeight="1" spans="1:5">
       <c r="A878" s="2" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="B878" s="2" t="s">
-        <v>1466</v>
+        <v>604</v>
       </c>
       <c r="C878" s="2" t="s">
         <v>553</v>
@@ -18863,7 +18860,7 @@
         <v>1467</v>
       </c>
       <c r="B879" s="2" t="s">
-        <v>604</v>
+        <v>552</v>
       </c>
       <c r="C879" s="2" t="s">
         <v>553</v>
@@ -18877,7 +18874,7 @@
         <v>1468</v>
       </c>
       <c r="B880" s="2" t="s">
-        <v>552</v>
+        <v>682</v>
       </c>
       <c r="C880" s="2" t="s">
         <v>553</v>
@@ -18891,10 +18888,10 @@
         <v>1469</v>
       </c>
       <c r="B881" s="2" t="s">
-        <v>682</v>
+        <v>706</v>
       </c>
       <c r="C881" s="2" t="s">
-        <v>553</v>
+        <v>591</v>
       </c>
       <c r="E881" s="4">
         <v>0</v>
@@ -18905,10 +18902,10 @@
         <v>1470</v>
       </c>
       <c r="B882" s="2" t="s">
-        <v>706</v>
+        <v>1471</v>
       </c>
       <c r="C882" s="2" t="s">
-        <v>591</v>
+        <v>840</v>
       </c>
       <c r="E882" s="4">
         <v>0</v>
@@ -18916,10 +18913,10 @@
     </row>
     <row r="883" customHeight="1" spans="1:5">
       <c r="A883" s="2" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
       <c r="B883" s="2" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
       <c r="C883" s="2" t="s">
         <v>840</v>
@@ -18930,10 +18927,10 @@
     </row>
     <row r="884" customHeight="1" spans="1:5">
       <c r="A884" s="2" t="s">
+        <v>1474</v>
+      </c>
+      <c r="B884" s="2" t="s">
         <v>1473</v>
-      </c>
-      <c r="B884" s="2" t="s">
-        <v>1474</v>
       </c>
       <c r="C884" s="2" t="s">
         <v>840</v>
@@ -18947,7 +18944,7 @@
         <v>1475</v>
       </c>
       <c r="B885" s="2" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="C885" s="2" t="s">
         <v>840</v>
@@ -18961,7 +18958,7 @@
         <v>1476</v>
       </c>
       <c r="B886" s="2" t="s">
-        <v>1474</v>
+        <v>1477</v>
       </c>
       <c r="C886" s="2" t="s">
         <v>840</v>
@@ -18972,10 +18969,10 @@
     </row>
     <row r="887" customHeight="1" spans="1:5">
       <c r="A887" s="2" t="s">
+        <v>1478</v>
+      </c>
+      <c r="B887" s="2" t="s">
         <v>1477</v>
-      </c>
-      <c r="B887" s="2" t="s">
-        <v>1478</v>
       </c>
       <c r="C887" s="2" t="s">
         <v>840</v>
@@ -18989,7 +18986,7 @@
         <v>1479</v>
       </c>
       <c r="B888" s="2" t="s">
-        <v>1478</v>
+        <v>1480</v>
       </c>
       <c r="C888" s="2" t="s">
         <v>840</v>
@@ -19000,10 +18997,10 @@
     </row>
     <row r="889" customHeight="1" spans="1:5">
       <c r="A889" s="2" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="B889" s="2" t="s">
-        <v>1481</v>
+        <v>835</v>
       </c>
       <c r="C889" s="2" t="s">
         <v>840</v>
@@ -19031,7 +19028,7 @@
         <v>1483</v>
       </c>
       <c r="B891" s="2" t="s">
-        <v>835</v>
+        <v>1348</v>
       </c>
       <c r="C891" s="2" t="s">
         <v>840</v>
@@ -19045,7 +19042,7 @@
         <v>1484</v>
       </c>
       <c r="B892" s="2" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="C892" s="2" t="s">
         <v>840</v>
@@ -19059,7 +19056,7 @@
         <v>1485</v>
       </c>
       <c r="B893" s="2" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="C893" s="2" t="s">
         <v>840</v>
@@ -19073,7 +19070,7 @@
         <v>1486</v>
       </c>
       <c r="B894" s="2" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="C894" s="2" t="s">
         <v>840</v>
@@ -19087,7 +19084,7 @@
         <v>1487</v>
       </c>
       <c r="B895" s="2" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="C895" s="2" t="s">
         <v>840</v>
@@ -19101,7 +19098,7 @@
         <v>1488</v>
       </c>
       <c r="B896" s="2" t="s">
-        <v>1349</v>
+        <v>719</v>
       </c>
       <c r="C896" s="2" t="s">
         <v>840</v>
@@ -19199,7 +19196,7 @@
         <v>1495</v>
       </c>
       <c r="B903" s="2" t="s">
-        <v>719</v>
+        <v>1496</v>
       </c>
       <c r="C903" s="2" t="s">
         <v>840</v>
@@ -19210,10 +19207,10 @@
     </row>
     <row r="904" customHeight="1" spans="1:5">
       <c r="A904" s="2" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="B904" s="2" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="C904" s="2" t="s">
         <v>840</v>
@@ -19224,10 +19221,10 @@
     </row>
     <row r="905" customHeight="1" spans="1:5">
       <c r="A905" s="2" t="s">
+        <v>1499</v>
+      </c>
+      <c r="B905" s="2" t="s">
         <v>1498</v>
-      </c>
-      <c r="B905" s="2" t="s">
-        <v>1499</v>
       </c>
       <c r="C905" s="2" t="s">
         <v>840</v>
@@ -19241,7 +19238,7 @@
         <v>1500</v>
       </c>
       <c r="B906" s="2" t="s">
-        <v>1499</v>
+        <v>1501</v>
       </c>
       <c r="C906" s="2" t="s">
         <v>840</v>
@@ -19252,10 +19249,10 @@
     </row>
     <row r="907" customHeight="1" spans="1:5">
       <c r="A907" s="2" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="B907" s="2" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="C907" s="2" t="s">
         <v>840</v>
@@ -19266,10 +19263,10 @@
     </row>
     <row r="908" customHeight="1" spans="1:5">
       <c r="A908" s="2" t="s">
+        <v>1504</v>
+      </c>
+      <c r="B908" s="2" t="s">
         <v>1503</v>
-      </c>
-      <c r="B908" s="2" t="s">
-        <v>1504</v>
       </c>
       <c r="C908" s="2" t="s">
         <v>840</v>
@@ -19283,36 +19280,36 @@
         <v>1505</v>
       </c>
       <c r="B909" s="2" t="s">
-        <v>1504</v>
+        <v>1506</v>
       </c>
       <c r="C909" s="2" t="s">
         <v>840</v>
       </c>
+      <c r="D909" s="2"/>
       <c r="E909" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="910" customHeight="1" spans="1:5">
       <c r="A910" s="2" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="B910" s="2" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="C910" s="2" t="s">
         <v>840</v>
       </c>
-      <c r="D910" s="2"/>
       <c r="E910" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="911" customHeight="1" spans="1:5">
       <c r="A911" s="2" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="B911" s="2" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="C911" s="2" t="s">
         <v>840</v>
@@ -19323,10 +19320,10 @@
     </row>
     <row r="912" customHeight="1" spans="1:5">
       <c r="A912" s="2" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="B912" s="2" t="s">
-        <v>1511</v>
+        <v>1255</v>
       </c>
       <c r="C912" s="2" t="s">
         <v>840</v>
@@ -19340,7 +19337,7 @@
         <v>1512</v>
       </c>
       <c r="B913" s="2" t="s">
-        <v>1256</v>
+        <v>1513</v>
       </c>
       <c r="C913" s="2" t="s">
         <v>840</v>
@@ -19351,10 +19348,10 @@
     </row>
     <row r="914" customHeight="1" spans="1:5">
       <c r="A914" s="2" t="s">
+        <v>1514</v>
+      </c>
+      <c r="B914" s="2" t="s">
         <v>1513</v>
-      </c>
-      <c r="B914" s="2" t="s">
-        <v>1514</v>
       </c>
       <c r="C914" s="2" t="s">
         <v>840</v>
@@ -19363,29 +19360,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="915" customHeight="1" spans="1:5">
+    <row r="915" customHeight="1" spans="1:3">
       <c r="A915" s="2" t="s">
         <v>1515</v>
       </c>
       <c r="B915" s="2" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C915" s="2" t="s">
         <v>840</v>
       </c>
-      <c r="E915" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="916" customHeight="1" spans="1:3">
+    </row>
+    <row r="916" customHeight="1" spans="1:5">
       <c r="A916" s="2" t="s">
         <v>1516</v>
       </c>
       <c r="B916" s="2" t="s">
-        <v>1514</v>
+        <v>677</v>
       </c>
       <c r="C916" s="2" t="s">
         <v>840</v>
+      </c>
+      <c r="E916" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="917" customHeight="1" spans="1:5">
@@ -19393,7 +19390,7 @@
         <v>1517</v>
       </c>
       <c r="B917" s="2" t="s">
-        <v>677</v>
+        <v>1518</v>
       </c>
       <c r="C917" s="2" t="s">
         <v>840</v>
@@ -19402,40 +19399,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="918" customHeight="1" spans="1:5">
+    <row r="918" customHeight="1" spans="1:3">
       <c r="A918" s="2" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="B918" s="2" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="C918" s="2" t="s">
         <v>840</v>
       </c>
-      <c r="E918" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="919" customHeight="1" spans="1:3">
+    </row>
+    <row r="919" customHeight="1" spans="1:5">
       <c r="A919" s="2" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="B919" s="2" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="C919" s="2" t="s">
-        <v>840</v>
+        <v>1523</v>
+      </c>
+      <c r="E919" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="920" customHeight="1" spans="1:5">
       <c r="A920" s="2" t="s">
-        <v>1522</v>
+        <v>1524</v>
       </c>
       <c r="B920" s="2" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C920" s="2" t="s">
         <v>1523</v>
-      </c>
-      <c r="C920" s="2" t="s">
-        <v>1524</v>
       </c>
       <c r="E920" s="4">
         <v>0</v>
@@ -19443,13 +19440,13 @@
     </row>
     <row r="921" customHeight="1" spans="1:5">
       <c r="A921" s="2" t="s">
+        <v>1526</v>
+      </c>
+      <c r="B921" s="2" t="s">
         <v>1525</v>
       </c>
-      <c r="B921" s="2" t="s">
-        <v>1526</v>
-      </c>
       <c r="C921" s="2" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="E921" s="4">
         <v>0</v>
@@ -19460,10 +19457,10 @@
         <v>1527</v>
       </c>
       <c r="B922" s="2" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="C922" s="2" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="E922" s="4">
         <v>0</v>
@@ -19474,10 +19471,10 @@
         <v>1528</v>
       </c>
       <c r="B923" s="2" t="s">
-        <v>1526</v>
+        <v>1529</v>
       </c>
       <c r="C923" s="2" t="s">
-        <v>1524</v>
+        <v>1098</v>
       </c>
       <c r="E923" s="4">
         <v>0</v>
@@ -19485,10 +19482,10 @@
     </row>
     <row r="924" customHeight="1" spans="1:5">
       <c r="A924" s="2" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="B924" s="2" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="C924" s="2" t="s">
         <v>1098</v>
@@ -19499,10 +19496,10 @@
     </row>
     <row r="925" customHeight="1" spans="1:5">
       <c r="A925" s="2" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="B925" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="C925" s="2" t="s">
         <v>1098</v>
@@ -19513,10 +19510,10 @@
     </row>
     <row r="926" customHeight="1" spans="1:5">
       <c r="A926" s="2" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="B926" s="2" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="C926" s="2" t="s">
         <v>1098</v>
@@ -19527,10 +19524,10 @@
     </row>
     <row r="927" customHeight="1" spans="1:5">
       <c r="A927" s="2" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="B927" s="2" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="C927" s="2" t="s">
         <v>1098</v>
@@ -19541,10 +19538,10 @@
     </row>
     <row r="928" customHeight="1" spans="1:5">
       <c r="A928" s="2" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="B928" s="2" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="C928" s="2" t="s">
         <v>1098</v>
@@ -19555,10 +19552,10 @@
     </row>
     <row r="929" customHeight="1" spans="1:5">
       <c r="A929" s="2" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="B929" s="2" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="C929" s="2" t="s">
         <v>1098</v>
@@ -19569,10 +19566,10 @@
     </row>
     <row r="930" customHeight="1" spans="1:5">
       <c r="A930" s="2" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="B930" s="2" t="s">
-        <v>1542</v>
+        <v>817</v>
       </c>
       <c r="C930" s="2" t="s">
         <v>1098</v>
@@ -19586,7 +19583,7 @@
         <v>1543</v>
       </c>
       <c r="B931" s="2" t="s">
-        <v>817</v>
+        <v>1535</v>
       </c>
       <c r="C931" s="2" t="s">
         <v>1098</v>
@@ -19600,7 +19597,7 @@
         <v>1544</v>
       </c>
       <c r="B932" s="2" t="s">
-        <v>1536</v>
+        <v>1545</v>
       </c>
       <c r="C932" s="2" t="s">
         <v>1098</v>
@@ -19611,10 +19608,10 @@
     </row>
     <row r="933" customHeight="1" spans="1:5">
       <c r="A933" s="2" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="B933" s="2" t="s">
-        <v>1546</v>
+        <v>1531</v>
       </c>
       <c r="C933" s="2" t="s">
         <v>1098</v>
@@ -19628,7 +19625,7 @@
         <v>1547</v>
       </c>
       <c r="B934" s="2" t="s">
-        <v>1532</v>
+        <v>1535</v>
       </c>
       <c r="C934" s="2" t="s">
         <v>1098</v>
@@ -19642,7 +19639,7 @@
         <v>1548</v>
       </c>
       <c r="B935" s="2" t="s">
-        <v>1536</v>
+        <v>1541</v>
       </c>
       <c r="C935" s="2" t="s">
         <v>1098</v>
@@ -19656,7 +19653,7 @@
         <v>1549</v>
       </c>
       <c r="B936" s="2" t="s">
-        <v>1542</v>
+        <v>1539</v>
       </c>
       <c r="C936" s="2" t="s">
         <v>1098</v>
@@ -19670,7 +19667,7 @@
         <v>1550</v>
       </c>
       <c r="B937" s="2" t="s">
-        <v>1540</v>
+        <v>1535</v>
       </c>
       <c r="C937" s="2" t="s">
         <v>1098</v>
@@ -19684,7 +19681,7 @@
         <v>1551</v>
       </c>
       <c r="B938" s="2" t="s">
-        <v>1536</v>
+        <v>1552</v>
       </c>
       <c r="C938" s="2" t="s">
         <v>1098</v>
@@ -19695,10 +19692,10 @@
     </row>
     <row r="939" customHeight="1" spans="1:5">
       <c r="A939" s="2" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="B939" s="2" t="s">
-        <v>1553</v>
+        <v>1535</v>
       </c>
       <c r="C939" s="2" t="s">
         <v>1098</v>
@@ -19712,7 +19709,7 @@
         <v>1554</v>
       </c>
       <c r="B940" s="2" t="s">
-        <v>1536</v>
+        <v>1555</v>
       </c>
       <c r="C940" s="2" t="s">
         <v>1098</v>
@@ -19723,10 +19720,10 @@
     </row>
     <row r="941" customHeight="1" spans="1:5">
       <c r="A941" s="2" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="B941" s="2" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="C941" s="2" t="s">
         <v>1098</v>
@@ -19737,10 +19734,10 @@
     </row>
     <row r="942" customHeight="1" spans="1:5">
       <c r="A942" s="2" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="B942" s="2" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="C942" s="2" t="s">
         <v>1098</v>
@@ -19751,10 +19748,10 @@
     </row>
     <row r="943" customHeight="1" spans="1:5">
       <c r="A943" s="2" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="B943" s="2" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="C943" s="2" t="s">
         <v>1098</v>
@@ -19765,56 +19762,56 @@
     </row>
     <row r="944" customHeight="1" spans="1:5">
       <c r="A944" s="2" t="s">
-        <v>1561</v>
-      </c>
-      <c r="B944" s="2" t="s">
         <v>1562</v>
+      </c>
+      <c r="B944" s="10" t="s">
+        <v>1563</v>
       </c>
       <c r="C944" s="2" t="s">
         <v>1098</v>
       </c>
+      <c r="D944" s="2" t="s">
+        <v>1564</v>
+      </c>
       <c r="E944" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="945" customHeight="1" spans="1:5">
       <c r="A945" s="2" t="s">
-        <v>1563</v>
+        <v>1565</v>
       </c>
       <c r="B945" s="10" t="s">
-        <v>1564</v>
+        <v>1566</v>
       </c>
       <c r="C945" s="2" t="s">
         <v>1098</v>
       </c>
-      <c r="D945" s="2" t="s">
-        <v>1565</v>
-      </c>
+      <c r="D945" s="2"/>
       <c r="E945" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="946" customHeight="1" spans="1:5">
       <c r="A946" s="2" t="s">
-        <v>1566</v>
-      </c>
-      <c r="B946" s="10" t="s">
         <v>1567</v>
+      </c>
+      <c r="B946" s="2" t="s">
+        <v>1568</v>
       </c>
       <c r="C946" s="2" t="s">
         <v>1098</v>
       </c>
-      <c r="D946" s="2"/>
       <c r="E946" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="947" customHeight="1" spans="1:5">
       <c r="A947" s="2" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="B947" s="2" t="s">
-        <v>1569</v>
+        <v>1535</v>
       </c>
       <c r="C947" s="2" t="s">
         <v>1098</v>
@@ -19828,7 +19825,7 @@
         <v>1570</v>
       </c>
       <c r="B948" s="2" t="s">
-        <v>1536</v>
+        <v>1552</v>
       </c>
       <c r="C948" s="2" t="s">
         <v>1098</v>
@@ -19842,7 +19839,7 @@
         <v>1571</v>
       </c>
       <c r="B949" s="2" t="s">
-        <v>1553</v>
+        <v>1572</v>
       </c>
       <c r="C949" s="2" t="s">
         <v>1098</v>
@@ -19853,10 +19850,10 @@
     </row>
     <row r="950" customHeight="1" spans="1:5">
       <c r="A950" s="2" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="B950" s="2" t="s">
-        <v>1573</v>
+        <v>1541</v>
       </c>
       <c r="C950" s="2" t="s">
         <v>1098</v>
@@ -19870,7 +19867,7 @@
         <v>1574</v>
       </c>
       <c r="B951" s="2" t="s">
-        <v>1542</v>
+        <v>1535</v>
       </c>
       <c r="C951" s="2" t="s">
         <v>1098</v>
@@ -19883,8 +19880,8 @@
       <c r="A952" s="2" t="s">
         <v>1575</v>
       </c>
-      <c r="B952" s="2" t="s">
-        <v>1536</v>
+      <c r="B952" s="10" t="s">
+        <v>1576</v>
       </c>
       <c r="C952" s="2" t="s">
         <v>1098</v>
@@ -19895,10 +19892,10 @@
     </row>
     <row r="953" customHeight="1" spans="1:5">
       <c r="A953" s="2" t="s">
-        <v>1576</v>
-      </c>
-      <c r="B953" s="10" t="s">
         <v>1577</v>
+      </c>
+      <c r="B953" s="2" t="s">
+        <v>1539</v>
       </c>
       <c r="C953" s="2" t="s">
         <v>1098</v>
@@ -19912,7 +19909,7 @@
         <v>1578</v>
       </c>
       <c r="B954" s="2" t="s">
-        <v>1540</v>
+        <v>1535</v>
       </c>
       <c r="C954" s="2" t="s">
         <v>1098</v>
@@ -19926,7 +19923,7 @@
         <v>1579</v>
       </c>
       <c r="B955" s="2" t="s">
-        <v>1536</v>
+        <v>1541</v>
       </c>
       <c r="C955" s="2" t="s">
         <v>1098</v>
@@ -19936,33 +19933,19 @@
       </c>
     </row>
     <row r="956" customHeight="1" spans="1:5">
-      <c r="A956" s="2" t="s">
+      <c r="A956" s="24" t="s">
         <v>1580</v>
       </c>
       <c r="B956" s="2" t="s">
-        <v>1542</v>
+        <v>1581</v>
       </c>
       <c r="C956" s="2" t="s">
-        <v>1098</v>
+        <v>1582</v>
+      </c>
+      <c r="D956" s="2" t="s">
+        <v>1583</v>
       </c>
       <c r="E956" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="957" customHeight="1" spans="1:5">
-      <c r="A957" s="24" t="s">
-        <v>1581</v>
-      </c>
-      <c r="B957" s="2" t="s">
-        <v>1582</v>
-      </c>
-      <c r="C957" s="2" t="s">
-        <v>1583</v>
-      </c>
-      <c r="D957" s="2" t="s">
-        <v>1584</v>
-      </c>
-      <c r="E957" s="4">
         <v>0</v>
       </c>
     </row>
@@ -19972,7 +19955,7 @@
     <mergeCell ref="A1:D2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="输入内容有误" error="请选择勾选或取消勾选" sqref="E14 E181 E568 E919 E2:E13 E15:E18 E19:E180 E182:E567 E569:E918 E920:E923 E924:E1048576">
+    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="输入内容有误" error="请选择勾选或取消勾选" sqref="E2:E645 E646:E1048576">
       <formula1>IF(TRUE,OR(E2=0,E2=1),"Checkbox")</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
v0.1.8 update, updated song list 20230329
</commit_message>
<xml_diff>
--- a/歌单.xlsx
+++ b/歌单.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2991" uniqueCount="1509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2991" uniqueCount="1508">
   <si>
     <t>2022年3月22日18:18:30更新</t>
   </si>
@@ -3697,10 +3697,7 @@
     <t>陈洁仪/徐佳莹</t>
   </si>
   <si>
-    <t>喜欢你（粤）</t>
-  </si>
-  <si>
-    <t>Beyond</t>
+    <t>行走的鱼</t>
   </si>
   <si>
     <t>夏天的风</t>
@@ -4586,45 +4583,45 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="39">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;"/>
     <numFmt numFmtId="6" formatCode="&quot;￥&quot;#,##0;[Red]&quot;￥&quot;\-#,##0"/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="\¥#,##0.00;[Red]\¥\-#,##0.00"/>
     <numFmt numFmtId="23" formatCode="\$#,##0_);\(\$#,##0\)"/>
-    <numFmt numFmtId="178" formatCode="#\ ??/??"/>
-    <numFmt numFmtId="179" formatCode="mmmm\-yy"/>
+    <numFmt numFmtId="5" formatCode="&quot;￥&quot;#,##0;&quot;￥&quot;\-#,##0"/>
+    <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
+    <numFmt numFmtId="178" formatCode="#\ ?/?"/>
+    <numFmt numFmtId="25" formatCode="\$#,##0.00_);\(\$#,##0.00\)"/>
+    <numFmt numFmtId="179" formatCode="[$-804]aaa"/>
+    <numFmt numFmtId="180" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="181" formatCode="h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="182" formatCode="[DBNum1][$-804]m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="8" formatCode="&quot;￥&quot;#,##0.00;[Red]&quot;￥&quot;\-#,##0.00"/>
+    <numFmt numFmtId="183" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="184" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
     <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
-    <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="25" formatCode="\$#,##0.00_);\(\$#,##0.00\)"/>
-    <numFmt numFmtId="180" formatCode="h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="181" formatCode="[$-804]aaa"/>
-    <numFmt numFmtId="8" formatCode="&quot;￥&quot;#,##0.00;[Red]&quot;￥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="182" formatCode="mmmmm\-yy"/>
-    <numFmt numFmtId="183" formatCode="m/d"/>
-    <numFmt numFmtId="5" formatCode="&quot;￥&quot;#,##0;&quot;￥&quot;\-#,##0"/>
-    <numFmt numFmtId="184" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
-    <numFmt numFmtId="185" formatCode="yy/m/d"/>
-    <numFmt numFmtId="186" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="187" formatCode="[=1]&quot;☑&quot;;[=0]&quot;☐&quot;;0;@"/>
+    <numFmt numFmtId="185" formatCode="#\ ??"/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="186" formatCode="mmmmm"/>
+    <numFmt numFmtId="187" formatCode="mmmmm\-yy"/>
     <numFmt numFmtId="188" formatCode="h:mm\ AM/PM"/>
-    <numFmt numFmtId="189" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
-    <numFmt numFmtId="190" formatCode="mmmmm"/>
-    <numFmt numFmtId="191" formatCode="#\ ?/?"/>
-    <numFmt numFmtId="192" formatCode="mm/dd/yy"/>
-    <numFmt numFmtId="193" formatCode="[$-804]aaaa"/>
-    <numFmt numFmtId="194" formatCode="[DBNum1][$-804]m&quot;月&quot;d&quot;日&quot;"/>
-    <numFmt numFmtId="195" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
-    <numFmt numFmtId="196" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="197" formatCode="#\ ??"/>
-    <numFmt numFmtId="198" formatCode="\¥#,##0;\¥\-#,##0"/>
-    <numFmt numFmtId="199" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
+    <numFmt numFmtId="189" formatCode="mmmm\-yy"/>
+    <numFmt numFmtId="190" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="191" formatCode="\¥#,##0;\¥\-#,##0"/>
+    <numFmt numFmtId="192" formatCode="yy/m/d"/>
+    <numFmt numFmtId="193" formatCode="m/d"/>
+    <numFmt numFmtId="194" formatCode="dd\-mmm\-yy"/>
+    <numFmt numFmtId="195" formatCode="[=1]&quot;☑&quot;;[=0]&quot;☐&quot;;0;@"/>
+    <numFmt numFmtId="196" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
+    <numFmt numFmtId="197" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="198" formatCode="[$-804]aaaa"/>
+    <numFmt numFmtId="199" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="200" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="201" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
+    <numFmt numFmtId="201" formatCode="#\ ??/??"/>
     <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
-    <numFmt numFmtId="202" formatCode="dd\-mmm\-yy"/>
+    <numFmt numFmtId="202" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -4691,54 +4688,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -4754,6 +4705,52 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
@@ -4762,7 +4759,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4776,16 +4788,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4800,22 +4805,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4848,13 +4845,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4866,37 +4863,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4908,25 +4911,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4938,13 +4923,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4962,7 +4947,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4974,7 +5007,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4986,43 +5019,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5091,30 +5088,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -5126,6 +5099,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5157,16 +5154,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5175,94 +5172,94 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="200" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="199" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -5271,46 +5268,46 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -5333,7 +5330,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="187" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="195" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5360,7 +5357,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="187" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="195" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5381,10 +5378,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="195" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="187" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="195" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5722,7 +5719,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D945" sqref="$A1:$XFD1048576"/>
+      <selection pane="bottomRight" activeCell="A751" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.625" defaultRowHeight="23.5" customHeight="1" outlineLevelCol="4"/>
@@ -16687,26 +16684,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="751" customHeight="1" spans="1:5">
+    <row r="751" customHeight="1" spans="1:3">
       <c r="A751" s="2" t="s">
         <v>1226</v>
       </c>
       <c r="B751" s="2" t="s">
-        <v>1227</v>
+        <v>553</v>
       </c>
       <c r="C751" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="E751" s="4">
-        <v>0</v>
+        <v>484</v>
       </c>
     </row>
     <row r="752" customHeight="1" spans="1:5">
       <c r="A752" s="2" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B752" s="2" t="s">
         <v>1228</v>
-      </c>
-      <c r="B752" s="2" t="s">
-        <v>1229</v>
       </c>
       <c r="C752" s="2" t="s">
         <v>484</v>
@@ -16717,7 +16711,7 @@
     </row>
     <row r="753" customHeight="1" spans="1:5">
       <c r="A753" s="2" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="B753" s="2" t="s">
         <v>553</v>
@@ -16731,10 +16725,10 @@
     </row>
     <row r="754" customHeight="1" spans="1:5">
       <c r="A754" s="2" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B754" s="2" t="s">
         <v>1231</v>
-      </c>
-      <c r="B754" s="2" t="s">
-        <v>1232</v>
       </c>
       <c r="C754" s="2" t="s">
         <v>484</v>
@@ -16745,10 +16739,10 @@
     </row>
     <row r="755" customHeight="1" spans="1:5">
       <c r="A755" s="2" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B755" s="2" t="s">
         <v>1233</v>
-      </c>
-      <c r="B755" s="2" t="s">
-        <v>1234</v>
       </c>
       <c r="C755" s="2" t="s">
         <v>484</v>
@@ -16759,7 +16753,7 @@
     </row>
     <row r="756" customHeight="1" spans="1:5">
       <c r="A756" s="2" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="B756" s="2" t="s">
         <v>483</v>
@@ -16773,7 +16767,7 @@
     </row>
     <row r="757" customHeight="1" spans="1:5">
       <c r="A757" s="2" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="B757" s="2" t="s">
         <v>508</v>
@@ -16787,10 +16781,10 @@
     </row>
     <row r="758" customHeight="1" spans="1:5">
       <c r="A758" s="2" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B758" s="2" t="s">
         <v>1237</v>
-      </c>
-      <c r="B758" s="2" t="s">
-        <v>1238</v>
       </c>
       <c r="C758" s="2" t="s">
         <v>484</v>
@@ -16801,7 +16795,7 @@
     </row>
     <row r="759" customHeight="1" spans="1:5">
       <c r="A759" s="2" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="B759" s="2" t="s">
         <v>652</v>
@@ -16815,7 +16809,7 @@
     </row>
     <row r="760" customHeight="1" spans="1:5">
       <c r="A760" s="2" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="B760" s="2" t="s">
         <v>659</v>
@@ -16829,10 +16823,10 @@
     </row>
     <row r="761" customHeight="1" spans="1:5">
       <c r="A761" s="2" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B761" s="2" t="s">
         <v>1241</v>
-      </c>
-      <c r="B761" s="2" t="s">
-        <v>1242</v>
       </c>
       <c r="C761" s="2" t="s">
         <v>484</v>
@@ -16843,7 +16837,7 @@
     </row>
     <row r="762" customHeight="1" spans="1:5">
       <c r="A762" s="2" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="B762" s="2" t="s">
         <v>662</v>
@@ -16857,7 +16851,7 @@
     </row>
     <row r="763" customHeight="1" spans="1:5">
       <c r="A763" s="2" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="B763" s="2" t="s">
         <v>549</v>
@@ -16871,10 +16865,10 @@
     </row>
     <row r="764" customHeight="1" spans="1:5">
       <c r="A764" s="2" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B764" s="2" t="s">
         <v>1245</v>
-      </c>
-      <c r="B764" s="2" t="s">
-        <v>1246</v>
       </c>
       <c r="C764" s="2" t="s">
         <v>484</v>
@@ -16885,10 +16879,10 @@
     </row>
     <row r="765" customHeight="1" spans="1:5">
       <c r="A765" s="2" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B765" s="2" t="s">
         <v>1247</v>
-      </c>
-      <c r="B765" s="2" t="s">
-        <v>1248</v>
       </c>
       <c r="C765" s="2" t="s">
         <v>484</v>
@@ -16899,10 +16893,10 @@
     </row>
     <row r="766" customHeight="1" spans="1:5">
       <c r="A766" s="2" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B766" s="2" t="s">
         <v>1249</v>
-      </c>
-      <c r="B766" s="2" t="s">
-        <v>1250</v>
       </c>
       <c r="C766" s="2" t="s">
         <v>484</v>
@@ -16913,7 +16907,7 @@
     </row>
     <row r="767" customHeight="1" spans="1:5">
       <c r="A767" s="2" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="B767" s="2" t="s">
         <v>737</v>
@@ -16927,7 +16921,7 @@
     </row>
     <row r="768" customHeight="1" spans="1:5">
       <c r="A768" s="2" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="B768" s="2" t="s">
         <v>525</v>
@@ -16941,10 +16935,10 @@
     </row>
     <row r="769" customHeight="1" spans="1:5">
       <c r="A769" s="2" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B769" s="2" t="s">
         <v>1253</v>
-      </c>
-      <c r="B769" s="2" t="s">
-        <v>1254</v>
       </c>
       <c r="C769" s="2" t="s">
         <v>545</v>
@@ -16955,10 +16949,10 @@
     </row>
     <row r="770" customHeight="1" spans="1:5">
       <c r="A770" s="2" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B770" s="2" t="s">
         <v>1255</v>
-      </c>
-      <c r="B770" s="2" t="s">
-        <v>1256</v>
       </c>
       <c r="C770" s="2" t="s">
         <v>484</v>
@@ -16969,7 +16963,7 @@
     </row>
     <row r="771" customHeight="1" spans="1:5">
       <c r="A771" s="2" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="B771" s="2" t="s">
         <v>839</v>
@@ -16983,7 +16977,7 @@
     </row>
     <row r="772" customHeight="1" spans="1:5">
       <c r="A772" s="2" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="B772" s="2" t="s">
         <v>1201</v>
@@ -16997,10 +16991,10 @@
     </row>
     <row r="773" customHeight="1" spans="1:5">
       <c r="A773" s="2" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B773" s="2" t="s">
         <v>1259</v>
-      </c>
-      <c r="B773" s="2" t="s">
-        <v>1260</v>
       </c>
       <c r="C773" s="2" t="s">
         <v>484</v>
@@ -17011,10 +17005,10 @@
     </row>
     <row r="774" customHeight="1" spans="1:5">
       <c r="A774" s="2" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B774" s="2" t="s">
         <v>1261</v>
-      </c>
-      <c r="B774" s="2" t="s">
-        <v>1262</v>
       </c>
       <c r="C774" s="2" t="s">
         <v>484</v>
@@ -17025,7 +17019,7 @@
     </row>
     <row r="775" customHeight="1" spans="1:5">
       <c r="A775" s="2" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="B775" s="2" t="s">
         <v>737</v>
@@ -17039,7 +17033,7 @@
     </row>
     <row r="776" customHeight="1" spans="1:5">
       <c r="A776" s="2" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="B776" s="2" t="s">
         <v>680</v>
@@ -17053,7 +17047,7 @@
     </row>
     <row r="777" customHeight="1" spans="1:5">
       <c r="A777" s="2" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="B777" s="2" t="s">
         <v>549</v>
@@ -17067,7 +17061,7 @@
     </row>
     <row r="778" customHeight="1" spans="1:5">
       <c r="A778" s="2" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="B778" s="2" t="s">
         <v>633</v>
@@ -17081,7 +17075,7 @@
     </row>
     <row r="779" customHeight="1" spans="1:5">
       <c r="A779" s="2" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="B779" s="2" t="s">
         <v>737</v>
@@ -17095,7 +17089,7 @@
     </row>
     <row r="780" customHeight="1" spans="1:5">
       <c r="A780" s="5" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="B780" s="5" t="s">
         <v>520</v>
@@ -17110,7 +17104,7 @@
     </row>
     <row r="781" customHeight="1" spans="1:5">
       <c r="A781" s="2" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="B781" s="2" t="s">
         <v>520</v>
@@ -17124,10 +17118,10 @@
     </row>
     <row r="782" customHeight="1" spans="1:5">
       <c r="A782" s="2" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B782" s="2" t="s">
         <v>1270</v>
-      </c>
-      <c r="B782" s="2" t="s">
-        <v>1271</v>
       </c>
       <c r="C782" s="2" t="s">
         <v>484</v>
@@ -17142,7 +17136,7 @@
         <v>1219</v>
       </c>
       <c r="B783" s="2" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="C783" s="2" t="s">
         <v>484</v>
@@ -17153,10 +17147,10 @@
     </row>
     <row r="784" customHeight="1" spans="1:5">
       <c r="A784" s="2" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B784" s="2" t="s">
         <v>1273</v>
-      </c>
-      <c r="B784" s="2" t="s">
-        <v>1274</v>
       </c>
       <c r="C784" s="2" t="s">
         <v>765</v>
@@ -17167,7 +17161,7 @@
     </row>
     <row r="785" customHeight="1" spans="1:5">
       <c r="A785" s="2" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="B785" s="2" t="s">
         <v>551</v>
@@ -17181,7 +17175,7 @@
     </row>
     <row r="786" customHeight="1" spans="1:5">
       <c r="A786" s="2" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="B786" s="2" t="s">
         <v>882</v>
@@ -17195,7 +17189,7 @@
     </row>
     <row r="787" customHeight="1" spans="1:5">
       <c r="A787" s="2" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="B787" s="2" t="s">
         <v>622</v>
@@ -17209,7 +17203,7 @@
     </row>
     <row r="788" customHeight="1" spans="1:5">
       <c r="A788" s="2" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="B788" s="2" t="s">
         <v>631</v>
@@ -17223,7 +17217,7 @@
     </row>
     <row r="789" customHeight="1" spans="1:5">
       <c r="A789" s="2" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="B789" s="2" t="s">
         <v>853</v>
@@ -17237,10 +17231,10 @@
     </row>
     <row r="790" customHeight="1" spans="1:5">
       <c r="A790" s="2" t="s">
+        <v>1279</v>
+      </c>
+      <c r="B790" s="2" t="s">
         <v>1280</v>
-      </c>
-      <c r="B790" s="2" t="s">
-        <v>1281</v>
       </c>
       <c r="C790" s="2" t="s">
         <v>484</v>
@@ -17251,10 +17245,10 @@
     </row>
     <row r="791" customHeight="1" spans="1:5">
       <c r="A791" s="2" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B791" s="2" t="s">
         <v>1282</v>
-      </c>
-      <c r="B791" s="2" t="s">
-        <v>1283</v>
       </c>
       <c r="C791" s="2" t="s">
         <v>484</v>
@@ -17265,10 +17259,10 @@
     </row>
     <row r="792" customHeight="1" spans="1:5">
       <c r="A792" s="2" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B792" s="2" t="s">
         <v>1284</v>
-      </c>
-      <c r="B792" s="2" t="s">
-        <v>1285</v>
       </c>
       <c r="C792" s="2" t="s">
         <v>484</v>
@@ -17279,7 +17273,7 @@
     </row>
     <row r="793" customHeight="1" spans="1:5">
       <c r="A793" s="2" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="B793" s="2" t="s">
         <v>614</v>
@@ -17293,7 +17287,7 @@
     </row>
     <row r="794" customHeight="1" spans="1:5">
       <c r="A794" s="2" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="B794" s="2" t="s">
         <v>551</v>
@@ -17307,10 +17301,10 @@
     </row>
     <row r="795" customHeight="1" spans="1:5">
       <c r="A795" s="2" t="s">
+        <v>1286</v>
+      </c>
+      <c r="B795" s="2" t="s">
         <v>1287</v>
-      </c>
-      <c r="B795" s="2" t="s">
-        <v>1288</v>
       </c>
       <c r="C795" s="2" t="s">
         <v>484</v>
@@ -17321,7 +17315,7 @@
     </row>
     <row r="796" customHeight="1" spans="1:5">
       <c r="A796" s="2" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="B796" s="2" t="s">
         <v>534</v>
@@ -17335,10 +17329,10 @@
     </row>
     <row r="797" customHeight="1" spans="1:5">
       <c r="A797" s="2" t="s">
+        <v>1289</v>
+      </c>
+      <c r="B797" s="2" t="s">
         <v>1290</v>
-      </c>
-      <c r="B797" s="2" t="s">
-        <v>1291</v>
       </c>
       <c r="C797" s="2" t="s">
         <v>484</v>
@@ -17349,7 +17343,7 @@
     </row>
     <row r="798" customHeight="1" spans="1:5">
       <c r="A798" s="2" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="B798" s="2" t="s">
         <v>498</v>
@@ -17363,10 +17357,10 @@
     </row>
     <row r="799" customHeight="1" spans="1:5">
       <c r="A799" s="2" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B799" s="2" t="s">
         <v>1293</v>
-      </c>
-      <c r="B799" s="2" t="s">
-        <v>1294</v>
       </c>
       <c r="C799" s="2" t="s">
         <v>484</v>
@@ -17377,7 +17371,7 @@
     </row>
     <row r="800" customHeight="1" spans="1:5">
       <c r="A800" s="2" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="B800" s="2" t="s">
         <v>525</v>
@@ -17391,7 +17385,7 @@
     </row>
     <row r="801" customHeight="1" spans="1:5">
       <c r="A801" s="2" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="B801" s="2" t="s">
         <v>502</v>
@@ -17405,7 +17399,7 @@
     </row>
     <row r="802" customHeight="1" spans="1:5">
       <c r="A802" s="2" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="B802" s="2" t="s">
         <v>520</v>
@@ -17419,7 +17413,7 @@
     </row>
     <row r="803" customHeight="1" spans="1:5">
       <c r="A803" s="2" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="B803" s="2" t="s">
         <v>570</v>
@@ -17433,10 +17427,10 @@
     </row>
     <row r="804" customHeight="1" spans="1:5">
       <c r="A804" s="2" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B804" s="2" t="s">
         <v>1297</v>
-      </c>
-      <c r="B804" s="2" t="s">
-        <v>1298</v>
       </c>
       <c r="C804" s="2" t="s">
         <v>484</v>
@@ -17447,7 +17441,7 @@
     </row>
     <row r="805" customHeight="1" spans="1:5">
       <c r="A805" s="2" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="B805" s="2" t="s">
         <v>549</v>
@@ -17461,7 +17455,7 @@
     </row>
     <row r="806" customHeight="1" spans="1:5">
       <c r="A806" s="2" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="B806" s="2" t="s">
         <v>659</v>
@@ -17475,10 +17469,10 @@
     </row>
     <row r="807" customHeight="1" spans="1:5">
       <c r="A807" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B807" s="2" t="s">
         <v>1301</v>
-      </c>
-      <c r="B807" s="2" t="s">
-        <v>1302</v>
       </c>
       <c r="C807" s="2" t="s">
         <v>484</v>
@@ -17489,10 +17483,10 @@
     </row>
     <row r="808" customHeight="1" spans="1:5">
       <c r="A808" s="2" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="B808" s="2" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="C808" s="2" t="s">
         <v>484</v>
@@ -17503,7 +17497,7 @@
     </row>
     <row r="809" customHeight="1" spans="1:5">
       <c r="A809" s="2" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="B809" s="2" t="s">
         <v>1032</v>
@@ -17517,7 +17511,7 @@
     </row>
     <row r="810" customHeight="1" spans="1:5">
       <c r="A810" s="2" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="B810" s="2" t="s">
         <v>805</v>
@@ -17531,7 +17525,7 @@
     </row>
     <row r="811" customHeight="1" spans="1:5">
       <c r="A811" s="2" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="B811" s="2" t="s">
         <v>644</v>
@@ -17545,10 +17539,10 @@
     </row>
     <row r="812" customHeight="1" spans="1:5">
       <c r="A812" s="2" t="s">
+        <v>1306</v>
+      </c>
+      <c r="B812" s="2" t="s">
         <v>1307</v>
-      </c>
-      <c r="B812" s="2" t="s">
-        <v>1308</v>
       </c>
       <c r="C812" s="2" t="s">
         <v>484</v>
@@ -17559,10 +17553,10 @@
     </row>
     <row r="813" customHeight="1" spans="1:5">
       <c r="A813" s="2" t="s">
+        <v>1308</v>
+      </c>
+      <c r="B813" s="2" t="s">
         <v>1309</v>
-      </c>
-      <c r="B813" s="2" t="s">
-        <v>1310</v>
       </c>
       <c r="C813" s="2" t="s">
         <v>484</v>
@@ -17573,7 +17567,7 @@
     </row>
     <row r="814" customHeight="1" spans="1:5">
       <c r="A814" s="2" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="B814" s="2" t="s">
         <v>523</v>
@@ -17587,7 +17581,7 @@
     </row>
     <row r="815" customHeight="1" spans="1:5">
       <c r="A815" s="2" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="B815" s="2" t="s">
         <v>523</v>
@@ -17601,7 +17595,7 @@
     </row>
     <row r="816" customHeight="1" spans="1:5">
       <c r="A816" s="2" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="B816" s="2" t="s">
         <v>580</v>
@@ -17615,10 +17609,10 @@
     </row>
     <row r="817" customHeight="1" spans="1:5">
       <c r="A817" s="2" t="s">
+        <v>1313</v>
+      </c>
+      <c r="B817" s="2" t="s">
         <v>1314</v>
-      </c>
-      <c r="B817" s="2" t="s">
-        <v>1315</v>
       </c>
       <c r="C817" s="2" t="s">
         <v>484</v>
@@ -17629,7 +17623,7 @@
     </row>
     <row r="818" customHeight="1" spans="1:5">
       <c r="A818" s="2" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="B818" s="2" t="s">
         <v>570</v>
@@ -17643,7 +17637,7 @@
     </row>
     <row r="819" customHeight="1" spans="1:5">
       <c r="A819" s="2" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="B819" s="2" t="s">
         <v>580</v>
@@ -17657,7 +17651,7 @@
     </row>
     <row r="820" customHeight="1" spans="1:5">
       <c r="A820" s="2" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="B820" s="2" t="s">
         <v>488</v>
@@ -17671,7 +17665,7 @@
     </row>
     <row r="821" customHeight="1" spans="1:5">
       <c r="A821" s="2" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="B821" s="2" t="s">
         <v>760</v>
@@ -17685,7 +17679,7 @@
     </row>
     <row r="822" customHeight="1" spans="1:5">
       <c r="A822" s="2" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="B822" s="2" t="s">
         <v>943</v>
@@ -17699,7 +17693,7 @@
     </row>
     <row r="823" customHeight="1" spans="1:5">
       <c r="A823" s="2" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="B823" s="2" t="s">
         <v>570</v>
@@ -17713,10 +17707,10 @@
     </row>
     <row r="824" customHeight="1" spans="1:5">
       <c r="A824" s="2" t="s">
+        <v>1321</v>
+      </c>
+      <c r="B824" s="2" t="s">
         <v>1322</v>
-      </c>
-      <c r="B824" s="2" t="s">
-        <v>1323</v>
       </c>
       <c r="C824" s="2" t="s">
         <v>735</v>
@@ -17727,7 +17721,7 @@
     </row>
     <row r="825" customHeight="1" spans="1:5">
       <c r="A825" s="2" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="B825" s="2" t="s">
         <v>751</v>
@@ -17741,7 +17735,7 @@
     </row>
     <row r="826" customHeight="1" spans="1:5">
       <c r="A826" s="2" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="B826" s="2" t="s">
         <v>488</v>
@@ -17755,7 +17749,7 @@
     </row>
     <row r="827" customHeight="1" spans="1:5">
       <c r="A827" s="2" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="B827" s="2" t="s">
         <v>572</v>
@@ -17769,7 +17763,7 @@
     </row>
     <row r="828" customHeight="1" spans="1:5">
       <c r="A828" s="2" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="B828" s="2" t="s">
         <v>722</v>
@@ -17783,7 +17777,7 @@
     </row>
     <row r="829" customHeight="1" spans="1:5">
       <c r="A829" s="2" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="B829" s="2" t="s">
         <v>570</v>
@@ -17797,7 +17791,7 @@
     </row>
     <row r="830" customHeight="1" spans="1:5">
       <c r="A830" s="2" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="B830" s="2" t="s">
         <v>877</v>
@@ -17811,10 +17805,10 @@
     </row>
     <row r="831" customHeight="1" spans="1:5">
       <c r="A831" s="2" t="s">
+        <v>1329</v>
+      </c>
+      <c r="B831" s="2" t="s">
         <v>1330</v>
-      </c>
-      <c r="B831" s="2" t="s">
-        <v>1331</v>
       </c>
       <c r="C831" s="2" t="s">
         <v>484</v>
@@ -17825,7 +17819,7 @@
     </row>
     <row r="832" customHeight="1" spans="1:5">
       <c r="A832" s="2" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="B832" s="2" t="s">
         <v>1182</v>
@@ -17839,7 +17833,7 @@
     </row>
     <row r="833" customHeight="1" spans="1:5">
       <c r="A833" s="2" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="B833" s="2" t="s">
         <v>534</v>
@@ -17853,7 +17847,7 @@
     </row>
     <row r="834" customHeight="1" spans="1:5">
       <c r="A834" s="2" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="B834" s="2" t="s">
         <v>549</v>
@@ -17867,7 +17861,7 @@
     </row>
     <row r="835" customHeight="1" spans="1:5">
       <c r="A835" s="2" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="B835" s="2" t="s">
         <v>737</v>
@@ -17881,7 +17875,7 @@
     </row>
     <row r="836" customHeight="1" spans="1:5">
       <c r="A836" s="2" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="B836" s="2" t="s">
         <v>894</v>
@@ -17895,7 +17889,7 @@
     </row>
     <row r="837" customHeight="1" spans="1:5">
       <c r="A837" s="2" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="B837" s="2" t="s">
         <v>549</v>
@@ -17909,7 +17903,7 @@
     </row>
     <row r="838" customHeight="1" spans="1:5">
       <c r="A838" s="2" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="B838" s="2" t="s">
         <v>729</v>
@@ -17923,7 +17917,7 @@
     </row>
     <row r="839" customHeight="1" spans="1:5">
       <c r="A839" s="2" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="B839" s="2" t="s">
         <v>937</v>
@@ -17937,7 +17931,7 @@
     </row>
     <row r="840" customHeight="1" spans="1:5">
       <c r="A840" s="2" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="B840" s="2" t="s">
         <v>712</v>
@@ -17951,7 +17945,7 @@
     </row>
     <row r="841" customHeight="1" spans="1:5">
       <c r="A841" s="2" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="B841" s="2" t="s">
         <v>680</v>
@@ -17965,7 +17959,7 @@
     </row>
     <row r="842" customHeight="1" spans="1:5">
       <c r="A842" s="2" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="B842" s="2" t="s">
         <v>638</v>
@@ -17979,7 +17973,7 @@
     </row>
     <row r="843" customHeight="1" spans="1:5">
       <c r="A843" s="2" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="B843" s="2" t="s">
         <v>520</v>
@@ -17993,7 +17987,7 @@
     </row>
     <row r="844" customHeight="1" spans="1:5">
       <c r="A844" s="2" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="B844" s="2" t="s">
         <v>498</v>
@@ -18007,7 +18001,7 @@
     </row>
     <row r="845" customHeight="1" spans="1:5">
       <c r="A845" s="2" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="B845" s="2" t="s">
         <v>657</v>
@@ -18021,7 +18015,7 @@
     </row>
     <row r="846" customHeight="1" spans="1:5">
       <c r="A846" s="2" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="B846" s="2" t="s">
         <v>582</v>
@@ -18035,7 +18029,7 @@
     </row>
     <row r="847" customHeight="1" spans="1:5">
       <c r="A847" s="2" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="B847" s="2" t="s">
         <v>659</v>
@@ -18049,10 +18043,10 @@
     </row>
     <row r="848" customHeight="1" spans="1:5">
       <c r="A848" s="2" t="s">
+        <v>1347</v>
+      </c>
+      <c r="B848" s="2" t="s">
         <v>1348</v>
-      </c>
-      <c r="B848" s="2" t="s">
-        <v>1349</v>
       </c>
       <c r="C848" s="2" t="s">
         <v>765</v>
@@ -18063,7 +18057,7 @@
     </row>
     <row r="849" customHeight="1" spans="1:5">
       <c r="A849" s="2" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="B849" s="2" t="s">
         <v>877</v>
@@ -18077,7 +18071,7 @@
     </row>
     <row r="850" customHeight="1" spans="1:5">
       <c r="A850" s="2" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="B850" s="2" t="s">
         <v>865</v>
@@ -18091,7 +18085,7 @@
     </row>
     <row r="851" customHeight="1" spans="1:5">
       <c r="A851" s="2" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="B851" s="2" t="s">
         <v>647</v>
@@ -18105,7 +18099,7 @@
     </row>
     <row r="852" customHeight="1" spans="1:5">
       <c r="A852" s="2" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="B852" s="2" t="s">
         <v>805</v>
@@ -18119,7 +18113,7 @@
     </row>
     <row r="853" customHeight="1" spans="1:5">
       <c r="A853" s="2" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="B853" s="2" t="s">
         <v>1201</v>
@@ -18133,7 +18127,7 @@
     </row>
     <row r="854" customHeight="1" spans="1:5">
       <c r="A854" s="2" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="B854" s="2" t="s">
         <v>520</v>
@@ -18147,7 +18141,7 @@
     </row>
     <row r="855" customHeight="1" spans="1:5">
       <c r="A855" s="2" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="B855" s="2" t="s">
         <v>602</v>
@@ -18161,7 +18155,7 @@
     </row>
     <row r="856" customHeight="1" spans="1:5">
       <c r="A856" s="2" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="B856" s="2" t="s">
         <v>572</v>
@@ -18175,7 +18169,7 @@
     </row>
     <row r="857" customHeight="1" spans="1:5">
       <c r="A857" s="2" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="B857" s="2" t="s">
         <v>707</v>
@@ -18189,7 +18183,7 @@
     </row>
     <row r="858" customHeight="1" spans="1:5">
       <c r="A858" s="2" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="B858" s="2" t="s">
         <v>534</v>
@@ -18203,10 +18197,10 @@
     </row>
     <row r="859" customHeight="1" spans="1:5">
       <c r="A859" s="2" t="s">
+        <v>1359</v>
+      </c>
+      <c r="B859" s="2" t="s">
         <v>1360</v>
-      </c>
-      <c r="B859" s="2" t="s">
-        <v>1361</v>
       </c>
       <c r="C859" s="2" t="s">
         <v>484</v>
@@ -18217,10 +18211,10 @@
     </row>
     <row r="860" customHeight="1" spans="1:5">
       <c r="A860" s="2" t="s">
+        <v>1361</v>
+      </c>
+      <c r="B860" s="2" t="s">
         <v>1362</v>
-      </c>
-      <c r="B860" s="2" t="s">
-        <v>1363</v>
       </c>
       <c r="C860" s="2" t="s">
         <v>484</v>
@@ -18231,10 +18225,10 @@
     </row>
     <row r="861" customHeight="1" spans="1:5">
       <c r="A861" s="2" t="s">
+        <v>1363</v>
+      </c>
+      <c r="B861" s="2" t="s">
         <v>1364</v>
-      </c>
-      <c r="B861" s="2" t="s">
-        <v>1365</v>
       </c>
       <c r="C861" s="2" t="s">
         <v>484</v>
@@ -18245,7 +18239,7 @@
     </row>
     <row r="862" customHeight="1" spans="1:5">
       <c r="A862" s="2" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="B862" s="2" t="s">
         <v>602</v>
@@ -18259,10 +18253,10 @@
     </row>
     <row r="863" customHeight="1" spans="1:5">
       <c r="A863" s="2" t="s">
+        <v>1366</v>
+      </c>
+      <c r="B863" s="2" t="s">
         <v>1367</v>
-      </c>
-      <c r="B863" s="2" t="s">
-        <v>1368</v>
       </c>
       <c r="C863" s="2" t="s">
         <v>545</v>
@@ -18273,10 +18267,10 @@
     </row>
     <row r="864" customHeight="1" spans="1:5">
       <c r="A864" s="2" t="s">
+        <v>1368</v>
+      </c>
+      <c r="B864" s="2" t="s">
         <v>1369</v>
-      </c>
-      <c r="B864" s="2" t="s">
-        <v>1370</v>
       </c>
       <c r="C864" s="2" t="s">
         <v>735</v>
@@ -18287,10 +18281,10 @@
     </row>
     <row r="865" customHeight="1" spans="1:5">
       <c r="A865" s="5" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B865" s="5" t="s">
         <v>1371</v>
-      </c>
-      <c r="B865" s="5" t="s">
-        <v>1372</v>
       </c>
       <c r="C865" s="5" t="s">
         <v>491</v>
@@ -18302,10 +18296,10 @@
     </row>
     <row r="866" customHeight="1" spans="1:5">
       <c r="A866" s="5" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B866" s="5" t="s">
         <v>1373</v>
-      </c>
-      <c r="B866" s="5" t="s">
-        <v>1374</v>
       </c>
       <c r="C866" s="5" t="s">
         <v>494</v>
@@ -18317,10 +18311,10 @@
     </row>
     <row r="867" customHeight="1" spans="1:5">
       <c r="A867" s="1" t="s">
+        <v>1374</v>
+      </c>
+      <c r="B867" s="2" t="s">
         <v>1375</v>
-      </c>
-      <c r="B867" s="2" t="s">
-        <v>1376</v>
       </c>
       <c r="C867" s="2" t="s">
         <v>484</v>
@@ -18331,7 +18325,7 @@
     </row>
     <row r="868" customHeight="1" spans="1:5">
       <c r="A868" s="2" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="B868" s="2" t="s">
         <v>657</v>
@@ -18345,7 +18339,7 @@
     </row>
     <row r="869" customHeight="1" spans="1:5">
       <c r="A869" s="2" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="B869" s="2" t="s">
         <v>488</v>
@@ -18359,7 +18353,7 @@
     </row>
     <row r="870" customHeight="1" spans="1:5">
       <c r="A870" s="2" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="B870" s="2" t="s">
         <v>657</v>
@@ -18373,7 +18367,7 @@
     </row>
     <row r="871" customHeight="1" spans="1:5">
       <c r="A871" s="2" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="B871" s="2" t="s">
         <v>602</v>
@@ -18387,7 +18381,7 @@
     </row>
     <row r="872" customHeight="1" spans="1:5">
       <c r="A872" s="2" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="B872" s="2" t="s">
         <v>1038</v>
@@ -18401,10 +18395,10 @@
     </row>
     <row r="873" customHeight="1" spans="1:5">
       <c r="A873" s="2" t="s">
+        <v>1381</v>
+      </c>
+      <c r="B873" s="2" t="s">
         <v>1382</v>
-      </c>
-      <c r="B873" s="2" t="s">
-        <v>1383</v>
       </c>
       <c r="C873" s="2" t="s">
         <v>484</v>
@@ -18415,10 +18409,10 @@
     </row>
     <row r="874" customHeight="1" spans="1:5">
       <c r="A874" s="2" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B874" s="2" t="s">
         <v>1384</v>
-      </c>
-      <c r="B874" s="2" t="s">
-        <v>1385</v>
       </c>
       <c r="C874" s="2" t="s">
         <v>484</v>
@@ -18429,10 +18423,10 @@
     </row>
     <row r="875" customHeight="1" spans="1:5">
       <c r="A875" s="2" t="s">
+        <v>1385</v>
+      </c>
+      <c r="B875" s="2" t="s">
         <v>1386</v>
-      </c>
-      <c r="B875" s="2" t="s">
-        <v>1387</v>
       </c>
       <c r="C875" s="2" t="s">
         <v>484</v>
@@ -18443,7 +18437,7 @@
     </row>
     <row r="876" customHeight="1" spans="1:5">
       <c r="A876" s="2" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="B876" s="2" t="s">
         <v>1182</v>
@@ -18457,10 +18451,10 @@
     </row>
     <row r="877" customHeight="1" spans="1:5">
       <c r="A877" s="2" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="B877" s="2" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="C877" s="2" t="s">
         <v>484</v>
@@ -18471,10 +18465,10 @@
     </row>
     <row r="878" customHeight="1" spans="1:5">
       <c r="A878" s="2" t="s">
+        <v>1389</v>
+      </c>
+      <c r="B878" s="2" t="s">
         <v>1390</v>
-      </c>
-      <c r="B878" s="2" t="s">
-        <v>1391</v>
       </c>
       <c r="C878" s="2" t="s">
         <v>484</v>
@@ -18485,7 +18479,7 @@
     </row>
     <row r="879" customHeight="1" spans="1:5">
       <c r="A879" s="2" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="B879" s="2" t="s">
         <v>534</v>
@@ -18499,7 +18493,7 @@
     </row>
     <row r="880" customHeight="1" spans="1:5">
       <c r="A880" s="2" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="B880" s="2" t="s">
         <v>483</v>
@@ -18513,7 +18507,7 @@
     </row>
     <row r="881" customHeight="1" spans="1:5">
       <c r="A881" s="2" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="B881" s="2" t="s">
         <v>607</v>
@@ -18527,7 +18521,7 @@
     </row>
     <row r="882" customHeight="1" spans="1:5">
       <c r="A882" s="2" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="B882" s="2" t="s">
         <v>631</v>
@@ -18541,10 +18535,10 @@
     </row>
     <row r="883" customHeight="1" spans="1:5">
       <c r="A883" s="2" t="s">
+        <v>1395</v>
+      </c>
+      <c r="B883" s="2" t="s">
         <v>1396</v>
-      </c>
-      <c r="B883" s="2" t="s">
-        <v>1397</v>
       </c>
       <c r="C883" s="2" t="s">
         <v>765</v>
@@ -18555,10 +18549,10 @@
     </row>
     <row r="884" customHeight="1" spans="1:5">
       <c r="A884" s="2" t="s">
+        <v>1397</v>
+      </c>
+      <c r="B884" s="2" t="s">
         <v>1398</v>
-      </c>
-      <c r="B884" s="2" t="s">
-        <v>1399</v>
       </c>
       <c r="C884" s="2" t="s">
         <v>765</v>
@@ -18569,10 +18563,10 @@
     </row>
     <row r="885" customHeight="1" spans="1:5">
       <c r="A885" s="2" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="B885" s="2" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="C885" s="2" t="s">
         <v>765</v>
@@ -18583,10 +18577,10 @@
     </row>
     <row r="886" customHeight="1" spans="1:5">
       <c r="A886" s="2" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="B886" s="2" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="C886" s="2" t="s">
         <v>765</v>
@@ -18597,10 +18591,10 @@
     </row>
     <row r="887" customHeight="1" spans="1:5">
       <c r="A887" s="2" t="s">
+        <v>1401</v>
+      </c>
+      <c r="B887" s="2" t="s">
         <v>1402</v>
-      </c>
-      <c r="B887" s="2" t="s">
-        <v>1403</v>
       </c>
       <c r="C887" s="2" t="s">
         <v>765</v>
@@ -18611,10 +18605,10 @@
     </row>
     <row r="888" customHeight="1" spans="1:5">
       <c r="A888" s="2" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="B888" s="2" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="C888" s="2" t="s">
         <v>765</v>
@@ -18625,10 +18619,10 @@
     </row>
     <row r="889" customHeight="1" spans="1:5">
       <c r="A889" s="2" t="s">
+        <v>1404</v>
+      </c>
+      <c r="B889" s="2" t="s">
         <v>1405</v>
-      </c>
-      <c r="B889" s="2" t="s">
-        <v>1406</v>
       </c>
       <c r="C889" s="2" t="s">
         <v>765</v>
@@ -18639,7 +18633,7 @@
     </row>
     <row r="890" customHeight="1" spans="1:5">
       <c r="A890" s="2" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="B890" s="2" t="s">
         <v>760</v>
@@ -18653,7 +18647,7 @@
     </row>
     <row r="891" customHeight="1" spans="1:5">
       <c r="A891" s="2" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="B891" s="2" t="s">
         <v>760</v>
@@ -18667,10 +18661,10 @@
     </row>
     <row r="892" customHeight="1" spans="1:5">
       <c r="A892" s="2" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="B892" s="2" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="C892" s="2" t="s">
         <v>765</v>
@@ -18681,10 +18675,10 @@
     </row>
     <row r="893" customHeight="1" spans="1:5">
       <c r="A893" s="2" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="B893" s="2" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="C893" s="2" t="s">
         <v>765</v>
@@ -18695,10 +18689,10 @@
     </row>
     <row r="894" customHeight="1" spans="1:5">
       <c r="A894" s="2" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="B894" s="2" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="C894" s="2" t="s">
         <v>765</v>
@@ -18709,10 +18703,10 @@
     </row>
     <row r="895" customHeight="1" spans="1:5">
       <c r="A895" s="2" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="B895" s="2" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="C895" s="2" t="s">
         <v>765</v>
@@ -18723,10 +18717,10 @@
     </row>
     <row r="896" customHeight="1" spans="1:5">
       <c r="A896" s="2" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="B896" s="2" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="C896" s="2" t="s">
         <v>765</v>
@@ -18737,7 +18731,7 @@
     </row>
     <row r="897" customHeight="1" spans="1:5">
       <c r="A897" s="2" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="B897" s="2" t="s">
         <v>644</v>
@@ -18751,7 +18745,7 @@
     </row>
     <row r="898" customHeight="1" spans="1:5">
       <c r="A898" s="2" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="B898" s="2" t="s">
         <v>644</v>
@@ -18765,7 +18759,7 @@
     </row>
     <row r="899" customHeight="1" spans="1:5">
       <c r="A899" s="2" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="B899" s="2" t="s">
         <v>644</v>
@@ -18779,7 +18773,7 @@
     </row>
     <row r="900" customHeight="1" spans="1:5">
       <c r="A900" s="2" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="B900" s="2" t="s">
         <v>644</v>
@@ -18793,7 +18787,7 @@
     </row>
     <row r="901" customHeight="1" spans="1:5">
       <c r="A901" s="2" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="B901" s="2" t="s">
         <v>644</v>
@@ -18807,7 +18801,7 @@
     </row>
     <row r="902" customHeight="1" spans="1:5">
       <c r="A902" s="2" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="B902" s="2" t="s">
         <v>644</v>
@@ -18821,7 +18815,7 @@
     </row>
     <row r="903" customHeight="1" spans="1:5">
       <c r="A903" s="2" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="B903" s="2" t="s">
         <v>644</v>
@@ -18835,10 +18829,10 @@
     </row>
     <row r="904" customHeight="1" spans="1:5">
       <c r="A904" s="2" t="s">
+        <v>1420</v>
+      </c>
+      <c r="B904" s="2" t="s">
         <v>1421</v>
-      </c>
-      <c r="B904" s="2" t="s">
-        <v>1422</v>
       </c>
       <c r="C904" s="2" t="s">
         <v>765</v>
@@ -18849,10 +18843,10 @@
     </row>
     <row r="905" customHeight="1" spans="1:5">
       <c r="A905" s="2" t="s">
+        <v>1422</v>
+      </c>
+      <c r="B905" s="2" t="s">
         <v>1423</v>
-      </c>
-      <c r="B905" s="2" t="s">
-        <v>1424</v>
       </c>
       <c r="C905" s="2" t="s">
         <v>765</v>
@@ -18863,10 +18857,10 @@
     </row>
     <row r="906" customHeight="1" spans="1:5">
       <c r="A906" s="2" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="B906" s="2" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="C906" s="2" t="s">
         <v>765</v>
@@ -18877,10 +18871,10 @@
     </row>
     <row r="907" customHeight="1" spans="1:5">
       <c r="A907" s="2" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B907" s="2" t="s">
         <v>1426</v>
-      </c>
-      <c r="B907" s="2" t="s">
-        <v>1427</v>
       </c>
       <c r="C907" s="2" t="s">
         <v>765</v>
@@ -18891,10 +18885,10 @@
     </row>
     <row r="908" customHeight="1" spans="1:5">
       <c r="A908" s="2" t="s">
+        <v>1427</v>
+      </c>
+      <c r="B908" s="2" t="s">
         <v>1428</v>
-      </c>
-      <c r="B908" s="2" t="s">
-        <v>1429</v>
       </c>
       <c r="C908" s="2" t="s">
         <v>765</v>
@@ -18905,10 +18899,10 @@
     </row>
     <row r="909" customHeight="1" spans="1:5">
       <c r="A909" s="2" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="B909" s="2" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="C909" s="2" t="s">
         <v>765</v>
@@ -18919,10 +18913,10 @@
     </row>
     <row r="910" customHeight="1" spans="1:5">
       <c r="A910" s="2" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B910" s="2" t="s">
         <v>1431</v>
-      </c>
-      <c r="B910" s="2" t="s">
-        <v>1432</v>
       </c>
       <c r="C910" s="2" t="s">
         <v>765</v>
@@ -18934,10 +18928,10 @@
     </row>
     <row r="911" customHeight="1" spans="1:5">
       <c r="A911" s="2" t="s">
+        <v>1432</v>
+      </c>
+      <c r="B911" s="2" t="s">
         <v>1433</v>
-      </c>
-      <c r="B911" s="2" t="s">
-        <v>1434</v>
       </c>
       <c r="C911" s="2" t="s">
         <v>765</v>
@@ -18948,10 +18942,10 @@
     </row>
     <row r="912" customHeight="1" spans="1:5">
       <c r="A912" s="2" t="s">
+        <v>1434</v>
+      </c>
+      <c r="B912" s="2" t="s">
         <v>1435</v>
-      </c>
-      <c r="B912" s="2" t="s">
-        <v>1436</v>
       </c>
       <c r="C912" s="2" t="s">
         <v>765</v>
@@ -18962,7 +18956,7 @@
     </row>
     <row r="913" customHeight="1" spans="1:5">
       <c r="A913" s="2" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="B913" s="2" t="s">
         <v>1182</v>
@@ -18976,10 +18970,10 @@
     </row>
     <row r="914" customHeight="1" spans="1:5">
       <c r="A914" s="2" t="s">
+        <v>1437</v>
+      </c>
+      <c r="B914" s="2" t="s">
         <v>1438</v>
-      </c>
-      <c r="B914" s="2" t="s">
-        <v>1439</v>
       </c>
       <c r="C914" s="2" t="s">
         <v>765</v>
@@ -18990,10 +18984,10 @@
     </row>
     <row r="915" customHeight="1" spans="1:5">
       <c r="A915" s="2" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="B915" s="2" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="C915" s="2" t="s">
         <v>765</v>
@@ -19004,10 +18998,10 @@
     </row>
     <row r="916" customHeight="1" spans="1:3">
       <c r="A916" s="2" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="B916" s="2" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="C916" s="2" t="s">
         <v>765</v>
@@ -19015,7 +19009,7 @@
     </row>
     <row r="917" customHeight="1" spans="1:5">
       <c r="A917" s="2" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="B917" s="2" t="s">
         <v>602</v>
@@ -19029,10 +19023,10 @@
     </row>
     <row r="918" customHeight="1" spans="1:5">
       <c r="A918" s="2" t="s">
+        <v>1442</v>
+      </c>
+      <c r="B918" s="2" t="s">
         <v>1443</v>
-      </c>
-      <c r="B918" s="2" t="s">
-        <v>1444</v>
       </c>
       <c r="C918" s="2" t="s">
         <v>765</v>
@@ -19043,10 +19037,10 @@
     </row>
     <row r="919" customHeight="1" spans="1:3">
       <c r="A919" s="2" t="s">
+        <v>1444</v>
+      </c>
+      <c r="B919" s="2" t="s">
         <v>1445</v>
-      </c>
-      <c r="B919" s="2" t="s">
-        <v>1446</v>
       </c>
       <c r="C919" s="2" t="s">
         <v>765</v>
@@ -19054,13 +19048,13 @@
     </row>
     <row r="920" customHeight="1" spans="1:5">
       <c r="A920" s="2" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B920" s="2" t="s">
         <v>1447</v>
       </c>
-      <c r="B920" s="2" t="s">
+      <c r="C920" s="2" t="s">
         <v>1448</v>
-      </c>
-      <c r="C920" s="2" t="s">
-        <v>1449</v>
       </c>
       <c r="E920" s="4">
         <v>0</v>
@@ -19068,13 +19062,13 @@
     </row>
     <row r="921" customHeight="1" spans="1:5">
       <c r="A921" s="2" t="s">
+        <v>1449</v>
+      </c>
+      <c r="B921" s="2" t="s">
         <v>1450</v>
       </c>
-      <c r="B921" s="2" t="s">
-        <v>1451</v>
-      </c>
       <c r="C921" s="2" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="E921" s="4">
         <v>0</v>
@@ -19082,13 +19076,13 @@
     </row>
     <row r="922" customHeight="1" spans="1:5">
       <c r="A922" s="2" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="B922" s="2" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="C922" s="2" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="E922" s="4">
         <v>0</v>
@@ -19096,13 +19090,13 @@
     </row>
     <row r="923" customHeight="1" spans="1:5">
       <c r="A923" s="2" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="B923" s="2" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="C923" s="2" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="E923" s="4">
         <v>0</v>
@@ -19110,10 +19104,10 @@
     </row>
     <row r="924" customHeight="1" spans="1:5">
       <c r="A924" s="2" t="s">
+        <v>1453</v>
+      </c>
+      <c r="B924" s="2" t="s">
         <v>1454</v>
-      </c>
-      <c r="B924" s="2" t="s">
-        <v>1455</v>
       </c>
       <c r="C924" s="2" t="s">
         <v>1025</v>
@@ -19124,10 +19118,10 @@
     </row>
     <row r="925" customHeight="1" spans="1:5">
       <c r="A925" s="2" t="s">
+        <v>1455</v>
+      </c>
+      <c r="B925" s="2" t="s">
         <v>1456</v>
-      </c>
-      <c r="B925" s="2" t="s">
-        <v>1457</v>
       </c>
       <c r="C925" s="2" t="s">
         <v>1025</v>
@@ -19138,10 +19132,10 @@
     </row>
     <row r="926" customHeight="1" spans="1:5">
       <c r="A926" s="2" t="s">
+        <v>1457</v>
+      </c>
+      <c r="B926" s="2" t="s">
         <v>1458</v>
-      </c>
-      <c r="B926" s="2" t="s">
-        <v>1459</v>
       </c>
       <c r="C926" s="2" t="s">
         <v>1025</v>
@@ -19152,10 +19146,10 @@
     </row>
     <row r="927" customHeight="1" spans="1:5">
       <c r="A927" s="2" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B927" s="2" t="s">
         <v>1460</v>
-      </c>
-      <c r="B927" s="2" t="s">
-        <v>1461</v>
       </c>
       <c r="C927" s="2" t="s">
         <v>1025</v>
@@ -19166,10 +19160,10 @@
     </row>
     <row r="928" customHeight="1" spans="1:5">
       <c r="A928" s="2" t="s">
+        <v>1461</v>
+      </c>
+      <c r="B928" s="2" t="s">
         <v>1462</v>
-      </c>
-      <c r="B928" s="2" t="s">
-        <v>1463</v>
       </c>
       <c r="C928" s="2" t="s">
         <v>1025</v>
@@ -19180,10 +19174,10 @@
     </row>
     <row r="929" customHeight="1" spans="1:5">
       <c r="A929" s="2" t="s">
+        <v>1463</v>
+      </c>
+      <c r="B929" s="2" t="s">
         <v>1464</v>
-      </c>
-      <c r="B929" s="2" t="s">
-        <v>1465</v>
       </c>
       <c r="C929" s="2" t="s">
         <v>1025</v>
@@ -19194,10 +19188,10 @@
     </row>
     <row r="930" customHeight="1" spans="1:5">
       <c r="A930" s="2" t="s">
+        <v>1465</v>
+      </c>
+      <c r="B930" s="2" t="s">
         <v>1466</v>
-      </c>
-      <c r="B930" s="2" t="s">
-        <v>1467</v>
       </c>
       <c r="C930" s="2" t="s">
         <v>1025</v>
@@ -19208,7 +19202,7 @@
     </row>
     <row r="931" customHeight="1" spans="1:5">
       <c r="A931" s="2" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="B931" s="2" t="s">
         <v>742</v>
@@ -19222,10 +19216,10 @@
     </row>
     <row r="932" customHeight="1" spans="1:5">
       <c r="A932" s="2" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="B932" s="2" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="C932" s="2" t="s">
         <v>1025</v>
@@ -19236,10 +19230,10 @@
     </row>
     <row r="933" customHeight="1" spans="1:5">
       <c r="A933" s="2" t="s">
+        <v>1469</v>
+      </c>
+      <c r="B933" s="2" t="s">
         <v>1470</v>
-      </c>
-      <c r="B933" s="2" t="s">
-        <v>1471</v>
       </c>
       <c r="C933" s="2" t="s">
         <v>1025</v>
@@ -19250,10 +19244,10 @@
     </row>
     <row r="934" customHeight="1" spans="1:5">
       <c r="A934" s="2" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
       <c r="B934" s="2" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="C934" s="2" t="s">
         <v>1025</v>
@@ -19264,10 +19258,10 @@
     </row>
     <row r="935" customHeight="1" spans="1:5">
       <c r="A935" s="2" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="B935" s="2" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="C935" s="2" t="s">
         <v>1025</v>
@@ -19278,10 +19272,10 @@
     </row>
     <row r="936" customHeight="1" spans="1:5">
       <c r="A936" s="2" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="B936" s="2" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="C936" s="2" t="s">
         <v>1025</v>
@@ -19292,10 +19286,10 @@
     </row>
     <row r="937" customHeight="1" spans="1:5">
       <c r="A937" s="2" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="B937" s="2" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="C937" s="2" t="s">
         <v>1025</v>
@@ -19306,10 +19300,10 @@
     </row>
     <row r="938" customHeight="1" spans="1:5">
       <c r="A938" s="2" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="B938" s="2" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="C938" s="2" t="s">
         <v>1025</v>
@@ -19320,10 +19314,10 @@
     </row>
     <row r="939" customHeight="1" spans="1:5">
       <c r="A939" s="2" t="s">
+        <v>1476</v>
+      </c>
+      <c r="B939" s="2" t="s">
         <v>1477</v>
-      </c>
-      <c r="B939" s="2" t="s">
-        <v>1478</v>
       </c>
       <c r="C939" s="2" t="s">
         <v>1025</v>
@@ -19334,10 +19328,10 @@
     </row>
     <row r="940" customHeight="1" spans="1:5">
       <c r="A940" s="2" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="B940" s="2" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="C940" s="2" t="s">
         <v>1025</v>
@@ -19348,10 +19342,10 @@
     </row>
     <row r="941" customHeight="1" spans="1:5">
       <c r="A941" s="2" t="s">
+        <v>1479</v>
+      </c>
+      <c r="B941" s="2" t="s">
         <v>1480</v>
-      </c>
-      <c r="B941" s="2" t="s">
-        <v>1481</v>
       </c>
       <c r="C941" s="2" t="s">
         <v>1025</v>
@@ -19362,10 +19356,10 @@
     </row>
     <row r="942" customHeight="1" spans="1:5">
       <c r="A942" s="2" t="s">
+        <v>1481</v>
+      </c>
+      <c r="B942" s="2" t="s">
         <v>1482</v>
-      </c>
-      <c r="B942" s="2" t="s">
-        <v>1483</v>
       </c>
       <c r="C942" s="2" t="s">
         <v>1025</v>
@@ -19376,10 +19370,10 @@
     </row>
     <row r="943" customHeight="1" spans="1:5">
       <c r="A943" s="2" t="s">
+        <v>1483</v>
+      </c>
+      <c r="B943" s="2" t="s">
         <v>1484</v>
-      </c>
-      <c r="B943" s="2" t="s">
-        <v>1485</v>
       </c>
       <c r="C943" s="2" t="s">
         <v>1025</v>
@@ -19390,10 +19384,10 @@
     </row>
     <row r="944" customHeight="1" spans="1:5">
       <c r="A944" s="2" t="s">
+        <v>1485</v>
+      </c>
+      <c r="B944" s="2" t="s">
         <v>1486</v>
-      </c>
-      <c r="B944" s="2" t="s">
-        <v>1487</v>
       </c>
       <c r="C944" s="2" t="s">
         <v>1025</v>
@@ -19404,10 +19398,10 @@
     </row>
     <row r="945" customHeight="1" spans="1:5">
       <c r="A945" s="2" t="s">
+        <v>1487</v>
+      </c>
+      <c r="B945" s="10" t="s">
         <v>1488</v>
-      </c>
-      <c r="B945" s="10" t="s">
-        <v>1489</v>
       </c>
       <c r="C945" s="2" t="s">
         <v>1025</v>
@@ -19419,10 +19413,10 @@
     </row>
     <row r="946" customHeight="1" spans="1:5">
       <c r="A946" s="2" t="s">
+        <v>1489</v>
+      </c>
+      <c r="B946" s="10" t="s">
         <v>1490</v>
-      </c>
-      <c r="B946" s="10" t="s">
-        <v>1491</v>
       </c>
       <c r="C946" s="2" t="s">
         <v>1025</v>
@@ -19434,10 +19428,10 @@
     </row>
     <row r="947" customHeight="1" spans="1:5">
       <c r="A947" s="2" t="s">
+        <v>1491</v>
+      </c>
+      <c r="B947" s="2" t="s">
         <v>1492</v>
-      </c>
-      <c r="B947" s="2" t="s">
-        <v>1493</v>
       </c>
       <c r="C947" s="2" t="s">
         <v>1025</v>
@@ -19448,10 +19442,10 @@
     </row>
     <row r="948" customHeight="1" spans="1:5">
       <c r="A948" s="2" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="B948" s="2" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="C948" s="2" t="s">
         <v>1025</v>
@@ -19462,10 +19456,10 @@
     </row>
     <row r="949" customHeight="1" spans="1:5">
       <c r="A949" s="2" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="B949" s="2" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="C949" s="2" t="s">
         <v>1025</v>
@@ -19476,10 +19470,10 @@
     </row>
     <row r="950" customHeight="1" spans="1:5">
       <c r="A950" s="2" t="s">
+        <v>1495</v>
+      </c>
+      <c r="B950" s="2" t="s">
         <v>1496</v>
-      </c>
-      <c r="B950" s="2" t="s">
-        <v>1497</v>
       </c>
       <c r="C950" s="2" t="s">
         <v>1025</v>
@@ -19490,10 +19484,10 @@
     </row>
     <row r="951" customHeight="1" spans="1:5">
       <c r="A951" s="2" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="B951" s="2" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="C951" s="2" t="s">
         <v>1025</v>
@@ -19504,10 +19498,10 @@
     </row>
     <row r="952" customHeight="1" spans="1:5">
       <c r="A952" s="2" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="B952" s="2" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="C952" s="2" t="s">
         <v>1025</v>
@@ -19518,10 +19512,10 @@
     </row>
     <row r="953" customHeight="1" spans="1:5">
       <c r="A953" s="2" t="s">
+        <v>1499</v>
+      </c>
+      <c r="B953" s="10" t="s">
         <v>1500</v>
-      </c>
-      <c r="B953" s="10" t="s">
-        <v>1501</v>
       </c>
       <c r="C953" s="2" t="s">
         <v>1025</v>
@@ -19532,10 +19526,10 @@
     </row>
     <row r="954" customHeight="1" spans="1:5">
       <c r="A954" s="2" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="B954" s="2" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="C954" s="2" t="s">
         <v>1025</v>
@@ -19546,10 +19540,10 @@
     </row>
     <row r="955" customHeight="1" spans="1:5">
       <c r="A955" s="2" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="B955" s="2" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="C955" s="2" t="s">
         <v>1025</v>
@@ -19560,10 +19554,10 @@
     </row>
     <row r="956" customHeight="1" spans="1:5">
       <c r="A956" s="2" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="B956" s="2" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="C956" s="2" t="s">
         <v>1025</v>
@@ -19574,16 +19568,16 @@
     </row>
     <row r="957" customHeight="1" spans="1:5">
       <c r="A957" s="24" t="s">
+        <v>1504</v>
+      </c>
+      <c r="B957" s="2" t="s">
         <v>1505</v>
       </c>
-      <c r="B957" s="2" t="s">
+      <c r="C957" s="2" t="s">
         <v>1506</v>
       </c>
-      <c r="C957" s="2" t="s">
+      <c r="D957" s="2" t="s">
         <v>1507</v>
-      </c>
-      <c r="D957" s="2" t="s">
-        <v>1508</v>
       </c>
       <c r="E957" s="4">
         <v>0</v>

</xml_diff>

<commit_message>
v0.2.0 updated, implemented copyright restricted songs
</commit_message>
<xml_diff>
--- a/歌单.xlsx
+++ b/歌单.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2991" uniqueCount="1508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2991" uniqueCount="1509">
   <si>
     <t>2022年3月22日18:18:30更新</t>
   </si>
@@ -1882,7 +1882,7 @@
     <t>匆匆那年</t>
   </si>
   <si>
-    <t>错位时空</t>
+    <t>×错位时空</t>
   </si>
   <si>
     <t>艾辰</t>
@@ -1903,7 +1903,7 @@
     <t>小爱的妈</t>
   </si>
   <si>
-    <t>吹梦到西洲</t>
+    <t>×吹梦到西洲</t>
   </si>
   <si>
     <t>大眠</t>
@@ -2239,7 +2239,7 @@
     <t>后弦</t>
   </si>
   <si>
-    <t>红豆</t>
+    <t>×红豆</t>
   </si>
   <si>
     <t>画心</t>
@@ -2977,7 +2977,7 @@
     <t>银临&amp;Aki阿杰</t>
   </si>
   <si>
-    <t>起风了</t>
+    <t>×起风了</t>
   </si>
   <si>
     <t>买辣椒也用券</t>
@@ -3895,10 +3895,13 @@
     <t>羽毛</t>
   </si>
   <si>
+    <t>×勇气</t>
+  </si>
+  <si>
+    <t>棉子</t>
+  </si>
+  <si>
     <t>勇气</t>
-  </si>
-  <si>
-    <t>棉子</t>
   </si>
   <si>
     <t>勇敢</t>
@@ -4583,47 +4586,47 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="39">
-    <numFmt numFmtId="176" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;"/>
     <numFmt numFmtId="6" formatCode="&quot;￥&quot;#,##0;[Red]&quot;￥&quot;\-#,##0"/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="\¥#,##0.00;[Red]\¥\-#,##0.00"/>
     <numFmt numFmtId="23" formatCode="\$#,##0_);\(\$#,##0\)"/>
+    <numFmt numFmtId="176" formatCode="#\ ??/??"/>
+    <numFmt numFmtId="177" formatCode="mmmm\-yy"/>
+    <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
+    <numFmt numFmtId="25" formatCode="\$#,##0.00_);\(\$#,##0.00\)"/>
+    <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
+    <numFmt numFmtId="178" formatCode="h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="[DBNum1][$-804]m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="180" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
+    <numFmt numFmtId="181" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="182" formatCode="h:mm\ AM/PM"/>
+    <numFmt numFmtId="183" formatCode="yy/m/d"/>
+    <numFmt numFmtId="184" formatCode="dd\-mmm\-yy"/>
+    <numFmt numFmtId="185" formatCode="mmmmm"/>
+    <numFmt numFmtId="186" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;"/>
     <numFmt numFmtId="5" formatCode="&quot;￥&quot;#,##0;&quot;￥&quot;\-#,##0"/>
+    <numFmt numFmtId="187" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
+    <numFmt numFmtId="188" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
+    <numFmt numFmtId="189" formatCode="[$-804]aaaa"/>
+    <numFmt numFmtId="190" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
+    <numFmt numFmtId="191" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="192" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="193" formatCode="#\ ?/?"/>
+    <numFmt numFmtId="194" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
+    <numFmt numFmtId="195" formatCode="[=1]&quot;☑&quot;;[=0]&quot;☐&quot;;0;@"/>
     <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="178" formatCode="#\ ?/?"/>
-    <numFmt numFmtId="25" formatCode="\$#,##0.00_);\(\$#,##0.00\)"/>
-    <numFmt numFmtId="179" formatCode="[$-804]aaa"/>
-    <numFmt numFmtId="180" formatCode="mm/dd/yy"/>
-    <numFmt numFmtId="181" formatCode="h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="182" formatCode="[DBNum1][$-804]m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="196" formatCode="\¥#,##0;\¥\-#,##0"/>
+    <numFmt numFmtId="197" formatCode="#\ ??"/>
+    <numFmt numFmtId="198" formatCode="m/d"/>
     <numFmt numFmtId="8" formatCode="&quot;￥&quot;#,##0.00;[Red]&quot;￥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="183" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="184" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
-    <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
-    <numFmt numFmtId="185" formatCode="#\ ??"/>
+    <numFmt numFmtId="199" formatCode="\¥#,##0.00;[Red]\¥\-#,##0.00"/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="186" formatCode="mmmmm"/>
-    <numFmt numFmtId="187" formatCode="mmmmm\-yy"/>
-    <numFmt numFmtId="188" formatCode="h:mm\ AM/PM"/>
-    <numFmt numFmtId="189" formatCode="mmmm\-yy"/>
-    <numFmt numFmtId="190" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
-    <numFmt numFmtId="191" formatCode="\¥#,##0;\¥\-#,##0"/>
-    <numFmt numFmtId="192" formatCode="yy/m/d"/>
-    <numFmt numFmtId="193" formatCode="m/d"/>
-    <numFmt numFmtId="194" formatCode="dd\-mmm\-yy"/>
-    <numFmt numFmtId="195" formatCode="[=1]&quot;☑&quot;;[=0]&quot;☐&quot;;0;@"/>
-    <numFmt numFmtId="196" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
-    <numFmt numFmtId="197" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="198" formatCode="[$-804]aaaa"/>
-    <numFmt numFmtId="199" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="200" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="201" formatCode="#\ ??/??"/>
-    <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
-    <numFmt numFmtId="202" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
+    <numFmt numFmtId="200" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="201" formatCode="[$-804]aaa"/>
+    <numFmt numFmtId="202" formatCode="mmmmm\-yy"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4668,6 +4671,12 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="汉仪书宋二KW"/>
@@ -4682,7 +4691,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4690,6 +4713,38 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -4705,52 +4760,6 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
@@ -4759,7 +4768,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4767,30 +4776,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4805,16 +4790,40 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -4839,7 +4848,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4851,37 +4956,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4893,133 +5028,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5079,6 +5088,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -5103,30 +5136,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -5138,17 +5147,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5167,157 +5165,168 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="200" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="192" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="199" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="191" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -5391,6 +5400,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5715,7 +5727,7 @@
   <dimension ref="A1:E957"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E751" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -10690,7 +10702,7 @@
       </c>
     </row>
     <row r="323" customHeight="1" spans="1:5">
-      <c r="A323" s="2" t="s">
+      <c r="A323" s="24" t="s">
         <v>621</v>
       </c>
       <c r="B323" s="2" t="s">
@@ -10746,7 +10758,7 @@
       </c>
     </row>
     <row r="327" customHeight="1" spans="1:5">
-      <c r="A327" s="2" t="s">
+      <c r="A327" s="24" t="s">
         <v>628</v>
       </c>
       <c r="B327" s="2" t="s">
@@ -14190,7 +14202,7 @@
       </c>
     </row>
     <row r="573" customHeight="1" spans="1:5">
-      <c r="A573" s="2" t="s">
+      <c r="A573" s="24" t="s">
         <v>986</v>
       </c>
       <c r="B573" s="2" t="s">
@@ -17356,7 +17368,7 @@
       </c>
     </row>
     <row r="799" customHeight="1" spans="1:5">
-      <c r="A799" s="2" t="s">
+      <c r="A799" s="24" t="s">
         <v>1292</v>
       </c>
       <c r="B799" s="2" t="s">
@@ -17371,7 +17383,7 @@
     </row>
     <row r="800" customHeight="1" spans="1:5">
       <c r="A800" s="2" t="s">
-        <v>1292</v>
+        <v>1294</v>
       </c>
       <c r="B800" s="2" t="s">
         <v>525</v>
@@ -17385,7 +17397,7 @@
     </row>
     <row r="801" customHeight="1" spans="1:5">
       <c r="A801" s="2" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="B801" s="2" t="s">
         <v>502</v>
@@ -17399,7 +17411,7 @@
     </row>
     <row r="802" customHeight="1" spans="1:5">
       <c r="A802" s="2" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="B802" s="2" t="s">
         <v>520</v>
@@ -17413,7 +17425,7 @@
     </row>
     <row r="803" customHeight="1" spans="1:5">
       <c r="A803" s="2" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="B803" s="2" t="s">
         <v>570</v>
@@ -17427,10 +17439,10 @@
     </row>
     <row r="804" customHeight="1" spans="1:5">
       <c r="A804" s="2" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="B804" s="2" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="C804" s="2" t="s">
         <v>484</v>
@@ -17441,7 +17453,7 @@
     </row>
     <row r="805" customHeight="1" spans="1:5">
       <c r="A805" s="2" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="B805" s="2" t="s">
         <v>549</v>
@@ -17455,7 +17467,7 @@
     </row>
     <row r="806" customHeight="1" spans="1:5">
       <c r="A806" s="2" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="B806" s="2" t="s">
         <v>659</v>
@@ -17469,10 +17481,10 @@
     </row>
     <row r="807" customHeight="1" spans="1:5">
       <c r="A807" s="2" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="B807" s="2" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="C807" s="2" t="s">
         <v>484</v>
@@ -17483,10 +17495,10 @@
     </row>
     <row r="808" customHeight="1" spans="1:5">
       <c r="A808" s="2" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B808" s="2" t="s">
         <v>1302</v>
-      </c>
-      <c r="B808" s="2" t="s">
-        <v>1301</v>
       </c>
       <c r="C808" s="2" t="s">
         <v>484</v>
@@ -17497,7 +17509,7 @@
     </row>
     <row r="809" customHeight="1" spans="1:5">
       <c r="A809" s="2" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="B809" s="2" t="s">
         <v>1032</v>
@@ -17511,7 +17523,7 @@
     </row>
     <row r="810" customHeight="1" spans="1:5">
       <c r="A810" s="2" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="B810" s="2" t="s">
         <v>805</v>
@@ -17525,7 +17537,7 @@
     </row>
     <row r="811" customHeight="1" spans="1:5">
       <c r="A811" s="2" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="B811" s="2" t="s">
         <v>644</v>
@@ -17539,10 +17551,10 @@
     </row>
     <row r="812" customHeight="1" spans="1:5">
       <c r="A812" s="2" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="B812" s="2" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="C812" s="2" t="s">
         <v>484</v>
@@ -17553,10 +17565,10 @@
     </row>
     <row r="813" customHeight="1" spans="1:5">
       <c r="A813" s="2" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="B813" s="2" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="C813" s="2" t="s">
         <v>484</v>
@@ -17567,7 +17579,7 @@
     </row>
     <row r="814" customHeight="1" spans="1:5">
       <c r="A814" s="2" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="B814" s="2" t="s">
         <v>523</v>
@@ -17581,7 +17593,7 @@
     </row>
     <row r="815" customHeight="1" spans="1:5">
       <c r="A815" s="2" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="B815" s="2" t="s">
         <v>523</v>
@@ -17595,7 +17607,7 @@
     </row>
     <row r="816" customHeight="1" spans="1:5">
       <c r="A816" s="2" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="B816" s="2" t="s">
         <v>580</v>
@@ -17609,10 +17621,10 @@
     </row>
     <row r="817" customHeight="1" spans="1:5">
       <c r="A817" s="2" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="B817" s="2" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="C817" s="2" t="s">
         <v>484</v>
@@ -17623,7 +17635,7 @@
     </row>
     <row r="818" customHeight="1" spans="1:5">
       <c r="A818" s="2" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="B818" s="2" t="s">
         <v>570</v>
@@ -17637,7 +17649,7 @@
     </row>
     <row r="819" customHeight="1" spans="1:5">
       <c r="A819" s="2" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="B819" s="2" t="s">
         <v>580</v>
@@ -17651,7 +17663,7 @@
     </row>
     <row r="820" customHeight="1" spans="1:5">
       <c r="A820" s="2" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="B820" s="2" t="s">
         <v>488</v>
@@ -17665,7 +17677,7 @@
     </row>
     <row r="821" customHeight="1" spans="1:5">
       <c r="A821" s="2" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="B821" s="2" t="s">
         <v>760</v>
@@ -17679,7 +17691,7 @@
     </row>
     <row r="822" customHeight="1" spans="1:5">
       <c r="A822" s="2" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="B822" s="2" t="s">
         <v>943</v>
@@ -17693,7 +17705,7 @@
     </row>
     <row r="823" customHeight="1" spans="1:5">
       <c r="A823" s="2" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="B823" s="2" t="s">
         <v>570</v>
@@ -17707,10 +17719,10 @@
     </row>
     <row r="824" customHeight="1" spans="1:5">
       <c r="A824" s="2" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="B824" s="2" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="C824" s="2" t="s">
         <v>735</v>
@@ -17721,7 +17733,7 @@
     </row>
     <row r="825" customHeight="1" spans="1:5">
       <c r="A825" s="2" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="B825" s="2" t="s">
         <v>751</v>
@@ -17735,7 +17747,7 @@
     </row>
     <row r="826" customHeight="1" spans="1:5">
       <c r="A826" s="2" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="B826" s="2" t="s">
         <v>488</v>
@@ -17749,7 +17761,7 @@
     </row>
     <row r="827" customHeight="1" spans="1:5">
       <c r="A827" s="2" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="B827" s="2" t="s">
         <v>572</v>
@@ -17763,7 +17775,7 @@
     </row>
     <row r="828" customHeight="1" spans="1:5">
       <c r="A828" s="2" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="B828" s="2" t="s">
         <v>722</v>
@@ -17777,7 +17789,7 @@
     </row>
     <row r="829" customHeight="1" spans="1:5">
       <c r="A829" s="2" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="B829" s="2" t="s">
         <v>570</v>
@@ -17791,7 +17803,7 @@
     </row>
     <row r="830" customHeight="1" spans="1:5">
       <c r="A830" s="2" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="B830" s="2" t="s">
         <v>877</v>
@@ -17805,10 +17817,10 @@
     </row>
     <row r="831" customHeight="1" spans="1:5">
       <c r="A831" s="2" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="B831" s="2" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="C831" s="2" t="s">
         <v>484</v>
@@ -17819,7 +17831,7 @@
     </row>
     <row r="832" customHeight="1" spans="1:5">
       <c r="A832" s="2" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="B832" s="2" t="s">
         <v>1182</v>
@@ -17833,7 +17845,7 @@
     </row>
     <row r="833" customHeight="1" spans="1:5">
       <c r="A833" s="2" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="B833" s="2" t="s">
         <v>534</v>
@@ -17847,7 +17859,7 @@
     </row>
     <row r="834" customHeight="1" spans="1:5">
       <c r="A834" s="2" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="B834" s="2" t="s">
         <v>549</v>
@@ -17861,7 +17873,7 @@
     </row>
     <row r="835" customHeight="1" spans="1:5">
       <c r="A835" s="2" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="B835" s="2" t="s">
         <v>737</v>
@@ -17875,7 +17887,7 @@
     </row>
     <row r="836" customHeight="1" spans="1:5">
       <c r="A836" s="2" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="B836" s="2" t="s">
         <v>894</v>
@@ -17889,7 +17901,7 @@
     </row>
     <row r="837" customHeight="1" spans="1:5">
       <c r="A837" s="2" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="B837" s="2" t="s">
         <v>549</v>
@@ -17903,7 +17915,7 @@
     </row>
     <row r="838" customHeight="1" spans="1:5">
       <c r="A838" s="2" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="B838" s="2" t="s">
         <v>729</v>
@@ -17917,7 +17929,7 @@
     </row>
     <row r="839" customHeight="1" spans="1:5">
       <c r="A839" s="2" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="B839" s="2" t="s">
         <v>937</v>
@@ -17931,7 +17943,7 @@
     </row>
     <row r="840" customHeight="1" spans="1:5">
       <c r="A840" s="2" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="B840" s="2" t="s">
         <v>712</v>
@@ -17945,7 +17957,7 @@
     </row>
     <row r="841" customHeight="1" spans="1:5">
       <c r="A841" s="2" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="B841" s="2" t="s">
         <v>680</v>
@@ -17959,7 +17971,7 @@
     </row>
     <row r="842" customHeight="1" spans="1:5">
       <c r="A842" s="2" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="B842" s="2" t="s">
         <v>638</v>
@@ -17973,7 +17985,7 @@
     </row>
     <row r="843" customHeight="1" spans="1:5">
       <c r="A843" s="2" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="B843" s="2" t="s">
         <v>520</v>
@@ -17987,7 +17999,7 @@
     </row>
     <row r="844" customHeight="1" spans="1:5">
       <c r="A844" s="2" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="B844" s="2" t="s">
         <v>498</v>
@@ -18001,7 +18013,7 @@
     </row>
     <row r="845" customHeight="1" spans="1:5">
       <c r="A845" s="2" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="B845" s="2" t="s">
         <v>657</v>
@@ -18015,7 +18027,7 @@
     </row>
     <row r="846" customHeight="1" spans="1:5">
       <c r="A846" s="2" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="B846" s="2" t="s">
         <v>582</v>
@@ -18029,7 +18041,7 @@
     </row>
     <row r="847" customHeight="1" spans="1:5">
       <c r="A847" s="2" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="B847" s="2" t="s">
         <v>659</v>
@@ -18043,10 +18055,10 @@
     </row>
     <row r="848" customHeight="1" spans="1:5">
       <c r="A848" s="2" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="B848" s="2" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="C848" s="2" t="s">
         <v>765</v>
@@ -18057,7 +18069,7 @@
     </row>
     <row r="849" customHeight="1" spans="1:5">
       <c r="A849" s="2" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="B849" s="2" t="s">
         <v>877</v>
@@ -18071,7 +18083,7 @@
     </row>
     <row r="850" customHeight="1" spans="1:5">
       <c r="A850" s="2" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="B850" s="2" t="s">
         <v>865</v>
@@ -18085,7 +18097,7 @@
     </row>
     <row r="851" customHeight="1" spans="1:5">
       <c r="A851" s="2" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="B851" s="2" t="s">
         <v>647</v>
@@ -18099,7 +18111,7 @@
     </row>
     <row r="852" customHeight="1" spans="1:5">
       <c r="A852" s="2" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="B852" s="2" t="s">
         <v>805</v>
@@ -18113,7 +18125,7 @@
     </row>
     <row r="853" customHeight="1" spans="1:5">
       <c r="A853" s="2" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="B853" s="2" t="s">
         <v>1201</v>
@@ -18127,7 +18139,7 @@
     </row>
     <row r="854" customHeight="1" spans="1:5">
       <c r="A854" s="2" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="B854" s="2" t="s">
         <v>520</v>
@@ -18141,7 +18153,7 @@
     </row>
     <row r="855" customHeight="1" spans="1:5">
       <c r="A855" s="2" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="B855" s="2" t="s">
         <v>602</v>
@@ -18155,7 +18167,7 @@
     </row>
     <row r="856" customHeight="1" spans="1:5">
       <c r="A856" s="2" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="B856" s="2" t="s">
         <v>572</v>
@@ -18169,7 +18181,7 @@
     </row>
     <row r="857" customHeight="1" spans="1:5">
       <c r="A857" s="2" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="B857" s="2" t="s">
         <v>707</v>
@@ -18183,7 +18195,7 @@
     </row>
     <row r="858" customHeight="1" spans="1:5">
       <c r="A858" s="2" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="B858" s="2" t="s">
         <v>534</v>
@@ -18197,10 +18209,10 @@
     </row>
     <row r="859" customHeight="1" spans="1:5">
       <c r="A859" s="2" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="B859" s="2" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="C859" s="2" t="s">
         <v>484</v>
@@ -18211,10 +18223,10 @@
     </row>
     <row r="860" customHeight="1" spans="1:5">
       <c r="A860" s="2" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="B860" s="2" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="C860" s="2" t="s">
         <v>484</v>
@@ -18225,10 +18237,10 @@
     </row>
     <row r="861" customHeight="1" spans="1:5">
       <c r="A861" s="2" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="B861" s="2" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="C861" s="2" t="s">
         <v>484</v>
@@ -18239,7 +18251,7 @@
     </row>
     <row r="862" customHeight="1" spans="1:5">
       <c r="A862" s="2" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="B862" s="2" t="s">
         <v>602</v>
@@ -18253,10 +18265,10 @@
     </row>
     <row r="863" customHeight="1" spans="1:5">
       <c r="A863" s="2" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="B863" s="2" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="C863" s="2" t="s">
         <v>545</v>
@@ -18267,10 +18279,10 @@
     </row>
     <row r="864" customHeight="1" spans="1:5">
       <c r="A864" s="2" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="B864" s="2" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="C864" s="2" t="s">
         <v>735</v>
@@ -18281,10 +18293,10 @@
     </row>
     <row r="865" customHeight="1" spans="1:5">
       <c r="A865" s="5" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="B865" s="5" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="C865" s="5" t="s">
         <v>491</v>
@@ -18296,10 +18308,10 @@
     </row>
     <row r="866" customHeight="1" spans="1:5">
       <c r="A866" s="5" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="B866" s="5" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="C866" s="5" t="s">
         <v>494</v>
@@ -18311,10 +18323,10 @@
     </row>
     <row r="867" customHeight="1" spans="1:5">
       <c r="A867" s="1" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="B867" s="2" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="C867" s="2" t="s">
         <v>484</v>
@@ -18325,7 +18337,7 @@
     </row>
     <row r="868" customHeight="1" spans="1:5">
       <c r="A868" s="2" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="B868" s="2" t="s">
         <v>657</v>
@@ -18339,7 +18351,7 @@
     </row>
     <row r="869" customHeight="1" spans="1:5">
       <c r="A869" s="2" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="B869" s="2" t="s">
         <v>488</v>
@@ -18353,7 +18365,7 @@
     </row>
     <row r="870" customHeight="1" spans="1:5">
       <c r="A870" s="2" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="B870" s="2" t="s">
         <v>657</v>
@@ -18367,7 +18379,7 @@
     </row>
     <row r="871" customHeight="1" spans="1:5">
       <c r="A871" s="2" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="B871" s="2" t="s">
         <v>602</v>
@@ -18381,7 +18393,7 @@
     </row>
     <row r="872" customHeight="1" spans="1:5">
       <c r="A872" s="2" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="B872" s="2" t="s">
         <v>1038</v>
@@ -18395,10 +18407,10 @@
     </row>
     <row r="873" customHeight="1" spans="1:5">
       <c r="A873" s="2" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="B873" s="2" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="C873" s="2" t="s">
         <v>484</v>
@@ -18409,10 +18421,10 @@
     </row>
     <row r="874" customHeight="1" spans="1:5">
       <c r="A874" s="2" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="B874" s="2" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="C874" s="2" t="s">
         <v>484</v>
@@ -18423,10 +18435,10 @@
     </row>
     <row r="875" customHeight="1" spans="1:5">
       <c r="A875" s="2" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="B875" s="2" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="C875" s="2" t="s">
         <v>484</v>
@@ -18437,7 +18449,7 @@
     </row>
     <row r="876" customHeight="1" spans="1:5">
       <c r="A876" s="2" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="B876" s="2" t="s">
         <v>1182</v>
@@ -18451,7 +18463,7 @@
     </row>
     <row r="877" customHeight="1" spans="1:5">
       <c r="A877" s="2" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="B877" s="2" t="s">
         <v>1228</v>
@@ -18465,10 +18477,10 @@
     </row>
     <row r="878" customHeight="1" spans="1:5">
       <c r="A878" s="2" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="B878" s="2" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="C878" s="2" t="s">
         <v>484</v>
@@ -18479,7 +18491,7 @@
     </row>
     <row r="879" customHeight="1" spans="1:5">
       <c r="A879" s="2" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="B879" s="2" t="s">
         <v>534</v>
@@ -18493,7 +18505,7 @@
     </row>
     <row r="880" customHeight="1" spans="1:5">
       <c r="A880" s="2" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="B880" s="2" t="s">
         <v>483</v>
@@ -18507,7 +18519,7 @@
     </row>
     <row r="881" customHeight="1" spans="1:5">
       <c r="A881" s="2" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="B881" s="2" t="s">
         <v>607</v>
@@ -18521,7 +18533,7 @@
     </row>
     <row r="882" customHeight="1" spans="1:5">
       <c r="A882" s="2" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="B882" s="2" t="s">
         <v>631</v>
@@ -18535,10 +18547,10 @@
     </row>
     <row r="883" customHeight="1" spans="1:5">
       <c r="A883" s="2" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="B883" s="2" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="C883" s="2" t="s">
         <v>765</v>
@@ -18549,10 +18561,10 @@
     </row>
     <row r="884" customHeight="1" spans="1:5">
       <c r="A884" s="2" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="B884" s="2" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="C884" s="2" t="s">
         <v>765</v>
@@ -18563,10 +18575,10 @@
     </row>
     <row r="885" customHeight="1" spans="1:5">
       <c r="A885" s="2" t="s">
+        <v>1400</v>
+      </c>
+      <c r="B885" s="2" t="s">
         <v>1399</v>
-      </c>
-      <c r="B885" s="2" t="s">
-        <v>1398</v>
       </c>
       <c r="C885" s="2" t="s">
         <v>765</v>
@@ -18577,10 +18589,10 @@
     </row>
     <row r="886" customHeight="1" spans="1:5">
       <c r="A886" s="2" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B886" s="2" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="C886" s="2" t="s">
         <v>765</v>
@@ -18591,10 +18603,10 @@
     </row>
     <row r="887" customHeight="1" spans="1:5">
       <c r="A887" s="2" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="B887" s="2" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="C887" s="2" t="s">
         <v>765</v>
@@ -18605,10 +18617,10 @@
     </row>
     <row r="888" customHeight="1" spans="1:5">
       <c r="A888" s="2" t="s">
+        <v>1404</v>
+      </c>
+      <c r="B888" s="2" t="s">
         <v>1403</v>
-      </c>
-      <c r="B888" s="2" t="s">
-        <v>1402</v>
       </c>
       <c r="C888" s="2" t="s">
         <v>765</v>
@@ -18619,10 +18631,10 @@
     </row>
     <row r="889" customHeight="1" spans="1:5">
       <c r="A889" s="2" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="B889" s="2" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="C889" s="2" t="s">
         <v>765</v>
@@ -18633,7 +18645,7 @@
     </row>
     <row r="890" customHeight="1" spans="1:5">
       <c r="A890" s="2" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="B890" s="2" t="s">
         <v>760</v>
@@ -18647,7 +18659,7 @@
     </row>
     <row r="891" customHeight="1" spans="1:5">
       <c r="A891" s="2" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="B891" s="2" t="s">
         <v>760</v>
@@ -18661,7 +18673,7 @@
     </row>
     <row r="892" customHeight="1" spans="1:5">
       <c r="A892" s="2" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="B892" s="2" t="s">
         <v>1273</v>
@@ -18675,7 +18687,7 @@
     </row>
     <row r="893" customHeight="1" spans="1:5">
       <c r="A893" s="2" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="B893" s="2" t="s">
         <v>1273</v>
@@ -18689,7 +18701,7 @@
     </row>
     <row r="894" customHeight="1" spans="1:5">
       <c r="A894" s="2" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="B894" s="2" t="s">
         <v>1273</v>
@@ -18703,7 +18715,7 @@
     </row>
     <row r="895" customHeight="1" spans="1:5">
       <c r="A895" s="2" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="B895" s="2" t="s">
         <v>1273</v>
@@ -18717,7 +18729,7 @@
     </row>
     <row r="896" customHeight="1" spans="1:5">
       <c r="A896" s="2" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="B896" s="2" t="s">
         <v>1273</v>
@@ -18731,7 +18743,7 @@
     </row>
     <row r="897" customHeight="1" spans="1:5">
       <c r="A897" s="2" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="B897" s="2" t="s">
         <v>644</v>
@@ -18745,7 +18757,7 @@
     </row>
     <row r="898" customHeight="1" spans="1:5">
       <c r="A898" s="2" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="B898" s="2" t="s">
         <v>644</v>
@@ -18759,7 +18771,7 @@
     </row>
     <row r="899" customHeight="1" spans="1:5">
       <c r="A899" s="2" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
       <c r="B899" s="2" t="s">
         <v>644</v>
@@ -18773,7 +18785,7 @@
     </row>
     <row r="900" customHeight="1" spans="1:5">
       <c r="A900" s="2" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="B900" s="2" t="s">
         <v>644</v>
@@ -18787,7 +18799,7 @@
     </row>
     <row r="901" customHeight="1" spans="1:5">
       <c r="A901" s="2" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="B901" s="2" t="s">
         <v>644</v>
@@ -18801,7 +18813,7 @@
     </row>
     <row r="902" customHeight="1" spans="1:5">
       <c r="A902" s="2" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="B902" s="2" t="s">
         <v>644</v>
@@ -18815,7 +18827,7 @@
     </row>
     <row r="903" customHeight="1" spans="1:5">
       <c r="A903" s="2" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="B903" s="2" t="s">
         <v>644</v>
@@ -18829,10 +18841,10 @@
     </row>
     <row r="904" customHeight="1" spans="1:5">
       <c r="A904" s="2" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="B904" s="2" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="C904" s="2" t="s">
         <v>765</v>
@@ -18843,10 +18855,10 @@
     </row>
     <row r="905" customHeight="1" spans="1:5">
       <c r="A905" s="2" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="B905" s="2" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="C905" s="2" t="s">
         <v>765</v>
@@ -18857,10 +18869,10 @@
     </row>
     <row r="906" customHeight="1" spans="1:5">
       <c r="A906" s="2" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B906" s="2" t="s">
         <v>1424</v>
-      </c>
-      <c r="B906" s="2" t="s">
-        <v>1423</v>
       </c>
       <c r="C906" s="2" t="s">
         <v>765</v>
@@ -18871,10 +18883,10 @@
     </row>
     <row r="907" customHeight="1" spans="1:5">
       <c r="A907" s="2" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="B907" s="2" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="C907" s="2" t="s">
         <v>765</v>
@@ -18885,10 +18897,10 @@
     </row>
     <row r="908" customHeight="1" spans="1:5">
       <c r="A908" s="2" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="B908" s="2" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="C908" s="2" t="s">
         <v>765</v>
@@ -18899,10 +18911,10 @@
     </row>
     <row r="909" customHeight="1" spans="1:5">
       <c r="A909" s="2" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B909" s="2" t="s">
         <v>1429</v>
-      </c>
-      <c r="B909" s="2" t="s">
-        <v>1428</v>
       </c>
       <c r="C909" s="2" t="s">
         <v>765</v>
@@ -18913,10 +18925,10 @@
     </row>
     <row r="910" customHeight="1" spans="1:5">
       <c r="A910" s="2" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="B910" s="2" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="C910" s="2" t="s">
         <v>765</v>
@@ -18928,10 +18940,10 @@
     </row>
     <row r="911" customHeight="1" spans="1:5">
       <c r="A911" s="2" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="B911" s="2" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="C911" s="2" t="s">
         <v>765</v>
@@ -18942,10 +18954,10 @@
     </row>
     <row r="912" customHeight="1" spans="1:5">
       <c r="A912" s="2" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="B912" s="2" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="C912" s="2" t="s">
         <v>765</v>
@@ -18956,7 +18968,7 @@
     </row>
     <row r="913" customHeight="1" spans="1:5">
       <c r="A913" s="2" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="B913" s="2" t="s">
         <v>1182</v>
@@ -18970,10 +18982,10 @@
     </row>
     <row r="914" customHeight="1" spans="1:5">
       <c r="A914" s="2" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="B914" s="2" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="C914" s="2" t="s">
         <v>765</v>
@@ -18984,10 +18996,10 @@
     </row>
     <row r="915" customHeight="1" spans="1:5">
       <c r="A915" s="2" t="s">
+        <v>1440</v>
+      </c>
+      <c r="B915" s="2" t="s">
         <v>1439</v>
-      </c>
-      <c r="B915" s="2" t="s">
-        <v>1438</v>
       </c>
       <c r="C915" s="2" t="s">
         <v>765</v>
@@ -18998,10 +19010,10 @@
     </row>
     <row r="916" customHeight="1" spans="1:3">
       <c r="A916" s="2" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="B916" s="2" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="C916" s="2" t="s">
         <v>765</v>
@@ -19009,7 +19021,7 @@
     </row>
     <row r="917" customHeight="1" spans="1:5">
       <c r="A917" s="2" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="B917" s="2" t="s">
         <v>602</v>
@@ -19023,10 +19035,10 @@
     </row>
     <row r="918" customHeight="1" spans="1:5">
       <c r="A918" s="2" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="B918" s="2" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="C918" s="2" t="s">
         <v>765</v>
@@ -19037,10 +19049,10 @@
     </row>
     <row r="919" customHeight="1" spans="1:3">
       <c r="A919" s="2" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="B919" s="2" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="C919" s="2" t="s">
         <v>765</v>
@@ -19048,13 +19060,13 @@
     </row>
     <row r="920" customHeight="1" spans="1:5">
       <c r="A920" s="2" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="B920" s="2" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="C920" s="2" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="E920" s="4">
         <v>0</v>
@@ -19062,13 +19074,13 @@
     </row>
     <row r="921" customHeight="1" spans="1:5">
       <c r="A921" s="2" t="s">
+        <v>1450</v>
+      </c>
+      <c r="B921" s="2" t="s">
+        <v>1451</v>
+      </c>
+      <c r="C921" s="2" t="s">
         <v>1449</v>
-      </c>
-      <c r="B921" s="2" t="s">
-        <v>1450</v>
-      </c>
-      <c r="C921" s="2" t="s">
-        <v>1448</v>
       </c>
       <c r="E921" s="4">
         <v>0</v>
@@ -19076,13 +19088,13 @@
     </row>
     <row r="922" customHeight="1" spans="1:5">
       <c r="A922" s="2" t="s">
+        <v>1452</v>
+      </c>
+      <c r="B922" s="2" t="s">
         <v>1451</v>
       </c>
-      <c r="B922" s="2" t="s">
-        <v>1450</v>
-      </c>
       <c r="C922" s="2" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="E922" s="4">
         <v>0</v>
@@ -19090,13 +19102,13 @@
     </row>
     <row r="923" customHeight="1" spans="1:5">
       <c r="A923" s="2" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="B923" s="2" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="C923" s="2" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="E923" s="4">
         <v>0</v>
@@ -19104,10 +19116,10 @@
     </row>
     <row r="924" customHeight="1" spans="1:5">
       <c r="A924" s="2" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="B924" s="2" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="C924" s="2" t="s">
         <v>1025</v>
@@ -19118,10 +19130,10 @@
     </row>
     <row r="925" customHeight="1" spans="1:5">
       <c r="A925" s="2" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="B925" s="2" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="C925" s="2" t="s">
         <v>1025</v>
@@ -19132,10 +19144,10 @@
     </row>
     <row r="926" customHeight="1" spans="1:5">
       <c r="A926" s="2" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="B926" s="2" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="C926" s="2" t="s">
         <v>1025</v>
@@ -19146,10 +19158,10 @@
     </row>
     <row r="927" customHeight="1" spans="1:5">
       <c r="A927" s="2" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="B927" s="2" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="C927" s="2" t="s">
         <v>1025</v>
@@ -19160,10 +19172,10 @@
     </row>
     <row r="928" customHeight="1" spans="1:5">
       <c r="A928" s="2" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="B928" s="2" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="C928" s="2" t="s">
         <v>1025</v>
@@ -19174,10 +19186,10 @@
     </row>
     <row r="929" customHeight="1" spans="1:5">
       <c r="A929" s="2" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="B929" s="2" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="C929" s="2" t="s">
         <v>1025</v>
@@ -19188,10 +19200,10 @@
     </row>
     <row r="930" customHeight="1" spans="1:5">
       <c r="A930" s="2" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="B930" s="2" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="C930" s="2" t="s">
         <v>1025</v>
@@ -19202,7 +19214,7 @@
     </row>
     <row r="931" customHeight="1" spans="1:5">
       <c r="A931" s="2" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="B931" s="2" t="s">
         <v>742</v>
@@ -19216,10 +19228,10 @@
     </row>
     <row r="932" customHeight="1" spans="1:5">
       <c r="A932" s="2" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
       <c r="B932" s="2" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="C932" s="2" t="s">
         <v>1025</v>
@@ -19230,10 +19242,10 @@
     </row>
     <row r="933" customHeight="1" spans="1:5">
       <c r="A933" s="2" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
       <c r="B933" s="2" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="C933" s="2" t="s">
         <v>1025</v>
@@ -19244,10 +19256,10 @@
     </row>
     <row r="934" customHeight="1" spans="1:5">
       <c r="A934" s="2" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
       <c r="B934" s="2" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="C934" s="2" t="s">
         <v>1025</v>
@@ -19258,10 +19270,10 @@
     </row>
     <row r="935" customHeight="1" spans="1:5">
       <c r="A935" s="2" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
       <c r="B935" s="2" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="C935" s="2" t="s">
         <v>1025</v>
@@ -19272,10 +19284,10 @@
     </row>
     <row r="936" customHeight="1" spans="1:5">
       <c r="A936" s="2" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="B936" s="2" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="C936" s="2" t="s">
         <v>1025</v>
@@ -19286,10 +19298,10 @@
     </row>
     <row r="937" customHeight="1" spans="1:5">
       <c r="A937" s="2" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
       <c r="B937" s="2" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="C937" s="2" t="s">
         <v>1025</v>
@@ -19300,10 +19312,10 @@
     </row>
     <row r="938" customHeight="1" spans="1:5">
       <c r="A938" s="2" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
       <c r="B938" s="2" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="C938" s="2" t="s">
         <v>1025</v>
@@ -19314,10 +19326,10 @@
     </row>
     <row r="939" customHeight="1" spans="1:5">
       <c r="A939" s="2" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="B939" s="2" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
       <c r="C939" s="2" t="s">
         <v>1025</v>
@@ -19328,10 +19340,10 @@
     </row>
     <row r="940" customHeight="1" spans="1:5">
       <c r="A940" s="2" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="B940" s="2" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="C940" s="2" t="s">
         <v>1025</v>
@@ -19342,10 +19354,10 @@
     </row>
     <row r="941" customHeight="1" spans="1:5">
       <c r="A941" s="2" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="B941" s="2" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="C941" s="2" t="s">
         <v>1025</v>
@@ -19356,10 +19368,10 @@
     </row>
     <row r="942" customHeight="1" spans="1:5">
       <c r="A942" s="2" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="B942" s="2" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="C942" s="2" t="s">
         <v>1025</v>
@@ -19370,10 +19382,10 @@
     </row>
     <row r="943" customHeight="1" spans="1:5">
       <c r="A943" s="2" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="B943" s="2" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="C943" s="2" t="s">
         <v>1025</v>
@@ -19384,10 +19396,10 @@
     </row>
     <row r="944" customHeight="1" spans="1:5">
       <c r="A944" s="2" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="B944" s="2" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="C944" s="2" t="s">
         <v>1025</v>
@@ -19398,10 +19410,10 @@
     </row>
     <row r="945" customHeight="1" spans="1:5">
       <c r="A945" s="2" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="B945" s="10" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="C945" s="2" t="s">
         <v>1025</v>
@@ -19413,10 +19425,10 @@
     </row>
     <row r="946" customHeight="1" spans="1:5">
       <c r="A946" s="2" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="B946" s="10" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="C946" s="2" t="s">
         <v>1025</v>
@@ -19428,10 +19440,10 @@
     </row>
     <row r="947" customHeight="1" spans="1:5">
       <c r="A947" s="2" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="B947" s="2" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="C947" s="2" t="s">
         <v>1025</v>
@@ -19442,10 +19454,10 @@
     </row>
     <row r="948" customHeight="1" spans="1:5">
       <c r="A948" s="2" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="B948" s="2" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="C948" s="2" t="s">
         <v>1025</v>
@@ -19456,10 +19468,10 @@
     </row>
     <row r="949" customHeight="1" spans="1:5">
       <c r="A949" s="2" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="B949" s="2" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
       <c r="C949" s="2" t="s">
         <v>1025</v>
@@ -19470,10 +19482,10 @@
     </row>
     <row r="950" customHeight="1" spans="1:5">
       <c r="A950" s="2" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="B950" s="2" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="C950" s="2" t="s">
         <v>1025</v>
@@ -19484,10 +19496,10 @@
     </row>
     <row r="951" customHeight="1" spans="1:5">
       <c r="A951" s="2" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="B951" s="2" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="C951" s="2" t="s">
         <v>1025</v>
@@ -19498,10 +19510,10 @@
     </row>
     <row r="952" customHeight="1" spans="1:5">
       <c r="A952" s="2" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="B952" s="2" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="C952" s="2" t="s">
         <v>1025</v>
@@ -19512,10 +19524,10 @@
     </row>
     <row r="953" customHeight="1" spans="1:5">
       <c r="A953" s="2" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="B953" s="10" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="C953" s="2" t="s">
         <v>1025</v>
@@ -19526,10 +19538,10 @@
     </row>
     <row r="954" customHeight="1" spans="1:5">
       <c r="A954" s="2" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="B954" s="2" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="C954" s="2" t="s">
         <v>1025</v>
@@ -19540,10 +19552,10 @@
     </row>
     <row r="955" customHeight="1" spans="1:5">
       <c r="A955" s="2" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="B955" s="2" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="C955" s="2" t="s">
         <v>1025</v>
@@ -19554,10 +19566,10 @@
     </row>
     <row r="956" customHeight="1" spans="1:5">
       <c r="A956" s="2" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="B956" s="2" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="C956" s="2" t="s">
         <v>1025</v>
@@ -19567,17 +19579,17 @@
       </c>
     </row>
     <row r="957" customHeight="1" spans="1:5">
-      <c r="A957" s="24" t="s">
-        <v>1504</v>
+      <c r="A957" s="25" t="s">
+        <v>1505</v>
       </c>
       <c r="B957" s="2" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="C957" s="2" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="D957" s="2" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="E957" s="4">
         <v>0</v>

</xml_diff>

<commit_message>
v0.5.1 update, updated song list 20230725
</commit_message>
<xml_diff>
--- a/歌单.xlsx
+++ b/歌单.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3112" uniqueCount="1573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3118" uniqueCount="1575">
   <si>
     <t>2023年6月17日00:18:17更新</t>
   </si>
@@ -4441,6 +4441,9 @@
     <t>假如让我说下去</t>
   </si>
   <si>
+    <t>怯</t>
+  </si>
+  <si>
     <t>烟霞</t>
   </si>
   <si>
@@ -4460,6 +4463,9 @@
   </si>
   <si>
     <t>习惯失恋</t>
+  </si>
+  <si>
+    <t>东京人寿</t>
   </si>
   <si>
     <t>16号爱人</t>
@@ -4779,44 +4785,44 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="39">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;"/>
+    <numFmt numFmtId="176" formatCode="\¥#,##0.00;[Red]\¥\-#,##0.00"/>
+    <numFmt numFmtId="23" formatCode="\$#,##0_);\(\$#,##0\)"/>
     <numFmt numFmtId="177" formatCode="mmmm\-yy"/>
     <numFmt numFmtId="5" formatCode="&quot;￥&quot;#,##0;&quot;￥&quot;\-#,##0"/>
+    <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
+    <numFmt numFmtId="178" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
+    <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
+    <numFmt numFmtId="25" formatCode="\$#,##0.00_);\(\$#,##0.00\)"/>
+    <numFmt numFmtId="6" formatCode="&quot;￥&quot;#,##0;[Red]&quot;￥&quot;\-#,##0"/>
+    <numFmt numFmtId="179" formatCode="#\ ??/??"/>
+    <numFmt numFmtId="180" formatCode="[$-804]aaa"/>
+    <numFmt numFmtId="181" formatCode="[DBNum1][$-804]m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="8" formatCode="&quot;￥&quot;#,##0.00;[Red]&quot;￥&quot;\-#,##0.00"/>
+    <numFmt numFmtId="182" formatCode="h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="183" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
+    <numFmt numFmtId="184" formatCode="[$-804]aaaa"/>
+    <numFmt numFmtId="185" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;"/>
+    <numFmt numFmtId="186" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="187" formatCode="yy/m/d"/>
+    <numFmt numFmtId="188" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="189" formatCode="m/d"/>
+    <numFmt numFmtId="190" formatCode="mmmmm\-yy"/>
+    <numFmt numFmtId="191" formatCode="#\ ?/?"/>
+    <numFmt numFmtId="192" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
+    <numFmt numFmtId="193" formatCode="mmmmm"/>
+    <numFmt numFmtId="194" formatCode="h:mm\ AM/PM"/>
+    <numFmt numFmtId="195" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="196" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
+    <numFmt numFmtId="197" formatCode="\¥#,##0;\¥\-#,##0"/>
+    <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="198" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
+    <numFmt numFmtId="199" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="200" formatCode="#\ ??"/>
+    <numFmt numFmtId="201" formatCode="[=1]&quot;☑&quot;;[=0]&quot;☐&quot;;0;@"/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="202" formatCode="dd\-mmm\-yy"/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="mmmmm"/>
-    <numFmt numFmtId="179" formatCode="#\ ?/?"/>
-    <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
-    <numFmt numFmtId="6" formatCode="&quot;￥&quot;#,##0;[Red]&quot;￥&quot;\-#,##0"/>
-    <numFmt numFmtId="8" formatCode="&quot;￥&quot;#,##0.00;[Red]&quot;￥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="180" formatCode="\¥#,##0.00;[Red]\¥\-#,##0.00"/>
-    <numFmt numFmtId="181" formatCode="mm/dd/yy"/>
-    <numFmt numFmtId="182" formatCode="yy/m/d"/>
-    <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="183" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
-    <numFmt numFmtId="184" formatCode="dd\-mmm\-yy"/>
-    <numFmt numFmtId="185" formatCode="#\ ??/??"/>
-    <numFmt numFmtId="186" formatCode="h:mm\ AM/PM"/>
-    <numFmt numFmtId="23" formatCode="\$#,##0_);\(\$#,##0\)"/>
-    <numFmt numFmtId="187" formatCode="[$-804]aaaa"/>
-    <numFmt numFmtId="188" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="189" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
-    <numFmt numFmtId="190" formatCode="mmmmm\-yy"/>
-    <numFmt numFmtId="191" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
-    <numFmt numFmtId="192" formatCode="[DBNum1][$-804]m&quot;月&quot;d&quot;日&quot;"/>
-    <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
-    <numFmt numFmtId="193" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
-    <numFmt numFmtId="194" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
-    <numFmt numFmtId="195" formatCode="[=1]&quot;☑&quot;;[=0]&quot;☐&quot;;0;@"/>
-    <numFmt numFmtId="196" formatCode="\¥#,##0;\¥\-#,##0"/>
-    <numFmt numFmtId="197" formatCode="#\ ??"/>
-    <numFmt numFmtId="198" formatCode="m/d"/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="25" formatCode="\$#,##0.00_);\(\$#,##0.00\)"/>
-    <numFmt numFmtId="199" formatCode="[$-804]aaa"/>
-    <numFmt numFmtId="200" formatCode="h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="201" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
-    <numFmt numFmtId="202" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -4876,120 +4882,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -5005,7 +4897,39 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -5016,6 +4940,88 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -5040,7 +5046,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5052,7 +5082,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5064,13 +5148,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5082,79 +5172,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5172,13 +5190,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5190,37 +5220,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5271,29 +5277,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5309,6 +5303,24 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5345,6 +5357,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -5353,168 +5374,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="202" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="199" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="195" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="188" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -5531,7 +5537,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="195" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="201" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5558,7 +5564,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="195" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="201" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5579,10 +5585,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="195" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="201" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="195" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="201" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5919,7 +5925,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F995"/>
+  <dimension ref="A1:F997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
@@ -19337,7 +19343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="931" customHeight="1" spans="1:5">
+    <row r="931" customHeight="1" spans="1:3">
       <c r="A931" s="2" t="s">
         <v>1474</v>
       </c>
@@ -19346,9 +19352,6 @@
       </c>
       <c r="C931" s="2" t="s">
         <v>1450</v>
-      </c>
-      <c r="E931" s="4">
-        <v>0</v>
       </c>
     </row>
     <row r="932" customHeight="1" spans="1:5">
@@ -19449,26 +19452,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="939" customHeight="1" spans="1:5">
+    <row r="939" customHeight="1" spans="1:3">
       <c r="A939" s="2" t="s">
         <v>1482</v>
       </c>
       <c r="B939" s="2" t="s">
-        <v>1483</v>
+        <v>688</v>
       </c>
       <c r="C939" s="2" t="s">
         <v>1450</v>
       </c>
-      <c r="E939" s="4">
-        <v>0</v>
-      </c>
     </row>
     <row r="940" customHeight="1" spans="1:5">
       <c r="A940" s="2" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="B940" s="2" t="s">
-        <v>1485</v>
+        <v>688</v>
       </c>
       <c r="C940" s="2" t="s">
         <v>1450</v>
@@ -19479,7 +19479,7 @@
     </row>
     <row r="941" customHeight="1" spans="1:5">
       <c r="A941" s="2" t="s">
-        <v>1486</v>
+        <v>1484</v>
       </c>
       <c r="B941" s="2" t="s">
         <v>1485</v>
@@ -19493,10 +19493,10 @@
     </row>
     <row r="942" customHeight="1" spans="1:5">
       <c r="A942" s="2" t="s">
+        <v>1486</v>
+      </c>
+      <c r="B942" s="2" t="s">
         <v>1487</v>
-      </c>
-      <c r="B942" s="2" t="s">
-        <v>1488</v>
       </c>
       <c r="C942" s="2" t="s">
         <v>1450</v>
@@ -19507,10 +19507,10 @@
     </row>
     <row r="943" customHeight="1" spans="1:5">
       <c r="A943" s="2" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="B943" s="2" t="s">
-        <v>1490</v>
+        <v>1487</v>
       </c>
       <c r="C943" s="2" t="s">
         <v>1450</v>
@@ -19521,7 +19521,7 @@
     </row>
     <row r="944" customHeight="1" spans="1:5">
       <c r="A944" s="2" t="s">
-        <v>1491</v>
+        <v>1489</v>
       </c>
       <c r="B944" s="2" t="s">
         <v>1490</v>
@@ -19535,25 +19535,24 @@
     </row>
     <row r="945" customHeight="1" spans="1:5">
       <c r="A945" s="2" t="s">
+        <v>1491</v>
+      </c>
+      <c r="B945" s="2" t="s">
         <v>1492</v>
-      </c>
-      <c r="B945" s="2" t="s">
-        <v>1493</v>
       </c>
       <c r="C945" s="2" t="s">
         <v>1450</v>
       </c>
-      <c r="D945" s="2"/>
       <c r="E945" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="946" customHeight="1" spans="1:5">
       <c r="A946" s="2" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="B946" s="2" t="s">
-        <v>1495</v>
+        <v>1492</v>
       </c>
       <c r="C946" s="2" t="s">
         <v>1450</v>
@@ -19562,9 +19561,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="947" customHeight="1" spans="1:3">
+    <row r="947" customHeight="1" spans="1:5">
       <c r="A947" s="2" t="s">
-        <v>1496</v>
+        <v>1494</v>
       </c>
       <c r="B947" s="2" t="s">
         <v>1495</v>
@@ -19572,13 +19571,17 @@
       <c r="C947" s="2" t="s">
         <v>1450</v>
       </c>
+      <c r="D947" s="2"/>
+      <c r="E947" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="948" customHeight="1" spans="1:5">
       <c r="A948" s="2" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B948" s="2" t="s">
         <v>1497</v>
-      </c>
-      <c r="B948" s="2" t="s">
-        <v>1498</v>
       </c>
       <c r="C948" s="2" t="s">
         <v>1450</v>
@@ -19587,26 +19590,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="949" customHeight="1" spans="1:5">
+    <row r="949" customHeight="1" spans="1:3">
       <c r="A949" s="2" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="B949" s="2" t="s">
-        <v>1237</v>
+        <v>1497</v>
       </c>
       <c r="C949" s="2" t="s">
         <v>1450</v>
       </c>
-      <c r="E949" s="4">
-        <v>0</v>
-      </c>
     </row>
     <row r="950" customHeight="1" spans="1:5">
       <c r="A950" s="2" t="s">
+        <v>1499</v>
+      </c>
+      <c r="B950" s="2" t="s">
         <v>1500</v>
-      </c>
-      <c r="B950" s="2" t="s">
-        <v>1501</v>
       </c>
       <c r="C950" s="2" t="s">
         <v>1450</v>
@@ -19617,10 +19617,10 @@
     </row>
     <row r="951" customHeight="1" spans="1:5">
       <c r="A951" s="2" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="B951" s="2" t="s">
-        <v>1501</v>
+        <v>1237</v>
       </c>
       <c r="C951" s="2" t="s">
         <v>1450</v>
@@ -19629,15 +19629,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="952" customHeight="1" spans="1:3">
+    <row r="952" customHeight="1" spans="1:5">
       <c r="A952" s="2" t="s">
+        <v>1502</v>
+      </c>
+      <c r="B952" s="2" t="s">
         <v>1503</v>
-      </c>
-      <c r="B952" s="2" t="s">
-        <v>1501</v>
       </c>
       <c r="C952" s="2" t="s">
         <v>1450</v>
+      </c>
+      <c r="E952" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="953" customHeight="1" spans="1:5">
@@ -19645,7 +19648,7 @@
         <v>1504</v>
       </c>
       <c r="B953" s="2" t="s">
-        <v>644</v>
+        <v>1503</v>
       </c>
       <c r="C953" s="2" t="s">
         <v>1450</v>
@@ -19654,73 +19657,70 @@
         <v>0</v>
       </c>
     </row>
-    <row r="954" customHeight="1" spans="1:5">
+    <row r="954" customHeight="1" spans="1:3">
       <c r="A954" s="2" t="s">
         <v>1505</v>
       </c>
       <c r="B954" s="2" t="s">
-        <v>1506</v>
+        <v>1503</v>
       </c>
       <c r="C954" s="2" t="s">
         <v>1450</v>
       </c>
-      <c r="E954" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="955" customHeight="1" spans="1:3">
+    </row>
+    <row r="955" customHeight="1" spans="1:5">
       <c r="A955" s="2" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="B955" s="2" t="s">
-        <v>1508</v>
+        <v>644</v>
       </c>
       <c r="C955" s="2" t="s">
         <v>1450</v>
       </c>
-    </row>
-    <row r="956" customHeight="1" spans="1:3">
+      <c r="E955" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="956" customHeight="1" spans="1:5">
       <c r="A956" s="2" t="s">
-        <v>1509</v>
+        <v>1507</v>
       </c>
       <c r="B956" s="2" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
       <c r="C956" s="2" t="s">
         <v>1450</v>
       </c>
-    </row>
-    <row r="957" customHeight="1" spans="1:5">
+      <c r="E956" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="957" customHeight="1" spans="1:3">
       <c r="A957" s="2" t="s">
-        <v>1511</v>
+        <v>1509</v>
       </c>
       <c r="B957" s="2" t="s">
-        <v>1512</v>
+        <v>1510</v>
       </c>
       <c r="C957" s="2" t="s">
         <v>1450</v>
       </c>
-      <c r="E957" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="958" customHeight="1" spans="1:5">
+    </row>
+    <row r="958" customHeight="1" spans="1:3">
       <c r="A958" s="2" t="s">
-        <v>1513</v>
+        <v>1511</v>
       </c>
       <c r="B958" s="2" t="s">
-        <v>1514</v>
+        <v>1512</v>
       </c>
       <c r="C958" s="2" t="s">
         <v>1450</v>
       </c>
-      <c r="E958" s="4">
-        <v>0</v>
-      </c>
     </row>
     <row r="959" customHeight="1" spans="1:5">
       <c r="A959" s="2" t="s">
-        <v>1515</v>
+        <v>1513</v>
       </c>
       <c r="B959" s="2" t="s">
         <v>1514</v>
@@ -19734,10 +19734,10 @@
     </row>
     <row r="960" customHeight="1" spans="1:5">
       <c r="A960" s="2" t="s">
+        <v>1515</v>
+      </c>
+      <c r="B960" s="2" t="s">
         <v>1516</v>
-      </c>
-      <c r="B960" s="2" t="s">
-        <v>1514</v>
       </c>
       <c r="C960" s="2" t="s">
         <v>1450</v>
@@ -19751,10 +19751,10 @@
         <v>1517</v>
       </c>
       <c r="B961" s="2" t="s">
-        <v>1518</v>
+        <v>1516</v>
       </c>
       <c r="C961" s="2" t="s">
-        <v>1074</v>
+        <v>1450</v>
       </c>
       <c r="E961" s="4">
         <v>0</v>
@@ -19762,13 +19762,13 @@
     </row>
     <row r="962" customHeight="1" spans="1:5">
       <c r="A962" s="2" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="B962" s="2" t="s">
-        <v>1520</v>
+        <v>1516</v>
       </c>
       <c r="C962" s="2" t="s">
-        <v>1074</v>
+        <v>1450</v>
       </c>
       <c r="E962" s="4">
         <v>0</v>
@@ -19776,10 +19776,10 @@
     </row>
     <row r="963" customHeight="1" spans="1:5">
       <c r="A963" s="2" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
       <c r="B963" s="2" t="s">
-        <v>1522</v>
+        <v>1520</v>
       </c>
       <c r="C963" s="2" t="s">
         <v>1074</v>
@@ -19790,10 +19790,10 @@
     </row>
     <row r="964" customHeight="1" spans="1:5">
       <c r="A964" s="2" t="s">
-        <v>1523</v>
+        <v>1521</v>
       </c>
       <c r="B964" s="2" t="s">
-        <v>1524</v>
+        <v>1522</v>
       </c>
       <c r="C964" s="2" t="s">
         <v>1074</v>
@@ -19804,10 +19804,10 @@
     </row>
     <row r="965" customHeight="1" spans="1:5">
       <c r="A965" s="2" t="s">
-        <v>1525</v>
+        <v>1523</v>
       </c>
       <c r="B965" s="2" t="s">
-        <v>1526</v>
+        <v>1524</v>
       </c>
       <c r="C965" s="2" t="s">
         <v>1074</v>
@@ -19818,10 +19818,10 @@
     </row>
     <row r="966" customHeight="1" spans="1:5">
       <c r="A966" s="2" t="s">
-        <v>1527</v>
+        <v>1525</v>
       </c>
       <c r="B966" s="2" t="s">
-        <v>1528</v>
+        <v>1526</v>
       </c>
       <c r="C966" s="2" t="s">
         <v>1074</v>
@@ -19830,23 +19830,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="967" customHeight="1" spans="1:3">
+    <row r="967" customHeight="1" spans="1:5">
       <c r="A967" s="2" t="s">
-        <v>1529</v>
+        <v>1527</v>
       </c>
       <c r="B967" s="2" t="s">
-        <v>1530</v>
+        <v>1528</v>
       </c>
       <c r="C967" s="2" t="s">
         <v>1074</v>
       </c>
+      <c r="E967" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="968" customHeight="1" spans="1:5">
       <c r="A968" s="2" t="s">
-        <v>1531</v>
+        <v>1529</v>
       </c>
       <c r="B968" s="2" t="s">
-        <v>1532</v>
+        <v>1530</v>
       </c>
       <c r="C968" s="2" t="s">
         <v>1074</v>
@@ -19855,26 +19858,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="969" customHeight="1" spans="1:5">
+    <row r="969" customHeight="1" spans="1:3">
       <c r="A969" s="2" t="s">
-        <v>1533</v>
+        <v>1531</v>
       </c>
       <c r="B969" s="2" t="s">
-        <v>787</v>
+        <v>1532</v>
       </c>
       <c r="C969" s="2" t="s">
         <v>1074</v>
       </c>
-      <c r="E969" s="4">
-        <v>0</v>
-      </c>
     </row>
     <row r="970" customHeight="1" spans="1:5">
       <c r="A970" s="2" t="s">
+        <v>1533</v>
+      </c>
+      <c r="B970" s="2" t="s">
         <v>1534</v>
-      </c>
-      <c r="B970" s="2" t="s">
-        <v>1524</v>
       </c>
       <c r="C970" s="2" t="s">
         <v>1074</v>
@@ -19888,7 +19888,7 @@
         <v>1535</v>
       </c>
       <c r="B971" s="2" t="s">
-        <v>1536</v>
+        <v>787</v>
       </c>
       <c r="C971" s="2" t="s">
         <v>1074</v>
@@ -19899,10 +19899,10 @@
     </row>
     <row r="972" customHeight="1" spans="1:5">
       <c r="A972" s="2" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="B972" s="2" t="s">
-        <v>1520</v>
+        <v>1526</v>
       </c>
       <c r="C972" s="2" t="s">
         <v>1074</v>
@@ -19913,10 +19913,10 @@
     </row>
     <row r="973" customHeight="1" spans="1:5">
       <c r="A973" s="2" t="s">
+        <v>1537</v>
+      </c>
+      <c r="B973" s="2" t="s">
         <v>1538</v>
-      </c>
-      <c r="B973" s="2" t="s">
-        <v>1524</v>
       </c>
       <c r="C973" s="2" t="s">
         <v>1074</v>
@@ -19930,7 +19930,7 @@
         <v>1539</v>
       </c>
       <c r="B974" s="2" t="s">
-        <v>1532</v>
+        <v>1522</v>
       </c>
       <c r="C974" s="2" t="s">
         <v>1074</v>
@@ -19944,7 +19944,7 @@
         <v>1540</v>
       </c>
       <c r="B975" s="2" t="s">
-        <v>1528</v>
+        <v>1526</v>
       </c>
       <c r="C975" s="2" t="s">
         <v>1074</v>
@@ -19958,7 +19958,7 @@
         <v>1541</v>
       </c>
       <c r="B976" s="2" t="s">
-        <v>1524</v>
+        <v>1534</v>
       </c>
       <c r="C976" s="2" t="s">
         <v>1074</v>
@@ -19972,7 +19972,7 @@
         <v>1542</v>
       </c>
       <c r="B977" s="2" t="s">
-        <v>1543</v>
+        <v>1530</v>
       </c>
       <c r="C977" s="2" t="s">
         <v>1074</v>
@@ -19983,10 +19983,10 @@
     </row>
     <row r="978" customHeight="1" spans="1:5">
       <c r="A978" s="2" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="B978" s="2" t="s">
-        <v>1524</v>
+        <v>1526</v>
       </c>
       <c r="C978" s="2" t="s">
         <v>1074</v>
@@ -19997,10 +19997,10 @@
     </row>
     <row r="979" customHeight="1" spans="1:5">
       <c r="A979" s="2" t="s">
+        <v>1544</v>
+      </c>
+      <c r="B979" s="2" t="s">
         <v>1545</v>
-      </c>
-      <c r="B979" s="2" t="s">
-        <v>1546</v>
       </c>
       <c r="C979" s="2" t="s">
         <v>1074</v>
@@ -20011,10 +20011,10 @@
     </row>
     <row r="980" customHeight="1" spans="1:5">
       <c r="A980" s="2" t="s">
-        <v>407</v>
+        <v>1546</v>
       </c>
       <c r="B980" s="2" t="s">
-        <v>1547</v>
+        <v>1526</v>
       </c>
       <c r="C980" s="2" t="s">
         <v>1074</v>
@@ -20025,10 +20025,10 @@
     </row>
     <row r="981" customHeight="1" spans="1:5">
       <c r="A981" s="2" t="s">
+        <v>1547</v>
+      </c>
+      <c r="B981" s="2" t="s">
         <v>1548</v>
-      </c>
-      <c r="B981" s="2" t="s">
-        <v>1549</v>
       </c>
       <c r="C981" s="2" t="s">
         <v>1074</v>
@@ -20039,10 +20039,10 @@
     </row>
     <row r="982" customHeight="1" spans="1:5">
       <c r="A982" s="2" t="s">
-        <v>1550</v>
+        <v>407</v>
       </c>
       <c r="B982" s="2" t="s">
-        <v>1551</v>
+        <v>1549</v>
       </c>
       <c r="C982" s="2" t="s">
         <v>1074</v>
@@ -20053,68 +20053,68 @@
     </row>
     <row r="983" customHeight="1" spans="1:5">
       <c r="A983" s="2" t="s">
-        <v>1552</v>
-      </c>
-      <c r="B983" s="10" t="s">
-        <v>1553</v>
+        <v>1550</v>
+      </c>
+      <c r="B983" s="2" t="s">
+        <v>1551</v>
       </c>
       <c r="C983" s="2" t="s">
         <v>1074</v>
       </c>
-      <c r="D983" s="2"/>
       <c r="E983" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="984" customHeight="1" spans="1:5">
       <c r="A984" s="2" t="s">
-        <v>1554</v>
-      </c>
-      <c r="B984" s="10" t="s">
-        <v>1555</v>
+        <v>1552</v>
+      </c>
+      <c r="B984" s="2" t="s">
+        <v>1553</v>
       </c>
       <c r="C984" s="2" t="s">
         <v>1074</v>
       </c>
-      <c r="D984" s="2"/>
       <c r="E984" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="985" customHeight="1" spans="1:5">
       <c r="A985" s="2" t="s">
-        <v>1556</v>
-      </c>
-      <c r="B985" s="2" t="s">
-        <v>1557</v>
+        <v>1554</v>
+      </c>
+      <c r="B985" s="10" t="s">
+        <v>1555</v>
       </c>
       <c r="C985" s="2" t="s">
         <v>1074</v>
       </c>
+      <c r="D985" s="2"/>
       <c r="E985" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="986" customHeight="1" spans="1:5">
       <c r="A986" s="2" t="s">
-        <v>1558</v>
-      </c>
-      <c r="B986" s="2" t="s">
-        <v>1524</v>
+        <v>1556</v>
+      </c>
+      <c r="B986" s="10" t="s">
+        <v>1557</v>
       </c>
       <c r="C986" s="2" t="s">
         <v>1074</v>
       </c>
+      <c r="D986" s="2"/>
       <c r="E986" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="987" customHeight="1" spans="1:5">
       <c r="A987" s="2" t="s">
+        <v>1558</v>
+      </c>
+      <c r="B987" s="2" t="s">
         <v>1559</v>
-      </c>
-      <c r="B987" s="2" t="s">
-        <v>1543</v>
       </c>
       <c r="C987" s="2" t="s">
         <v>1074</v>
@@ -20128,7 +20128,7 @@
         <v>1560</v>
       </c>
       <c r="B988" s="2" t="s">
-        <v>1561</v>
+        <v>1526</v>
       </c>
       <c r="C988" s="2" t="s">
         <v>1074</v>
@@ -20139,10 +20139,10 @@
     </row>
     <row r="989" customHeight="1" spans="1:5">
       <c r="A989" s="2" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="B989" s="2" t="s">
-        <v>1532</v>
+        <v>1545</v>
       </c>
       <c r="C989" s="2" t="s">
         <v>1074</v>
@@ -20153,10 +20153,10 @@
     </row>
     <row r="990" customHeight="1" spans="1:5">
       <c r="A990" s="2" t="s">
+        <v>1562</v>
+      </c>
+      <c r="B990" s="2" t="s">
         <v>1563</v>
-      </c>
-      <c r="B990" s="2" t="s">
-        <v>1524</v>
       </c>
       <c r="C990" s="2" t="s">
         <v>1074</v>
@@ -20169,8 +20169,8 @@
       <c r="A991" s="2" t="s">
         <v>1564</v>
       </c>
-      <c r="B991" s="10" t="s">
-        <v>1565</v>
+      <c r="B991" s="2" t="s">
+        <v>1534</v>
       </c>
       <c r="C991" s="2" t="s">
         <v>1074</v>
@@ -20181,10 +20181,10 @@
     </row>
     <row r="992" customHeight="1" spans="1:5">
       <c r="A992" s="2" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="B992" s="2" t="s">
-        <v>1528</v>
+        <v>1526</v>
       </c>
       <c r="C992" s="2" t="s">
         <v>1074</v>
@@ -20195,10 +20195,10 @@
     </row>
     <row r="993" customHeight="1" spans="1:5">
       <c r="A993" s="2" t="s">
+        <v>1566</v>
+      </c>
+      <c r="B993" s="10" t="s">
         <v>1567</v>
-      </c>
-      <c r="B993" s="2" t="s">
-        <v>1524</v>
       </c>
       <c r="C993" s="2" t="s">
         <v>1074</v>
@@ -20212,7 +20212,7 @@
         <v>1568</v>
       </c>
       <c r="B994" s="2" t="s">
-        <v>1532</v>
+        <v>1530</v>
       </c>
       <c r="C994" s="2" t="s">
         <v>1074</v>
@@ -20222,19 +20222,47 @@
       </c>
     </row>
     <row r="995" customHeight="1" spans="1:5">
-      <c r="A995" s="26" t="s">
+      <c r="A995" s="2" t="s">
         <v>1569</v>
       </c>
       <c r="B995" s="2" t="s">
+        <v>1526</v>
+      </c>
+      <c r="C995" s="2" t="s">
+        <v>1074</v>
+      </c>
+      <c r="E995" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="996" customHeight="1" spans="1:5">
+      <c r="A996" s="2" t="s">
         <v>1570</v>
       </c>
-      <c r="C995" s="2" t="s">
+      <c r="B996" s="2" t="s">
+        <v>1534</v>
+      </c>
+      <c r="C996" s="2" t="s">
+        <v>1074</v>
+      </c>
+      <c r="E996" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="997" customHeight="1" spans="1:5">
+      <c r="A997" s="26" t="s">
         <v>1571</v>
       </c>
-      <c r="D995" s="2" t="s">
+      <c r="B997" s="2" t="s">
         <v>1572</v>
       </c>
-      <c r="E995" s="4">
+      <c r="C997" s="2" t="s">
+        <v>1573</v>
+      </c>
+      <c r="D997" s="2" t="s">
+        <v>1574</v>
+      </c>
+      <c r="E997" s="4">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v0.6.2 update, updated song list 231021
</commit_message>
<xml_diff>
--- a/歌单.xlsx
+++ b/歌单.xlsx
@@ -1393,7 +1393,7 @@
     <t>※踊</t>
   </si>
   <si>
-    <t>カルデラ</t>
+    <t>※カルデラ</t>
   </si>
   <si>
     <t>黑木渚</t>
@@ -4510,7 +4510,7 @@
     <t>最熟悉的陌生人</t>
   </si>
   <si>
-    <t>自己按门铃自己听</t>
+    <t>※自己按门铃自己听</t>
   </si>
   <si>
     <t>呼吸有害</t>
@@ -4940,45 +4940,45 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="39">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;"/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="\¥#,##0.00;[Red]\¥\-#,##0.00"/>
+    <numFmt numFmtId="23" formatCode="\$#,##0_);\(\$#,##0\)"/>
+    <numFmt numFmtId="178" formatCode="#\ ??/??"/>
     <numFmt numFmtId="6" formatCode="&quot;￥&quot;#,##0;[Red]&quot;￥&quot;\-#,##0"/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="\¥#,##0.00;[Red]\¥\-#,##0.00"/>
-    <numFmt numFmtId="23" formatCode="\$#,##0_);\(\$#,##0\)"/>
-    <numFmt numFmtId="177" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;"/>
-    <numFmt numFmtId="178" formatCode="#\ ??/??"/>
-    <numFmt numFmtId="179" formatCode="mmmm\-yy"/>
+    <numFmt numFmtId="5" formatCode="&quot;￥&quot;#,##0;&quot;￥&quot;\-#,##0"/>
+    <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
+    <numFmt numFmtId="25" formatCode="\$#,##0.00_);\(\$#,##0.00\)"/>
+    <numFmt numFmtId="179" formatCode="[DBNum1][$-804]m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="180" formatCode="#\ ?/?"/>
+    <numFmt numFmtId="181" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
+    <numFmt numFmtId="182" formatCode="yy/m/d"/>
+    <numFmt numFmtId="183" formatCode="m/d"/>
+    <numFmt numFmtId="184" formatCode="dd\-mmm\-yy"/>
+    <numFmt numFmtId="185" formatCode="[$-804]aaaa"/>
+    <numFmt numFmtId="186" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
+    <numFmt numFmtId="187" formatCode="mmmmm"/>
+    <numFmt numFmtId="188" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="189" formatCode="[$-804]aaa"/>
+    <numFmt numFmtId="190" formatCode="mmmmm\-yy"/>
+    <numFmt numFmtId="191" formatCode="[=1]&quot;☑&quot;;[=0]&quot;☐&quot;;0;@"/>
+    <numFmt numFmtId="192" formatCode="mmmm\-yy"/>
+    <numFmt numFmtId="193" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="194" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
+    <numFmt numFmtId="195" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
+    <numFmt numFmtId="196" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
+    <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;￥&quot;#,##0.00;[Red]&quot;￥&quot;\-#,##0.00"/>
+    <numFmt numFmtId="197" formatCode="#\ ??"/>
+    <numFmt numFmtId="198" formatCode="h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="199" formatCode="\¥#,##0;\¥\-#,##0"/>
+    <numFmt numFmtId="200" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
     <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
-    <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="180" formatCode="h:mm\ AM/PM"/>
-    <numFmt numFmtId="25" formatCode="\$#,##0.00_);\(\$#,##0.00\)"/>
-    <numFmt numFmtId="181" formatCode="[$-804]aaaa"/>
-    <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
-    <numFmt numFmtId="182" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
-    <numFmt numFmtId="183" formatCode="mmmmm\-yy"/>
-    <numFmt numFmtId="184" formatCode="h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="185" formatCode="[DBNum1][$-804]m&quot;月&quot;d&quot;日&quot;"/>
-    <numFmt numFmtId="186" formatCode="[$-804]aaa"/>
-    <numFmt numFmtId="187" formatCode="mm/dd/yy"/>
-    <numFmt numFmtId="188" formatCode="yy/m/d"/>
+    <numFmt numFmtId="201" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="189" formatCode="m/d"/>
-    <numFmt numFmtId="190" formatCode="[=1]&quot;☑&quot;;[=0]&quot;☐&quot;;0;@"/>
-    <numFmt numFmtId="191" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
-    <numFmt numFmtId="192" formatCode="#\ ?/?"/>
-    <numFmt numFmtId="193" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
-    <numFmt numFmtId="194" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
-    <numFmt numFmtId="5" formatCode="&quot;￥&quot;#,##0;&quot;￥&quot;\-#,##0"/>
-    <numFmt numFmtId="8" formatCode="&quot;￥&quot;#,##0.00;[Red]&quot;￥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="195" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
-    <numFmt numFmtId="196" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="197" formatCode="#\ ??"/>
-    <numFmt numFmtId="198" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
-    <numFmt numFmtId="199" formatCode="\¥#,##0;\¥\-#,##0"/>
-    <numFmt numFmtId="200" formatCode="dd\-mmm\-yy"/>
-    <numFmt numFmtId="201" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="202" formatCode="mmmmm"/>
+    <numFmt numFmtId="202" formatCode="h:mm\ AM/PM"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -5044,22 +5044,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -5074,6 +5058,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
@@ -5082,7 +5105,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -5090,7 +5113,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -5105,6 +5128,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -5114,23 +5145,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -5145,7 +5160,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -5154,28 +5176,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -5202,7 +5202,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5214,7 +5280,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5226,13 +5310,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5244,145 +5376,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5451,21 +5451,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -5520,6 +5505,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -5535,145 +5535,145 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="201" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="196" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="188" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -5693,7 +5693,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="190" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="191" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5720,7 +5720,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="190" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="191" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5741,10 +5741,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="190" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="191" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="190" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="191" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -6088,7 +6088,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A1" sqref="$A1:$XFD1048576"/>
+      <selection pane="bottomRight" activeCell="A943" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.625" defaultRowHeight="23.5" customHeight="1" outlineLevelCol="5"/>
@@ -9670,16 +9670,16 @@
       </c>
     </row>
     <row r="229" customHeight="1" spans="1:5">
-      <c r="A229" s="2" t="s">
+      <c r="A229" s="5" t="s">
         <v>458</v>
       </c>
-      <c r="B229" s="2" t="s">
+      <c r="B229" s="5" t="s">
         <v>459</v>
       </c>
-      <c r="C229" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D229" s="2"/>
+      <c r="C229" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D229" s="5"/>
       <c r="E229" s="4">
         <v>0</v>
       </c>
@@ -19591,15 +19591,16 @@
       </c>
     </row>
     <row r="943" customHeight="1" spans="1:5">
-      <c r="A943" s="2" t="s">
+      <c r="A943" s="5" t="s">
         <v>1497</v>
       </c>
-      <c r="B943" s="2" t="s">
+      <c r="B943" s="5" t="s">
         <v>711</v>
       </c>
-      <c r="C943" s="2" t="s">
+      <c r="C943" s="5" t="s">
         <v>594</v>
       </c>
+      <c r="D943" s="6"/>
       <c r="E943" s="4">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
v0.7.5 update, updated song list 240401
</commit_message>
<xml_diff>
--- a/歌单.xlsx
+++ b/歌单.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3290" uniqueCount="1662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3296" uniqueCount="1664">
   <si>
     <t>2023年6月17日00:18:17更新</t>
   </si>
@@ -4408,6 +4408,9 @@
     <t>夜宴风波</t>
   </si>
   <si>
+    <t>越过山丘</t>
+  </si>
+  <si>
     <t>愚人的国度</t>
   </si>
   <si>
@@ -4852,7 +4855,7 @@
     <t>Blank Space</t>
   </si>
   <si>
-    <t>Taylor Swift（泰勒斯威夫特）</t>
+    <t>Taylor Swift</t>
   </si>
   <si>
     <t>Creep</t>
@@ -4864,7 +4867,7 @@
     <t>Complicated</t>
   </si>
   <si>
-    <t>Avril Lavigne（艾薇儿）</t>
+    <t>Avril Lavigne</t>
   </si>
   <si>
     <t>Close to the sun</t>
@@ -4888,7 +4891,7 @@
     <t>Everytime</t>
   </si>
   <si>
-    <t>Britney Spears（布兰妮）</t>
+    <t>Britney Spears</t>
   </si>
   <si>
     <t>Faded</t>
@@ -4913,6 +4916,9 @@
   </si>
   <si>
     <t>Love story</t>
+  </si>
+  <si>
+    <t>Long Live</t>
   </si>
   <si>
     <t>Let her go</t>
@@ -5045,45 +5051,45 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="39">
+    <numFmt numFmtId="176" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;"/>
     <numFmt numFmtId="6" formatCode="&quot;￥&quot;#,##0;[Red]&quot;￥&quot;\-#,##0"/>
+    <numFmt numFmtId="177" formatCode="\¥#,##0.00;[Red]\¥\-#,##0.00"/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="#\ ??/??"/>
-    <numFmt numFmtId="177" formatCode="\¥#,##0.00;[Red]\¥\-#,##0.00"/>
-    <numFmt numFmtId="178" formatCode="mmmm\-yy"/>
-    <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
-    <numFmt numFmtId="179" formatCode="#\ ?/?"/>
+    <numFmt numFmtId="5" formatCode="&quot;￥&quot;#,##0;&quot;￥&quot;\-#,##0"/>
+    <numFmt numFmtId="178" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
+    <numFmt numFmtId="25" formatCode="\$#,##0.00_);\(\$#,##0.00\)"/>
+    <numFmt numFmtId="179" formatCode="mmmm\-yy"/>
     <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
     <numFmt numFmtId="180" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
-    <numFmt numFmtId="5" formatCode="&quot;￥&quot;#,##0;&quot;￥&quot;\-#,##0"/>
     <numFmt numFmtId="181" formatCode="[$-804]aaa"/>
-    <numFmt numFmtId="182" formatCode="h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="182" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
     <numFmt numFmtId="183" formatCode="[DBNum1][$-804]m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="8" formatCode="&quot;￥&quot;#,##0.00;[Red]&quot;￥&quot;\-#,##0.00"/>
+    <numFmt numFmtId="184" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
+    <numFmt numFmtId="185" formatCode="h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
+    <numFmt numFmtId="186" formatCode="[$-804]aaaa"/>
+    <numFmt numFmtId="23" formatCode="\$#,##0_);\(\$#,##0\)"/>
+    <numFmt numFmtId="187" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
+    <numFmt numFmtId="188" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
+    <numFmt numFmtId="189" formatCode="mmmmm"/>
+    <numFmt numFmtId="190" formatCode="[=1]&quot;☑&quot;;[=0]&quot;☐&quot;;0;@"/>
+    <numFmt numFmtId="191" formatCode="mmmmm\-yy"/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="8" formatCode="&quot;￥&quot;#,##0.00;[Red]&quot;￥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="184" formatCode="[DBNum1]上午/下午h&quot;时&quot;mm&quot;分&quot;"/>
-    <numFmt numFmtId="185" formatCode="yy/m/d"/>
-    <numFmt numFmtId="186" formatCode="yyyy/m/d\ h:mm\ AM/PM"/>
-    <numFmt numFmtId="187" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
-    <numFmt numFmtId="188" formatCode="m/d"/>
-    <numFmt numFmtId="189" formatCode="mmmmm\-yy"/>
-    <numFmt numFmtId="190" formatCode="dd\-mmm\-yy"/>
-    <numFmt numFmtId="25" formatCode="\$#,##0.00_);\(\$#,##0.00\)"/>
+    <numFmt numFmtId="192" formatCode="#\ ??"/>
+    <numFmt numFmtId="193" formatCode="#\ ??/??"/>
+    <numFmt numFmtId="194" formatCode="h:mm\ AM/PM"/>
+    <numFmt numFmtId="195" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
+    <numFmt numFmtId="196" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="197" formatCode="dd\-mmm\-yy"/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="198" formatCode="#\ ?/?"/>
+    <numFmt numFmtId="199" formatCode="\¥#,##0;\¥\-#,##0"/>
+    <numFmt numFmtId="200" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="201" formatCode="yy/m/d"/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="191" formatCode="\¥#,##0;\¥\-#,##0"/>
-    <numFmt numFmtId="192" formatCode="[=1]&quot;☑&quot;;[=0]&quot;☐&quot;;0;@"/>
-    <numFmt numFmtId="193" formatCode="\¥#,##0;[Red]\¥\-#,##0"/>
-    <numFmt numFmtId="194" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;"/>
-    <numFmt numFmtId="195" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="196" formatCode="[$-804]aaaa"/>
-    <numFmt numFmtId="197" formatCode="\¥#,##0.00;\¥\-#,##0.00"/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="198" formatCode="#\ ??"/>
-    <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
-    <numFmt numFmtId="199" formatCode="h:mm\ AM/PM"/>
-    <numFmt numFmtId="23" formatCode="\$#,##0_);\(\$#,##0\)"/>
-    <numFmt numFmtId="200" formatCode="mmmmm"/>
-    <numFmt numFmtId="201" formatCode="mm/dd/yy"/>
-    <numFmt numFmtId="202" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="202" formatCode="m/d"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -5143,7 +5149,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -5156,17 +5162,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -5180,18 +5193,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -5206,13 +5212,6 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -5234,17 +5233,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -5259,7 +5257,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -5273,14 +5278,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -5307,31 +5313,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5349,7 +5343,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5361,13 +5361,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5379,13 +5391,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5403,91 +5475,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5541,23 +5547,32 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5577,17 +5592,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5621,15 +5636,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
@@ -5640,148 +5646,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="202" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="196" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="195" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -5798,7 +5804,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="192" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="190" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5825,7 +5831,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="192" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="190" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5843,7 +5849,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="192" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="190" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5855,7 +5861,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="192" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="190" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -6186,7 +6192,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F1054"/>
+  <dimension ref="A1:F1056"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
@@ -19194,18 +19200,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="911" customHeight="1" spans="1:5">
+    <row r="911" customHeight="1" spans="1:3">
       <c r="A911" s="2" t="s">
         <v>1463</v>
       </c>
       <c r="B911" s="2" t="s">
-        <v>670</v>
+        <v>983</v>
       </c>
       <c r="C911" s="2" t="s">
         <v>579</v>
-      </c>
-      <c r="E911" s="4">
-        <v>0</v>
       </c>
     </row>
     <row r="912" customHeight="1" spans="1:5">
@@ -19213,10 +19216,10 @@
         <v>1464</v>
       </c>
       <c r="B912" s="2" t="s">
-        <v>990</v>
+        <v>670</v>
       </c>
       <c r="C912" s="2" t="s">
-        <v>843</v>
+        <v>579</v>
       </c>
       <c r="E912" s="4">
         <v>0</v>
@@ -19227,10 +19230,10 @@
         <v>1465</v>
       </c>
       <c r="B913" s="2" t="s">
-        <v>1466</v>
+        <v>990</v>
       </c>
       <c r="C913" s="2" t="s">
-        <v>579</v>
+        <v>843</v>
       </c>
       <c r="E913" s="4">
         <v>0</v>
@@ -19238,10 +19241,10 @@
     </row>
     <row r="914" customHeight="1" spans="1:5">
       <c r="A914" s="2" t="s">
+        <v>1466</v>
+      </c>
+      <c r="B914" s="2" t="s">
         <v>1467</v>
-      </c>
-      <c r="B914" s="2" t="s">
-        <v>1312</v>
       </c>
       <c r="C914" s="2" t="s">
         <v>579</v>
@@ -19255,7 +19258,7 @@
         <v>1468</v>
       </c>
       <c r="B915" s="2" t="s">
-        <v>632</v>
+        <v>1312</v>
       </c>
       <c r="C915" s="2" t="s">
         <v>579</v>
@@ -19269,7 +19272,7 @@
         <v>1469</v>
       </c>
       <c r="B916" s="2" t="s">
-        <v>647</v>
+        <v>632</v>
       </c>
       <c r="C916" s="2" t="s">
         <v>579</v>
@@ -19283,7 +19286,7 @@
         <v>1470</v>
       </c>
       <c r="B917" s="2" t="s">
-        <v>848</v>
+        <v>647</v>
       </c>
       <c r="C917" s="2" t="s">
         <v>579</v>
@@ -19297,7 +19300,7 @@
         <v>1471</v>
       </c>
       <c r="B918" s="2" t="s">
-        <v>1007</v>
+        <v>848</v>
       </c>
       <c r="C918" s="2" t="s">
         <v>579</v>
@@ -19311,7 +19314,7 @@
         <v>1472</v>
       </c>
       <c r="B919" s="2" t="s">
-        <v>647</v>
+        <v>1007</v>
       </c>
       <c r="C919" s="2" t="s">
         <v>579</v>
@@ -19325,7 +19328,7 @@
         <v>1473</v>
       </c>
       <c r="B920" s="2" t="s">
-        <v>837</v>
+        <v>647</v>
       </c>
       <c r="C920" s="2" t="s">
         <v>579</v>
@@ -19339,7 +19342,7 @@
         <v>1474</v>
       </c>
       <c r="B921" s="2" t="s">
-        <v>1053</v>
+        <v>837</v>
       </c>
       <c r="C921" s="2" t="s">
         <v>579</v>
@@ -19353,7 +19356,7 @@
         <v>1475</v>
       </c>
       <c r="B922" s="2" t="s">
-        <v>820</v>
+        <v>1053</v>
       </c>
       <c r="C922" s="2" t="s">
         <v>579</v>
@@ -19367,7 +19370,7 @@
         <v>1476</v>
       </c>
       <c r="B923" s="2" t="s">
-        <v>788</v>
+        <v>820</v>
       </c>
       <c r="C923" s="2" t="s">
         <v>579</v>
@@ -19381,7 +19384,7 @@
         <v>1477</v>
       </c>
       <c r="B924" s="2" t="s">
-        <v>746</v>
+        <v>788</v>
       </c>
       <c r="C924" s="2" t="s">
         <v>579</v>
@@ -19395,7 +19398,7 @@
         <v>1478</v>
       </c>
       <c r="B925" s="2" t="s">
-        <v>618</v>
+        <v>746</v>
       </c>
       <c r="C925" s="2" t="s">
         <v>579</v>
@@ -19409,7 +19412,7 @@
         <v>1479</v>
       </c>
       <c r="B926" s="2" t="s">
-        <v>594</v>
+        <v>618</v>
       </c>
       <c r="C926" s="2" t="s">
         <v>579</v>
@@ -19423,7 +19426,7 @@
         <v>1480</v>
       </c>
       <c r="B927" s="2" t="s">
-        <v>765</v>
+        <v>594</v>
       </c>
       <c r="C927" s="2" t="s">
         <v>579</v>
@@ -19437,7 +19440,7 @@
         <v>1481</v>
       </c>
       <c r="B928" s="2" t="s">
-        <v>684</v>
+        <v>765</v>
       </c>
       <c r="C928" s="2" t="s">
         <v>579</v>
@@ -19451,7 +19454,7 @@
         <v>1482</v>
       </c>
       <c r="B929" s="2" t="s">
-        <v>767</v>
+        <v>684</v>
       </c>
       <c r="C929" s="2" t="s">
         <v>579</v>
@@ -19465,10 +19468,10 @@
         <v>1483</v>
       </c>
       <c r="B930" s="2" t="s">
-        <v>990</v>
+        <v>767</v>
       </c>
       <c r="C930" s="2" t="s">
-        <v>843</v>
+        <v>579</v>
       </c>
       <c r="E930" s="4">
         <v>0</v>
@@ -19479,10 +19482,10 @@
         <v>1484</v>
       </c>
       <c r="B931" s="2" t="s">
-        <v>978</v>
+        <v>990</v>
       </c>
       <c r="C931" s="2" t="s">
-        <v>579</v>
+        <v>843</v>
       </c>
       <c r="E931" s="4">
         <v>0</v>
@@ -19493,7 +19496,7 @@
         <v>1485</v>
       </c>
       <c r="B932" s="2" t="s">
-        <v>755</v>
+        <v>978</v>
       </c>
       <c r="C932" s="2" t="s">
         <v>579</v>
@@ -19507,7 +19510,7 @@
         <v>1486</v>
       </c>
       <c r="B933" s="2" t="s">
-        <v>916</v>
+        <v>755</v>
       </c>
       <c r="C933" s="2" t="s">
         <v>579</v>
@@ -19521,7 +19524,7 @@
         <v>1487</v>
       </c>
       <c r="B934" s="2" t="s">
-        <v>1331</v>
+        <v>916</v>
       </c>
       <c r="C934" s="2" t="s">
         <v>579</v>
@@ -19530,40 +19533,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="935" customHeight="1" spans="1:3">
+    <row r="935" customHeight="1" spans="1:5">
       <c r="A935" s="2" t="s">
         <v>1488</v>
       </c>
       <c r="B935" s="2" t="s">
-        <v>1489</v>
+        <v>1331</v>
       </c>
       <c r="C935" s="2" t="s">
         <v>579</v>
+      </c>
+      <c r="E935" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="936" customHeight="1" spans="1:3">
       <c r="A936" s="2" t="s">
+        <v>1489</v>
+      </c>
+      <c r="B936" s="2" t="s">
         <v>1490</v>
       </c>
-      <c r="B936" s="2" t="s">
-        <v>848</v>
-      </c>
       <c r="C936" s="2" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="937" customHeight="1" spans="1:5">
+    <row r="937" customHeight="1" spans="1:3">
       <c r="A937" s="2" t="s">
         <v>1491</v>
       </c>
       <c r="B937" s="2" t="s">
-        <v>618</v>
+        <v>848</v>
       </c>
       <c r="C937" s="2" t="s">
         <v>579</v>
-      </c>
-      <c r="E937" s="4">
-        <v>0</v>
       </c>
     </row>
     <row r="938" customHeight="1" spans="1:5">
@@ -19571,7 +19574,7 @@
         <v>1492</v>
       </c>
       <c r="B938" s="2" t="s">
-        <v>682</v>
+        <v>618</v>
       </c>
       <c r="C938" s="2" t="s">
         <v>579</v>
@@ -19585,7 +19588,7 @@
         <v>1493</v>
       </c>
       <c r="B939" s="2" t="s">
-        <v>672</v>
+        <v>682</v>
       </c>
       <c r="C939" s="2" t="s">
         <v>579</v>
@@ -19599,7 +19602,7 @@
         <v>1494</v>
       </c>
       <c r="B940" s="2" t="s">
-        <v>815</v>
+        <v>672</v>
       </c>
       <c r="C940" s="2" t="s">
         <v>579</v>
@@ -19613,7 +19616,7 @@
         <v>1495</v>
       </c>
       <c r="B941" s="2" t="s">
-        <v>632</v>
+        <v>815</v>
       </c>
       <c r="C941" s="2" t="s">
         <v>579</v>
@@ -19627,7 +19630,7 @@
         <v>1496</v>
       </c>
       <c r="B942" s="2" t="s">
-        <v>1497</v>
+        <v>632</v>
       </c>
       <c r="C942" s="2" t="s">
         <v>579</v>
@@ -19638,10 +19641,10 @@
     </row>
     <row r="943" customHeight="1" spans="1:5">
       <c r="A943" s="2" t="s">
+        <v>1497</v>
+      </c>
+      <c r="B943" s="2" t="s">
         <v>1498</v>
-      </c>
-      <c r="B943" s="2" t="s">
-        <v>1499</v>
       </c>
       <c r="C943" s="2" t="s">
         <v>579</v>
@@ -19652,10 +19655,10 @@
     </row>
     <row r="944" customHeight="1" spans="1:5">
       <c r="A944" s="2" t="s">
+        <v>1499</v>
+      </c>
+      <c r="B944" s="2" t="s">
         <v>1500</v>
-      </c>
-      <c r="B944" s="2" t="s">
-        <v>1501</v>
       </c>
       <c r="C944" s="2" t="s">
         <v>579</v>
@@ -19666,10 +19669,10 @@
     </row>
     <row r="945" customHeight="1" spans="1:5">
       <c r="A945" s="2" t="s">
+        <v>1501</v>
+      </c>
+      <c r="B945" s="2" t="s">
         <v>1502</v>
-      </c>
-      <c r="B945" s="2" t="s">
-        <v>682</v>
       </c>
       <c r="C945" s="2" t="s">
         <v>579</v>
@@ -19683,10 +19686,10 @@
         <v>1503</v>
       </c>
       <c r="B946" s="2" t="s">
-        <v>1504</v>
+        <v>682</v>
       </c>
       <c r="C946" s="2" t="s">
-        <v>643</v>
+        <v>579</v>
       </c>
       <c r="E946" s="4">
         <v>0</v>
@@ -19694,42 +19697,41 @@
     </row>
     <row r="947" customHeight="1" spans="1:5">
       <c r="A947" s="2" t="s">
+        <v>1504</v>
+      </c>
+      <c r="B947" s="2" t="s">
         <v>1505</v>
       </c>
-      <c r="B947" s="2" t="s">
+      <c r="C947" s="2" t="s">
+        <v>643</v>
+      </c>
+      <c r="E947" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="948" customHeight="1" spans="1:5">
+      <c r="A948" s="2" t="s">
         <v>1506</v>
       </c>
-      <c r="C947" s="2" t="s">
+      <c r="B948" s="2" t="s">
+        <v>1507</v>
+      </c>
+      <c r="C948" s="2" t="s">
         <v>843</v>
       </c>
-      <c r="E947" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="948" customHeight="1" spans="1:5">
-      <c r="A948" s="5" t="s">
-        <v>1507</v>
-      </c>
-      <c r="B948" s="5" t="s">
-        <v>1508</v>
-      </c>
-      <c r="C948" s="5" t="s">
-        <v>587</v>
-      </c>
-      <c r="D948" s="6"/>
       <c r="E948" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="949" customHeight="1" spans="1:5">
       <c r="A949" s="5" t="s">
+        <v>1508</v>
+      </c>
+      <c r="B949" s="5" t="s">
         <v>1509</v>
       </c>
-      <c r="B949" s="5" t="s">
-        <v>1510</v>
-      </c>
       <c r="C949" s="5" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="D949" s="6"/>
       <c r="E949" s="4">
@@ -19737,25 +19739,26 @@
       </c>
     </row>
     <row r="950" customHeight="1" spans="1:5">
-      <c r="A950" s="1" t="s">
+      <c r="A950" s="5" t="s">
+        <v>1510</v>
+      </c>
+      <c r="B950" s="5" t="s">
         <v>1511</v>
       </c>
-      <c r="B950" s="2" t="s">
+      <c r="C950" s="5" t="s">
+        <v>590</v>
+      </c>
+      <c r="D950" s="6"/>
+      <c r="E950" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="951" customHeight="1" spans="1:5">
+      <c r="A951" s="1" t="s">
         <v>1512</v>
       </c>
-      <c r="C950" s="2" t="s">
-        <v>579</v>
-      </c>
-      <c r="E950" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="951" customHeight="1" spans="1:5">
-      <c r="A951" s="2" t="s">
+      <c r="B951" s="2" t="s">
         <v>1513</v>
-      </c>
-      <c r="B951" s="2" t="s">
-        <v>765</v>
       </c>
       <c r="C951" s="2" t="s">
         <v>579</v>
@@ -19769,7 +19772,7 @@
         <v>1514</v>
       </c>
       <c r="B952" s="2" t="s">
-        <v>583</v>
+        <v>765</v>
       </c>
       <c r="C952" s="2" t="s">
         <v>579</v>
@@ -19783,7 +19786,7 @@
         <v>1515</v>
       </c>
       <c r="B953" s="2" t="s">
-        <v>765</v>
+        <v>583</v>
       </c>
       <c r="C953" s="2" t="s">
         <v>579</v>
@@ -19797,13 +19800,13 @@
         <v>1516</v>
       </c>
       <c r="B954" s="2" t="s">
-        <v>682</v>
+        <v>765</v>
       </c>
       <c r="C954" s="2" t="s">
         <v>579</v>
       </c>
       <c r="E954" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="955" customHeight="1" spans="1:5">
@@ -19811,13 +19814,13 @@
         <v>1517</v>
       </c>
       <c r="B955" s="2" t="s">
-        <v>1155</v>
+        <v>682</v>
       </c>
       <c r="C955" s="2" t="s">
         <v>579</v>
       </c>
       <c r="E955" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="956" customHeight="1" spans="1:5">
@@ -19825,7 +19828,7 @@
         <v>1518</v>
       </c>
       <c r="B956" s="2" t="s">
-        <v>1519</v>
+        <v>1155</v>
       </c>
       <c r="C956" s="2" t="s">
         <v>579</v>
@@ -19836,10 +19839,10 @@
     </row>
     <row r="957" customHeight="1" spans="1:5">
       <c r="A957" s="2" t="s">
+        <v>1519</v>
+      </c>
+      <c r="B957" s="2" t="s">
         <v>1520</v>
-      </c>
-      <c r="B957" s="2" t="s">
-        <v>1521</v>
       </c>
       <c r="C957" s="2" t="s">
         <v>579</v>
@@ -19850,10 +19853,10 @@
     </row>
     <row r="958" customHeight="1" spans="1:5">
       <c r="A958" s="2" t="s">
+        <v>1521</v>
+      </c>
+      <c r="B958" s="2" t="s">
         <v>1522</v>
-      </c>
-      <c r="B958" s="2" t="s">
-        <v>846</v>
       </c>
       <c r="C958" s="2" t="s">
         <v>579</v>
@@ -19867,7 +19870,7 @@
         <v>1523</v>
       </c>
       <c r="B959" s="2" t="s">
-        <v>1312</v>
+        <v>846</v>
       </c>
       <c r="C959" s="2" t="s">
         <v>579</v>
@@ -19881,7 +19884,7 @@
         <v>1524</v>
       </c>
       <c r="B960" s="2" t="s">
-        <v>1357</v>
+        <v>1312</v>
       </c>
       <c r="C960" s="2" t="s">
         <v>579</v>
@@ -19895,7 +19898,7 @@
         <v>1525</v>
       </c>
       <c r="B961" s="2" t="s">
-        <v>1526</v>
+        <v>1357</v>
       </c>
       <c r="C961" s="2" t="s">
         <v>579</v>
@@ -19906,10 +19909,10 @@
     </row>
     <row r="962" customHeight="1" spans="1:5">
       <c r="A962" s="2" t="s">
+        <v>1526</v>
+      </c>
+      <c r="B962" s="2" t="s">
         <v>1527</v>
-      </c>
-      <c r="B962" s="2" t="s">
-        <v>632</v>
       </c>
       <c r="C962" s="2" t="s">
         <v>579</v>
@@ -19923,7 +19926,7 @@
         <v>1528</v>
       </c>
       <c r="B963" s="2" t="s">
-        <v>578</v>
+        <v>632</v>
       </c>
       <c r="C963" s="2" t="s">
         <v>579</v>
@@ -19937,53 +19940,53 @@
         <v>1529</v>
       </c>
       <c r="B964" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="C964" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="E964" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="965" customHeight="1" spans="1:5">
+      <c r="A965" s="2" t="s">
+        <v>1530</v>
+      </c>
+      <c r="B965" s="2" t="s">
         <v>711</v>
       </c>
-      <c r="C964" s="2" t="s">
-        <v>579</v>
-      </c>
-      <c r="E964" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="965" customHeight="1" spans="1:5">
-      <c r="A965" s="5" t="s">
-        <v>1530</v>
-      </c>
-      <c r="B965" s="5" t="s">
+      <c r="C965" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="E965" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="966" customHeight="1" spans="1:5">
+      <c r="A966" s="5" t="s">
+        <v>1531</v>
+      </c>
+      <c r="B966" s="5" t="s">
         <v>739</v>
       </c>
-      <c r="C965" s="5" t="s">
+      <c r="C966" s="5" t="s">
         <v>619</v>
       </c>
-      <c r="D965" s="6"/>
-      <c r="E965" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="966" customHeight="1" spans="1:5">
-      <c r="A966" s="2" t="s">
-        <v>1531</v>
-      </c>
-      <c r="B966" s="2" t="s">
-        <v>578</v>
-      </c>
-      <c r="C966" s="2" t="s">
-        <v>1532</v>
-      </c>
+      <c r="D966" s="6"/>
       <c r="E966" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="967" customHeight="1" spans="1:5">
       <c r="A967" s="2" t="s">
+        <v>1532</v>
+      </c>
+      <c r="B967" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="C967" s="2" t="s">
         <v>1533</v>
-      </c>
-      <c r="B967" s="2" t="s">
-        <v>1534</v>
-      </c>
-      <c r="C967" s="2" t="s">
-        <v>1532</v>
       </c>
       <c r="E967" s="4">
         <v>0</v>
@@ -19991,13 +19994,13 @@
     </row>
     <row r="968" customHeight="1" spans="1:5">
       <c r="A968" s="2" t="s">
+        <v>1534</v>
+      </c>
+      <c r="B968" s="2" t="s">
         <v>1535</v>
       </c>
-      <c r="B968" s="2" t="s">
-        <v>746</v>
-      </c>
       <c r="C968" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E968" s="4">
         <v>0</v>
@@ -20008,10 +20011,10 @@
         <v>1536</v>
       </c>
       <c r="B969" s="2" t="s">
-        <v>1537</v>
+        <v>746</v>
       </c>
       <c r="C969" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E969" s="4">
         <v>0</v>
@@ -20019,13 +20022,13 @@
     </row>
     <row r="970" customHeight="1" spans="1:5">
       <c r="A970" s="2" t="s">
+        <v>1537</v>
+      </c>
+      <c r="B970" s="2" t="s">
         <v>1538</v>
       </c>
-      <c r="B970" s="2" t="s">
-        <v>1539</v>
-      </c>
       <c r="C970" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E970" s="4">
         <v>0</v>
@@ -20033,13 +20036,13 @@
     </row>
     <row r="971" customHeight="1" spans="1:5">
       <c r="A971" s="2" t="s">
+        <v>1539</v>
+      </c>
+      <c r="B971" s="2" t="s">
         <v>1540</v>
       </c>
-      <c r="B971" s="2" t="s">
-        <v>1539</v>
-      </c>
       <c r="C971" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E971" s="4">
         <v>0</v>
@@ -20050,10 +20053,10 @@
         <v>1541</v>
       </c>
       <c r="B972" s="2" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="C972" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E972" s="4">
         <v>0</v>
@@ -20064,10 +20067,10 @@
         <v>1542</v>
       </c>
       <c r="B973" s="2" t="s">
-        <v>1543</v>
+        <v>1540</v>
       </c>
       <c r="C973" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E973" s="4">
         <v>0</v>
@@ -20075,13 +20078,13 @@
     </row>
     <row r="974" customHeight="1" spans="1:5">
       <c r="A974" s="2" t="s">
+        <v>1543</v>
+      </c>
+      <c r="B974" s="2" t="s">
         <v>1544</v>
       </c>
-      <c r="B974" s="2" t="s">
-        <v>1543</v>
-      </c>
       <c r="C974" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E974" s="4">
         <v>0</v>
@@ -20092,10 +20095,10 @@
         <v>1545</v>
       </c>
       <c r="B975" s="2" t="s">
-        <v>1546</v>
+        <v>1544</v>
       </c>
       <c r="C975" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E975" s="4">
         <v>0</v>
@@ -20103,13 +20106,13 @@
     </row>
     <row r="976" customHeight="1" spans="1:5">
       <c r="A976" s="2" t="s">
+        <v>1546</v>
+      </c>
+      <c r="B976" s="2" t="s">
         <v>1547</v>
       </c>
-      <c r="B976" s="2" t="s">
-        <v>873</v>
-      </c>
       <c r="C976" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E976" s="4">
         <v>0</v>
@@ -20123,7 +20126,7 @@
         <v>873</v>
       </c>
       <c r="C977" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E977" s="4">
         <v>0</v>
@@ -20134,10 +20137,10 @@
         <v>1549</v>
       </c>
       <c r="B978" s="2" t="s">
-        <v>1550</v>
+        <v>873</v>
       </c>
       <c r="C978" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E978" s="4">
         <v>0</v>
@@ -20145,13 +20148,13 @@
     </row>
     <row r="979" customHeight="1" spans="1:5">
       <c r="A979" s="2" t="s">
+        <v>1550</v>
+      </c>
+      <c r="B979" s="2" t="s">
         <v>1551</v>
       </c>
-      <c r="B979" s="2" t="s">
-        <v>1550</v>
-      </c>
       <c r="C979" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E979" s="4">
         <v>0</v>
@@ -20162,10 +20165,10 @@
         <v>1552</v>
       </c>
       <c r="B980" s="2" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="C980" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E980" s="4">
         <v>0</v>
@@ -20176,10 +20179,10 @@
         <v>1553</v>
       </c>
       <c r="B981" s="2" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="C981" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E981" s="4">
         <v>0</v>
@@ -20190,10 +20193,10 @@
         <v>1554</v>
       </c>
       <c r="B982" s="2" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="C982" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E982" s="4">
         <v>0</v>
@@ -20204,27 +20207,30 @@
         <v>1555</v>
       </c>
       <c r="B983" s="2" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="C983" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E983" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="984" customHeight="1" spans="1:3">
+    <row r="984" customHeight="1" spans="1:5">
       <c r="A984" s="2" t="s">
         <v>1556</v>
       </c>
       <c r="B984" s="2" t="s">
-        <v>752</v>
+        <v>1551</v>
       </c>
       <c r="C984" s="2" t="s">
-        <v>1532</v>
-      </c>
-    </row>
-    <row r="985" customHeight="1" spans="1:5">
+        <v>1533</v>
+      </c>
+      <c r="E984" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="985" customHeight="1" spans="1:3">
       <c r="A985" s="2" t="s">
         <v>1557</v>
       </c>
@@ -20232,10 +20238,7 @@
         <v>752</v>
       </c>
       <c r="C985" s="2" t="s">
-        <v>1532</v>
-      </c>
-      <c r="E985" s="4">
-        <v>0</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="986" customHeight="1" spans="1:5">
@@ -20246,7 +20249,7 @@
         <v>752</v>
       </c>
       <c r="C986" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E986" s="4">
         <v>0</v>
@@ -20260,7 +20263,7 @@
         <v>752</v>
       </c>
       <c r="C987" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E987" s="4">
         <v>0</v>
@@ -20274,7 +20277,7 @@
         <v>752</v>
       </c>
       <c r="C988" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E988" s="4">
         <v>0</v>
@@ -20288,7 +20291,7 @@
         <v>752</v>
       </c>
       <c r="C989" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E989" s="4">
         <v>0</v>
@@ -20302,7 +20305,7 @@
         <v>752</v>
       </c>
       <c r="C990" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E990" s="4">
         <v>0</v>
@@ -20316,13 +20319,13 @@
         <v>752</v>
       </c>
       <c r="C991" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E991" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="992" customHeight="1" spans="1:3">
+    <row r="992" customHeight="1" spans="1:5">
       <c r="A992" s="2" t="s">
         <v>1564</v>
       </c>
@@ -20330,10 +20333,13 @@
         <v>752</v>
       </c>
       <c r="C992" s="2" t="s">
-        <v>1532</v>
-      </c>
-    </row>
-    <row r="993" customHeight="1" spans="1:5">
+        <v>1533</v>
+      </c>
+      <c r="E992" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="993" customHeight="1" spans="1:3">
       <c r="A993" s="2" t="s">
         <v>1565</v>
       </c>
@@ -20341,10 +20347,7 @@
         <v>752</v>
       </c>
       <c r="C993" s="2" t="s">
-        <v>1532</v>
-      </c>
-      <c r="E993" s="4">
-        <v>0</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="994" customHeight="1" spans="1:5">
@@ -20352,10 +20355,10 @@
         <v>1566</v>
       </c>
       <c r="B994" s="2" t="s">
-        <v>1567</v>
+        <v>752</v>
       </c>
       <c r="C994" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E994" s="4">
         <v>0</v>
@@ -20363,13 +20366,13 @@
     </row>
     <row r="995" customHeight="1" spans="1:5">
       <c r="A995" s="2" t="s">
+        <v>1567</v>
+      </c>
+      <c r="B995" s="2" t="s">
         <v>1568</v>
       </c>
-      <c r="B995" s="2" t="s">
-        <v>1569</v>
-      </c>
       <c r="C995" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E995" s="4">
         <v>0</v>
@@ -20377,13 +20380,13 @@
     </row>
     <row r="996" customHeight="1" spans="1:5">
       <c r="A996" s="2" t="s">
+        <v>1569</v>
+      </c>
+      <c r="B996" s="2" t="s">
         <v>1570</v>
       </c>
-      <c r="B996" s="2" t="s">
-        <v>1569</v>
-      </c>
       <c r="C996" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E996" s="4">
         <v>0</v>
@@ -20394,10 +20397,10 @@
         <v>1571</v>
       </c>
       <c r="B997" s="2" t="s">
-        <v>1572</v>
+        <v>1570</v>
       </c>
       <c r="C997" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E997" s="4">
         <v>0</v>
@@ -20405,13 +20408,13 @@
     </row>
     <row r="998" customHeight="1" spans="1:5">
       <c r="A998" s="2" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B998" s="2" t="s">
         <v>1573</v>
       </c>
-      <c r="B998" s="2" t="s">
-        <v>1574</v>
-      </c>
       <c r="C998" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E998" s="4">
         <v>0</v>
@@ -20419,13 +20422,13 @@
     </row>
     <row r="999" customHeight="1" spans="1:5">
       <c r="A999" s="2" t="s">
+        <v>1574</v>
+      </c>
+      <c r="B999" s="2" t="s">
         <v>1575</v>
       </c>
-      <c r="B999" s="2" t="s">
-        <v>1574</v>
-      </c>
       <c r="C999" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E999" s="4">
         <v>0</v>
@@ -20436,64 +20439,64 @@
         <v>1576</v>
       </c>
       <c r="B1000" s="2" t="s">
-        <v>1577</v>
+        <v>1575</v>
       </c>
       <c r="C1000" s="2" t="s">
-        <v>1532</v>
-      </c>
-      <c r="D1000" s="2"/>
+        <v>1533</v>
+      </c>
       <c r="E1000" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="1001" customHeight="1" spans="1:5">
       <c r="A1001" s="2" t="s">
+        <v>1577</v>
+      </c>
+      <c r="B1001" s="2" t="s">
         <v>1578</v>
       </c>
-      <c r="B1001" s="2" t="s">
-        <v>1489</v>
-      </c>
       <c r="C1001" s="2" t="s">
-        <v>1532</v>
-      </c>
+        <v>1533</v>
+      </c>
+      <c r="D1001" s="2"/>
       <c r="E1001" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="1002" customHeight="1" spans="1:3">
+    <row r="1002" customHeight="1" spans="1:5">
       <c r="A1002" s="2" t="s">
         <v>1579</v>
       </c>
       <c r="B1002" s="2" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="C1002" s="2" t="s">
-        <v>1532</v>
-      </c>
-    </row>
-    <row r="1003" customHeight="1" spans="1:5">
+        <v>1533</v>
+      </c>
+      <c r="E1002" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1003" customHeight="1" spans="1:3">
       <c r="A1003" s="2" t="s">
         <v>1580</v>
       </c>
       <c r="B1003" s="2" t="s">
-        <v>1581</v>
+        <v>1490</v>
       </c>
       <c r="C1003" s="2" t="s">
-        <v>1532</v>
-      </c>
-      <c r="E1003" s="4">
-        <v>0</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="1004" customHeight="1" spans="1:5">
       <c r="A1004" s="2" t="s">
+        <v>1581</v>
+      </c>
+      <c r="B1004" s="2" t="s">
         <v>1582</v>
       </c>
-      <c r="B1004" s="2" t="s">
-        <v>1312</v>
-      </c>
       <c r="C1004" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E1004" s="4">
         <v>0</v>
@@ -20504,10 +20507,10 @@
         <v>1583</v>
       </c>
       <c r="B1005" s="2" t="s">
-        <v>1584</v>
+        <v>1312</v>
       </c>
       <c r="C1005" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E1005" s="4">
         <v>0</v>
@@ -20515,27 +20518,30 @@
     </row>
     <row r="1006" customHeight="1" spans="1:5">
       <c r="A1006" s="2" t="s">
+        <v>1584</v>
+      </c>
+      <c r="B1006" s="2" t="s">
         <v>1585</v>
       </c>
-      <c r="B1006" s="2" t="s">
-        <v>1584</v>
-      </c>
       <c r="C1006" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E1006" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="1007" customHeight="1" spans="1:3">
+    <row r="1007" customHeight="1" spans="1:5">
       <c r="A1007" s="2" t="s">
         <v>1586</v>
       </c>
       <c r="B1007" s="2" t="s">
-        <v>1584</v>
+        <v>1585</v>
       </c>
       <c r="C1007" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
+      </c>
+      <c r="E1007" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="1008" customHeight="1" spans="1:3">
@@ -20543,13 +20549,13 @@
         <v>1587</v>
       </c>
       <c r="B1008" s="2" t="s">
-        <v>682</v>
+        <v>1585</v>
       </c>
       <c r="C1008" s="2" t="s">
-        <v>1532</v>
-      </c>
-    </row>
-    <row r="1009" customHeight="1" spans="1:5">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="1009" customHeight="1" spans="1:3">
       <c r="A1009" s="2" t="s">
         <v>1588</v>
       </c>
@@ -20557,10 +20563,7 @@
         <v>682</v>
       </c>
       <c r="C1009" s="2" t="s">
-        <v>1532</v>
-      </c>
-      <c r="E1009" s="4">
-        <v>0</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="1010" customHeight="1" spans="1:5">
@@ -20568,82 +20571,82 @@
         <v>1589</v>
       </c>
       <c r="B1010" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="C1010" s="2" t="s">
+        <v>1533</v>
+      </c>
+      <c r="E1010" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1011" customHeight="1" spans="1:5">
+      <c r="A1011" s="2" t="s">
         <v>1590</v>
       </c>
-      <c r="C1010" s="2" t="s">
-        <v>1532</v>
-      </c>
-      <c r="E1010" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1011" customHeight="1" spans="1:3">
-      <c r="A1011" s="2" t="s">
+      <c r="B1011" s="2" t="s">
         <v>1591</v>
       </c>
-      <c r="B1011" s="2" t="s">
-        <v>1592</v>
-      </c>
       <c r="C1011" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
+      </c>
+      <c r="E1011" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="1012" customHeight="1" spans="1:3">
       <c r="A1012" s="2" t="s">
+        <v>1592</v>
+      </c>
+      <c r="B1012" s="2" t="s">
         <v>1593</v>
       </c>
-      <c r="B1012" s="2" t="s">
-        <v>1594</v>
-      </c>
       <c r="C1012" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="1013" customHeight="1" spans="1:3">
       <c r="A1013" s="2" t="s">
+        <v>1594</v>
+      </c>
+      <c r="B1013" s="2" t="s">
         <v>1595</v>
       </c>
-      <c r="B1013" s="2" t="s">
-        <v>1596</v>
-      </c>
       <c r="C1013" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="1014" customHeight="1" spans="1:3">
       <c r="A1014" s="2" t="s">
+        <v>1596</v>
+      </c>
+      <c r="B1014" s="2" t="s">
         <v>1597</v>
       </c>
-      <c r="B1014" s="2" t="s">
-        <v>1596</v>
-      </c>
       <c r="C1014" s="2" t="s">
-        <v>1532</v>
-      </c>
-    </row>
-    <row r="1015" customHeight="1" spans="1:5">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="1015" customHeight="1" spans="1:3">
       <c r="A1015" s="2" t="s">
         <v>1598</v>
       </c>
       <c r="B1015" s="2" t="s">
-        <v>1599</v>
+        <v>1597</v>
       </c>
       <c r="C1015" s="2" t="s">
-        <v>1532</v>
-      </c>
-      <c r="E1015" s="4">
-        <v>0</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="1016" customHeight="1" spans="1:5">
       <c r="A1016" s="2" t="s">
+        <v>1599</v>
+      </c>
+      <c r="B1016" s="2" t="s">
         <v>1600</v>
       </c>
-      <c r="B1016" s="2" t="s">
-        <v>1601</v>
-      </c>
       <c r="C1016" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E1016" s="4">
         <v>0</v>
@@ -20651,13 +20654,13 @@
     </row>
     <row r="1017" customHeight="1" spans="1:5">
       <c r="A1017" s="2" t="s">
+        <v>1601</v>
+      </c>
+      <c r="B1017" s="2" t="s">
         <v>1602</v>
       </c>
-      <c r="B1017" s="2" t="s">
-        <v>1601</v>
-      </c>
       <c r="C1017" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E1017" s="4">
         <v>0</v>
@@ -20668,10 +20671,10 @@
         <v>1603</v>
       </c>
       <c r="B1018" s="2" t="s">
-        <v>1601</v>
+        <v>1602</v>
       </c>
       <c r="C1018" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="E1018" s="4">
         <v>0</v>
@@ -20682,10 +20685,10 @@
         <v>1604</v>
       </c>
       <c r="B1019" s="2" t="s">
-        <v>1605</v>
+        <v>1602</v>
       </c>
       <c r="C1019" s="2" t="s">
-        <v>1142</v>
+        <v>1533</v>
       </c>
       <c r="E1019" s="4">
         <v>0</v>
@@ -20693,10 +20696,10 @@
     </row>
     <row r="1020" customHeight="1" spans="1:5">
       <c r="A1020" s="2" t="s">
+        <v>1605</v>
+      </c>
+      <c r="B1020" s="2" t="s">
         <v>1606</v>
-      </c>
-      <c r="B1020" s="2" t="s">
-        <v>1607</v>
       </c>
       <c r="C1020" s="2" t="s">
         <v>1142</v>
@@ -20707,10 +20710,10 @@
     </row>
     <row r="1021" customHeight="1" spans="1:5">
       <c r="A1021" s="2" t="s">
+        <v>1607</v>
+      </c>
+      <c r="B1021" s="2" t="s">
         <v>1608</v>
-      </c>
-      <c r="B1021" s="2" t="s">
-        <v>1609</v>
       </c>
       <c r="C1021" s="2" t="s">
         <v>1142</v>
@@ -20721,10 +20724,10 @@
     </row>
     <row r="1022" customHeight="1" spans="1:5">
       <c r="A1022" s="2" t="s">
+        <v>1609</v>
+      </c>
+      <c r="B1022" s="2" t="s">
         <v>1610</v>
-      </c>
-      <c r="B1022" s="2" t="s">
-        <v>1611</v>
       </c>
       <c r="C1022" s="2" t="s">
         <v>1142</v>
@@ -20735,10 +20738,10 @@
     </row>
     <row r="1023" customHeight="1" spans="1:5">
       <c r="A1023" s="2" t="s">
+        <v>1611</v>
+      </c>
+      <c r="B1023" s="2" t="s">
         <v>1612</v>
-      </c>
-      <c r="B1023" s="2" t="s">
-        <v>1613</v>
       </c>
       <c r="C1023" s="2" t="s">
         <v>1142</v>
@@ -20749,10 +20752,10 @@
     </row>
     <row r="1024" customHeight="1" spans="1:5">
       <c r="A1024" s="2" t="s">
+        <v>1613</v>
+      </c>
+      <c r="B1024" s="2" t="s">
         <v>1614</v>
-      </c>
-      <c r="B1024" s="2" t="s">
-        <v>1615</v>
       </c>
       <c r="C1024" s="2" t="s">
         <v>1142</v>
@@ -20761,37 +20764,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1025" customHeight="1" spans="1:3">
+    <row r="1025" customHeight="1" spans="1:5">
       <c r="A1025" s="2" t="s">
+        <v>1615</v>
+      </c>
+      <c r="B1025" s="2" t="s">
         <v>1616</v>
-      </c>
-      <c r="B1025" s="2" t="s">
-        <v>1617</v>
       </c>
       <c r="C1025" s="2" t="s">
         <v>1142</v>
       </c>
-    </row>
-    <row r="1026" customHeight="1" spans="1:5">
+      <c r="E1025" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1026" customHeight="1" spans="1:3">
       <c r="A1026" s="2" t="s">
+        <v>1617</v>
+      </c>
+      <c r="B1026" s="2" t="s">
         <v>1618</v>
-      </c>
-      <c r="B1026" s="2" t="s">
-        <v>1619</v>
       </c>
       <c r="C1026" s="2" t="s">
         <v>1142</v>
       </c>
-      <c r="E1026" s="4">
-        <v>0</v>
-      </c>
     </row>
     <row r="1027" customHeight="1" spans="1:5">
       <c r="A1027" s="2" t="s">
+        <v>1619</v>
+      </c>
+      <c r="B1027" s="2" t="s">
         <v>1620</v>
-      </c>
-      <c r="B1027" s="2" t="s">
-        <v>853</v>
       </c>
       <c r="C1027" s="2" t="s">
         <v>1142</v>
@@ -20805,7 +20808,7 @@
         <v>1621</v>
       </c>
       <c r="B1028" s="2" t="s">
-        <v>1611</v>
+        <v>853</v>
       </c>
       <c r="C1028" s="2" t="s">
         <v>1142</v>
@@ -20819,7 +20822,7 @@
         <v>1622</v>
       </c>
       <c r="B1029" s="2" t="s">
-        <v>1623</v>
+        <v>1612</v>
       </c>
       <c r="C1029" s="2" t="s">
         <v>1142</v>
@@ -20830,10 +20833,10 @@
     </row>
     <row r="1030" customHeight="1" spans="1:5">
       <c r="A1030" s="2" t="s">
+        <v>1623</v>
+      </c>
+      <c r="B1030" s="2" t="s">
         <v>1624</v>
-      </c>
-      <c r="B1030" s="2" t="s">
-        <v>1607</v>
       </c>
       <c r="C1030" s="2" t="s">
         <v>1142</v>
@@ -20847,7 +20850,7 @@
         <v>1625</v>
       </c>
       <c r="B1031" s="2" t="s">
-        <v>1611</v>
+        <v>1608</v>
       </c>
       <c r="C1031" s="2" t="s">
         <v>1142</v>
@@ -20861,7 +20864,7 @@
         <v>1626</v>
       </c>
       <c r="B1032" s="2" t="s">
-        <v>1619</v>
+        <v>1612</v>
       </c>
       <c r="C1032" s="2" t="s">
         <v>1142</v>
@@ -20875,7 +20878,7 @@
         <v>1627</v>
       </c>
       <c r="B1033" s="2" t="s">
-        <v>1615</v>
+        <v>1620</v>
       </c>
       <c r="C1033" s="2" t="s">
         <v>1142</v>
@@ -20889,7 +20892,7 @@
         <v>1628</v>
       </c>
       <c r="B1034" s="2" t="s">
-        <v>1611</v>
+        <v>1616</v>
       </c>
       <c r="C1034" s="2" t="s">
         <v>1142</v>
@@ -20903,7 +20906,7 @@
         <v>1629</v>
       </c>
       <c r="B1035" s="2" t="s">
-        <v>1630</v>
+        <v>1612</v>
       </c>
       <c r="C1035" s="2" t="s">
         <v>1142</v>
@@ -20914,10 +20917,10 @@
     </row>
     <row r="1036" customHeight="1" spans="1:5">
       <c r="A1036" s="2" t="s">
+        <v>1630</v>
+      </c>
+      <c r="B1036" s="2" t="s">
         <v>1631</v>
-      </c>
-      <c r="B1036" s="2" t="s">
-        <v>1611</v>
       </c>
       <c r="C1036" s="2" t="s">
         <v>1142</v>
@@ -20931,7 +20934,7 @@
         <v>1632</v>
       </c>
       <c r="B1037" s="2" t="s">
-        <v>1633</v>
+        <v>1612</v>
       </c>
       <c r="C1037" s="2" t="s">
         <v>1142</v>
@@ -20940,26 +20943,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1038" customHeight="1" spans="1:5">
+    <row r="1038" customHeight="1" spans="1:3">
       <c r="A1038" s="2" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="B1038" s="2" t="s">
-        <v>1635</v>
+        <v>1612</v>
       </c>
       <c r="C1038" s="2" t="s">
         <v>1142</v>
       </c>
-      <c r="E1038" s="4">
-        <v>0</v>
-      </c>
     </row>
     <row r="1039" customHeight="1" spans="1:5">
       <c r="A1039" s="2" t="s">
-        <v>1636</v>
+        <v>1634</v>
       </c>
       <c r="B1039" s="2" t="s">
-        <v>1637</v>
+        <v>1635</v>
       </c>
       <c r="C1039" s="2" t="s">
         <v>1142</v>
@@ -20968,21 +20968,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1040" customHeight="1" spans="1:3">
+    <row r="1040" customHeight="1" spans="1:5">
       <c r="A1040" s="2" t="s">
-        <v>1638</v>
-      </c>
-      <c r="B1040" s="2"/>
+        <v>1636</v>
+      </c>
+      <c r="B1040" s="2" t="s">
+        <v>1637</v>
+      </c>
       <c r="C1040" s="2" t="s">
         <v>1142</v>
       </c>
+      <c r="E1040" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="1041" customHeight="1" spans="1:5">
       <c r="A1041" s="2" t="s">
+        <v>1638</v>
+      </c>
+      <c r="B1041" s="2" t="s">
         <v>1639</v>
-      </c>
-      <c r="B1041" s="2" t="s">
-        <v>1640</v>
       </c>
       <c r="C1041" s="2" t="s">
         <v>1142</v>
@@ -20991,70 +20996,65 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1042" customHeight="1" spans="1:5">
+    <row r="1042" customHeight="1" spans="1:3">
       <c r="A1042" s="2" t="s">
-        <v>1641</v>
-      </c>
-      <c r="B1042" s="10" t="s">
-        <v>1642</v>
-      </c>
+        <v>1640</v>
+      </c>
+      <c r="B1042" s="2"/>
       <c r="C1042" s="2" t="s">
         <v>1142</v>
       </c>
-      <c r="D1042" s="2"/>
-      <c r="E1042" s="4">
-        <v>0</v>
-      </c>
     </row>
     <row r="1043" customHeight="1" spans="1:5">
       <c r="A1043" s="2" t="s">
-        <v>1643</v>
-      </c>
-      <c r="B1043" s="10" t="s">
-        <v>1644</v>
+        <v>1641</v>
+      </c>
+      <c r="B1043" s="2" t="s">
+        <v>1642</v>
       </c>
       <c r="C1043" s="2" t="s">
         <v>1142</v>
       </c>
-      <c r="D1043" s="2"/>
       <c r="E1043" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="1044" customHeight="1" spans="1:5">
       <c r="A1044" s="2" t="s">
-        <v>1645</v>
-      </c>
-      <c r="B1044" s="2" t="s">
-        <v>1646</v>
+        <v>1643</v>
+      </c>
+      <c r="B1044" s="10" t="s">
+        <v>1644</v>
       </c>
       <c r="C1044" s="2" t="s">
         <v>1142</v>
       </c>
+      <c r="D1044" s="2"/>
       <c r="E1044" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="1045" customHeight="1" spans="1:5">
       <c r="A1045" s="2" t="s">
-        <v>1647</v>
-      </c>
-      <c r="B1045" s="2" t="s">
-        <v>1611</v>
+        <v>1645</v>
+      </c>
+      <c r="B1045" s="10" t="s">
+        <v>1646</v>
       </c>
       <c r="C1045" s="2" t="s">
         <v>1142</v>
       </c>
+      <c r="D1045" s="2"/>
       <c r="E1045" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="1046" customHeight="1" spans="1:5">
       <c r="A1046" s="2" t="s">
+        <v>1647</v>
+      </c>
+      <c r="B1046" s="2" t="s">
         <v>1648</v>
-      </c>
-      <c r="B1046" s="2" t="s">
-        <v>1630</v>
       </c>
       <c r="C1046" s="2" t="s">
         <v>1142</v>
@@ -21068,7 +21068,7 @@
         <v>1649</v>
       </c>
       <c r="B1047" s="2" t="s">
-        <v>1650</v>
+        <v>1612</v>
       </c>
       <c r="C1047" s="2" t="s">
         <v>1142</v>
@@ -21079,10 +21079,10 @@
     </row>
     <row r="1048" customHeight="1" spans="1:5">
       <c r="A1048" s="2" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="B1048" s="2" t="s">
-        <v>1619</v>
+        <v>1631</v>
       </c>
       <c r="C1048" s="2" t="s">
         <v>1142</v>
@@ -21093,10 +21093,10 @@
     </row>
     <row r="1049" customHeight="1" spans="1:5">
       <c r="A1049" s="2" t="s">
+        <v>1651</v>
+      </c>
+      <c r="B1049" s="2" t="s">
         <v>1652</v>
-      </c>
-      <c r="B1049" s="2" t="s">
-        <v>1611</v>
       </c>
       <c r="C1049" s="2" t="s">
         <v>1142</v>
@@ -21109,8 +21109,8 @@
       <c r="A1050" s="2" t="s">
         <v>1653</v>
       </c>
-      <c r="B1050" s="10" t="s">
-        <v>1654</v>
+      <c r="B1050" s="2" t="s">
+        <v>1620</v>
       </c>
       <c r="C1050" s="2" t="s">
         <v>1142</v>
@@ -21121,10 +21121,10 @@
     </row>
     <row r="1051" customHeight="1" spans="1:5">
       <c r="A1051" s="2" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="B1051" s="2" t="s">
-        <v>1615</v>
+        <v>1612</v>
       </c>
       <c r="C1051" s="2" t="s">
         <v>1142</v>
@@ -21135,10 +21135,10 @@
     </row>
     <row r="1052" customHeight="1" spans="1:5">
       <c r="A1052" s="2" t="s">
+        <v>1655</v>
+      </c>
+      <c r="B1052" s="10" t="s">
         <v>1656</v>
-      </c>
-      <c r="B1052" s="2" t="s">
-        <v>1611</v>
       </c>
       <c r="C1052" s="2" t="s">
         <v>1142</v>
@@ -21152,7 +21152,7 @@
         <v>1657</v>
       </c>
       <c r="B1053" s="2" t="s">
-        <v>1619</v>
+        <v>1616</v>
       </c>
       <c r="C1053" s="2" t="s">
         <v>1142</v>
@@ -21162,19 +21162,47 @@
       </c>
     </row>
     <row r="1054" customHeight="1" spans="1:5">
-      <c r="A1054" s="26" t="s">
+      <c r="A1054" s="2" t="s">
         <v>1658</v>
       </c>
       <c r="B1054" s="2" t="s">
+        <v>1612</v>
+      </c>
+      <c r="C1054" s="2" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E1054" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1055" customHeight="1" spans="1:5">
+      <c r="A1055" s="2" t="s">
         <v>1659</v>
       </c>
-      <c r="C1054" s="2" t="s">
+      <c r="B1055" s="2" t="s">
+        <v>1620</v>
+      </c>
+      <c r="C1055" s="2" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E1055" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1056" customHeight="1" spans="1:5">
+      <c r="A1056" s="26" t="s">
         <v>1660</v>
       </c>
-      <c r="D1054" s="2" t="s">
+      <c r="B1056" s="2" t="s">
         <v>1661</v>
       </c>
-      <c r="E1054" s="4">
+      <c r="C1056" s="2" t="s">
+        <v>1662</v>
+      </c>
+      <c r="D1056" s="2" t="s">
+        <v>1663</v>
+      </c>
+      <c r="E1056" s="4">
         <v>0</v>
       </c>
     </row>
@@ -21184,7 +21212,7 @@
     <mergeCell ref="A1:D2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="输入内容有误" error="请选择勾选或取消勾选" sqref="E2:E1048576">
+    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="输入内容有误" error="请选择勾选或取消勾选" sqref="E911 E2:E910 E912:E1048576">
       <formula1>IF(TRUE,OR(E2=0,E2=1),"Checkbox")</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>